<commit_message>
Changed from 240gf 100gf button
</commit_message>
<xml_diff>
--- a/documentation/reDIP-SID-BOM.xlsx
+++ b/documentation/reDIP-SID-BOM.xlsx
@@ -3060,11 +3060,11 @@
     25   $0.20      $5.00
    100   $0.18     $18.19
    250   $0.17     $42.75
-   500   $0.16     $78.23
-  1000   $0.13    $130.99
-  2500   $0.13    $318.38
-  8500   $0.12  $1,020.59
- 17000   $0.11  $1,917.43</t>
+   500   $0.16     $78.22
+  1000   $0.13    $130.97
+  2500   $0.13    $318.32
+  8500   $0.12  $1,020.43
+ 17000   $0.11  $1,917.26</t>
         </r>
       </text>
     </comment>
@@ -3080,31 +3080,10 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-    10   £0.16      £1.55
-    50   £0.15      £7.30
-   100   £0.13     £13.30
-   500   £0.12     £61.50</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB30" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Qty/Price Breaks (USD):
-  Qty  -  Unit$  -  Ext$
-================
-     1   $1.31      $1.31
-    10   $1.01     $10.07
-    30   $0.95     $28.53
-   100   $0.90     $89.52
-   500   $0.87    $435.20
-  1000   $0.86    $858.20</t>
+    10   £0.15      £1.51
+    50   £0.14      £7.15
+   100   £0.13     £13.00
+   500   £0.11     £56.00</t>
         </r>
       </text>
     </comment>
@@ -3122,10 +3101,10 @@
 ================
      1   $0.23      $0.23
     10   $0.22      $2.18
-    50   $0.20     $10.10
-   100   $0.18     $18.00
-  1000   $0.12    $123.00
- 10000   $0.12  $1,230.00</t>
+    50   $0.20     $10.05
+   100   $0.19     $18.90
+  1000   $0.15    $154.00
+ 10000   $0.15  $1,540.00</t>
         </r>
       </text>
     </comment>
@@ -3141,29 +3120,9 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.15      $0.15
-  8500   $0.16  $1,377.00
-100000   $0.14 $13,600.00</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AV30" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Qty/Price Breaks (GBP):
-  Qty  -  Unit£  -  Ext£
-================
-     5   £0.17      £0.87
-   100   £0.14     £14.25
-  1000   £0.10     £96.10
-  3000   £0.08    £249.30
-  8500   £0.08    £691.90</t>
+     1   $0.16      $0.16
+  8500   $0.17  $1,462.00
+100000   $0.14 $14,400.00</t>
         </r>
       </text>
     </comment>
@@ -4324,7 +4283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="332">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -4452,9 +4411,9 @@
     <t>GRM033R60J224KE15D</t>
   </si>
   <si>
-    <t>C7,C18: 1.2V DC DERATED TO 0.1uF
+    <t>C8,C9,C15-C17,C19,C20,C22,C23: 3.3V DC DERATED TO 0.1uF
 C10: 1.65V DC VAG DERATED TO 0.1uF
-C8,C9,C15-C17,C19,C20,C22,C23: 3.3V DC DERATED TO 0.1uF</t>
+C7,C18: 1.2V DC DERATED TO 0.1uF</t>
   </si>
   <si>
     <t>D1,D2</t>
@@ -4679,7 +4638,7 @@
     <t>SW1</t>
   </si>
   <si>
-    <t>KXT331LHS</t>
+    <t>KXT311LHS</t>
   </si>
   <si>
     <t>SW TACT 3.0 x 2.0 mm</t>
@@ -4874,7 +4833,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>lø. 21. aug. 2021 kl. 09.36 +0200</t>
+    <t>lø. 21. aug. 2021 kl. 22.57 +0200</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -4889,7 +4848,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2021-08-21 09:36:50</t>
+    <t>2021-08-21 22:57:35</t>
   </si>
   <si>
     <t>Arrow</t>
@@ -4967,7 +4926,7 @@
     <t>P123220CT-ND</t>
   </si>
   <si>
-    <t>CKN10779CT-ND</t>
+    <t>CKN10777CT-ND</t>
   </si>
   <si>
     <t>NCP115AMX120TCGOSCT-ND</t>
@@ -5054,7 +5013,7 @@
     <t>3303148</t>
   </si>
   <si>
-    <t>3023200</t>
+    <t>3023197</t>
   </si>
   <si>
     <t>3010452</t>
@@ -5102,9 +5061,6 @@
     <t>C713500</t>
   </si>
   <si>
-    <t>C221822</t>
-  </si>
-  <si>
     <t>C2683750</t>
   </si>
   <si>
@@ -5165,7 +5121,7 @@
     <t>667ERJ1GNJ101C</t>
   </si>
   <si>
-    <t>611KXT331LHS</t>
+    <t>611KXT311LHS</t>
   </si>
   <si>
     <t>863NCP115AMX120TCG</t>
@@ -5249,7 +5205,7 @@
     <t>51W5773</t>
   </si>
   <si>
-    <t>35AH1369</t>
+    <t>35AH1367</t>
   </si>
   <si>
     <t>97AC7838</t>
@@ -5319,9 +5275,6 @@
   </si>
   <si>
     <t>SMLLX0201UPGCTR</t>
-  </si>
-  <si>
-    <t>KXT331</t>
   </si>
   <si>
     <t>MCP6H01TE/OT</t>
@@ -6123,28 +6076,28 @@
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
       <c r="AE5" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AF5" s="12"/>
       <c r="AG5" s="12"/>
       <c r="AH5" s="12"/>
       <c r="AI5" s="12"/>
       <c r="AJ5" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AK5" s="13"/>
       <c r="AL5" s="13"/>
       <c r="AM5" s="13"/>
       <c r="AN5" s="13"/>
       <c r="AO5" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AP5" s="14"/>
       <c r="AQ5" s="14"/>
       <c r="AR5" s="14"/>
       <c r="AS5" s="14"/>
       <c r="AT5" s="15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AU5" s="15"/>
       <c r="AV5" s="15"/>
@@ -6377,7 +6330,7 @@
         <v>0</v>
       </c>
       <c r="AI7" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AJ7" s="17">
         <v>20</v>
@@ -6391,7 +6344,7 @@
         <v>0</v>
       </c>
       <c r="AN7" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:50">
@@ -6482,7 +6435,7 @@
         <v>0</v>
       </c>
       <c r="AI8" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AJ8" s="17">
         <v>20</v>
@@ -6496,7 +6449,7 @@
         <v>0</v>
       </c>
       <c r="AN8" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:50">
@@ -6573,7 +6526,7 @@
         <v>0</v>
       </c>
       <c r="AI9" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AJ9" s="20" t="s">
         <v>196</v>
@@ -6587,7 +6540,7 @@
         <v>0</v>
       </c>
       <c r="AN9" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AO9" s="17">
         <v>60</v>
@@ -6601,7 +6554,7 @@
         <v>0</v>
       </c>
       <c r="AS9" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:50">
@@ -6678,7 +6631,7 @@
         <v>0</v>
       </c>
       <c r="AI10" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AJ10" s="20" t="s">
         <v>196</v>
@@ -6692,7 +6645,7 @@
         <v>0</v>
       </c>
       <c r="AN10" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:50">
@@ -6783,7 +6736,7 @@
         <v>0</v>
       </c>
       <c r="AI11" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AJ11" s="17">
         <v>80000</v>
@@ -6797,7 +6750,7 @@
         <v>0</v>
       </c>
       <c r="AN11" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:50">
@@ -6888,7 +6841,7 @@
         <v>0</v>
       </c>
       <c r="AI12" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AJ12" s="17">
         <v>19878</v>
@@ -6902,7 +6855,7 @@
         <v>0</v>
       </c>
       <c r="AN12" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AO12" s="17">
         <v>7000</v>
@@ -6916,7 +6869,7 @@
         <v>0</v>
       </c>
       <c r="AS12" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:50">
@@ -6990,7 +6943,7 @@
         <v>0</v>
       </c>
       <c r="AI13" s="19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AJ13" s="20" t="s">
         <v>196</v>
@@ -7004,7 +6957,7 @@
         <v>0</v>
       </c>
       <c r="AN13" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:50">
@@ -7078,7 +7031,7 @@
         <v>0</v>
       </c>
       <c r="AI14" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AJ14" s="17">
         <v>5</v>
@@ -7092,7 +7045,7 @@
         <v>0</v>
       </c>
       <c r="AN14" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AT14" s="17">
         <v>3427</v>
@@ -7106,7 +7059,7 @@
         <v>0</v>
       </c>
       <c r="AX14" s="19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:50">
@@ -7180,7 +7133,7 @@
         <v>0</v>
       </c>
       <c r="AI15" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AJ15" s="17">
         <v>3287</v>
@@ -7194,7 +7147,7 @@
         <v>0</v>
       </c>
       <c r="AN15" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AT15" s="17">
         <v>2779</v>
@@ -7208,7 +7161,7 @@
         <v>0</v>
       </c>
       <c r="AX15" s="19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="16" spans="1:50">
@@ -7237,7 +7190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:50">
+    <row r="17" spans="1:45">
       <c r="A17" s="17" t="s">
         <v>61</v>
       </c>
@@ -7263,7 +7216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:50">
+    <row r="18" spans="1:45">
       <c r="A18" s="17" t="s">
         <v>65</v>
       </c>
@@ -7289,7 +7242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:50">
+    <row r="19" spans="1:45">
       <c r="A19" s="17" t="s">
         <v>69</v>
       </c>
@@ -7315,7 +7268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:50">
+    <row r="20" spans="1:45">
       <c r="A20" s="17" t="s">
         <v>73</v>
       </c>
@@ -7364,7 +7317,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="1:50">
+    <row r="21" spans="1:45">
       <c r="A21" s="17" t="s">
         <v>79</v>
       </c>
@@ -7435,7 +7388,7 @@
         <v>0</v>
       </c>
       <c r="AI21" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AJ21" s="20" t="s">
         <v>196</v>
@@ -7449,7 +7402,7 @@
         <v>0</v>
       </c>
       <c r="AN21" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AO21" s="17">
         <v>38000</v>
@@ -7463,10 +7416,10 @@
         <v>0</v>
       </c>
       <c r="AS21" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
-    <row r="22" spans="1:50">
+    <row r="22" spans="1:45">
       <c r="A22" s="17" t="s">
         <v>85</v>
       </c>
@@ -7551,7 +7504,7 @@
         <v>0</v>
       </c>
       <c r="AI22" s="19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AJ22" s="20" t="s">
         <v>196</v>
@@ -7565,7 +7518,7 @@
         <v>0</v>
       </c>
       <c r="AN22" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AO22" s="17">
         <v>58000</v>
@@ -7579,10 +7532,10 @@
         <v>0</v>
       </c>
       <c r="AS22" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
-    <row r="23" spans="1:50">
+    <row r="23" spans="1:45">
       <c r="A23" s="17" t="s">
         <v>89</v>
       </c>
@@ -7653,7 +7606,7 @@
         <v>0</v>
       </c>
       <c r="AI23" s="19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AJ23" s="17">
         <v>90000</v>
@@ -7667,7 +7620,7 @@
         <v>0</v>
       </c>
       <c r="AN23" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AO23" s="17">
         <v>772637</v>
@@ -7681,10 +7634,10 @@
         <v>0</v>
       </c>
       <c r="AS23" s="19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
-    <row r="24" spans="1:50">
+    <row r="24" spans="1:45">
       <c r="A24" s="17" t="s">
         <v>93</v>
       </c>
@@ -7755,7 +7708,7 @@
         <v>0</v>
       </c>
       <c r="AI24" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AJ24" s="20" t="s">
         <v>196</v>
@@ -7769,10 +7722,10 @@
         <v>0</v>
       </c>
       <c r="AN24" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:50">
+    <row r="25" spans="1:45">
       <c r="A25" s="17" t="s">
         <v>97</v>
       </c>
@@ -7843,7 +7796,7 @@
         <v>0</v>
       </c>
       <c r="AI25" s="19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AJ25" s="20" t="s">
         <v>196</v>
@@ -7857,7 +7810,7 @@
         <v>0</v>
       </c>
       <c r="AN25" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AO25" s="17">
         <v>28000</v>
@@ -7871,10 +7824,10 @@
         <v>0</v>
       </c>
       <c r="AS25" s="19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
-    <row r="26" spans="1:50">
+    <row r="26" spans="1:45">
       <c r="A26" s="17" t="s">
         <v>101</v>
       </c>
@@ -7945,7 +7898,7 @@
         <v>0</v>
       </c>
       <c r="AI26" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AJ26" s="17">
         <v>45000</v>
@@ -7959,10 +7912,10 @@
         <v>0</v>
       </c>
       <c r="AN26" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
-    <row r="27" spans="1:50">
+    <row r="27" spans="1:45">
       <c r="A27" s="17" t="s">
         <v>105</v>
       </c>
@@ -8047,7 +8000,7 @@
         <v>0</v>
       </c>
       <c r="AI27" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AJ27" s="17">
         <v>120000</v>
@@ -8061,7 +8014,7 @@
         <v>0</v>
       </c>
       <c r="AN27" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AO27" s="17">
         <v>699000</v>
@@ -8075,10 +8028,10 @@
         <v>0</v>
       </c>
       <c r="AS27" s="19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
-    <row r="28" spans="1:50">
+    <row r="28" spans="1:45">
       <c r="A28" s="17" t="s">
         <v>108</v>
       </c>
@@ -8149,7 +8102,7 @@
         <v>0</v>
       </c>
       <c r="AI28" s="19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AJ28" s="20" t="s">
         <v>196</v>
@@ -8163,10 +8116,10 @@
         <v>0</v>
       </c>
       <c r="AN28" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
-    <row r="29" spans="1:50">
+    <row r="29" spans="1:45">
       <c r="A29" s="17" t="s">
         <v>112</v>
       </c>
@@ -8251,7 +8204,7 @@
         <v>0</v>
       </c>
       <c r="AI29" s="19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AJ29" s="20" t="s">
         <v>196</v>
@@ -8265,7 +8218,7 @@
         <v>0</v>
       </c>
       <c r="AN29" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AO29" s="17">
         <v>37000</v>
@@ -8279,10 +8232,10 @@
         <v>0</v>
       </c>
       <c r="AS29" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
-    <row r="30" spans="1:50">
+    <row r="30" spans="1:45">
       <c r="A30" s="17" t="s">
         <v>116</v>
       </c>
@@ -8314,10 +8267,10 @@
         <v>0</v>
       </c>
       <c r="P30" s="17">
-        <v>94253</v>
+        <v>6438</v>
       </c>
       <c r="R30" s="18">
-        <f>iferror(lookup(if(Q30="",H30,Q30),{0,1,10,25,100,250,500,1000,2500,8500,17000},{0.0,0.22,0.211,0.2,0.1819,0.171,0.15646,0.13099,0.12735,0.12007,0.11279}),"")</f>
+        <f>iferror(lookup(if(Q30="",H30,Q30),{0,1,10,25,100,250,500,1000,2500,8500,17000},{0.0,0.22,0.211,0.2,0.1819,0.171,0.15644,0.13097,0.12733,0.12005,0.11278}),"")</f>
         <v>0</v>
       </c>
       <c r="S30" s="18">
@@ -8328,10 +8281,10 @@
         <v>213</v>
       </c>
       <c r="U30" s="17">
-        <v>4297</v>
+        <v>882</v>
       </c>
       <c r="W30" s="18">
-        <f>iferror(USD_GBP*lookup(if(V30="",H30,V30),{0,1,10,50,100,500},{0.0,0.155,0.155,0.146,0.133,0.123}),"")</f>
+        <f>iferror(USD_GBP*lookup(if(V30="",H30,V30),{0,1,10,50,100,500},{0.0,0.151,0.151,0.143,0.13,0.112}),"")</f>
         <v>0</v>
       </c>
       <c r="X30" s="18">
@@ -8341,25 +8294,11 @@
       <c r="Y30" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="Z30" s="17">
-        <v>16447</v>
-      </c>
-      <c r="AB30" s="18">
-        <f>iferror(lookup(if(AA30="",H30,AA30),{0,1,10,30,100,500,1000},{0.0,1.3101,1.0067,0.9509,0.8952,0.8704,0.8582}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="AC30" s="18">
-        <f>iferror(if(AA30="",H30,AA30)*AB30,"")</f>
-        <v>0</v>
-      </c>
-      <c r="AD30" s="19" t="s">
-        <v>258</v>
-      </c>
       <c r="AE30" s="17">
-        <v>5389</v>
+        <v>9735</v>
       </c>
       <c r="AG30" s="18">
-        <f>iferror(lookup(if(AF30="",H30,AF30),{0,1,10,50,100,1000,10000},{0.0,0.23,0.218,0.202,0.18,0.123,0.123}),"")</f>
+        <f>iferror(lookup(if(AF30="",H30,AF30),{0,1,10,50,100,1000,10000},{0.0,0.23,0.218,0.201,0.189,0.154,0.154}),"")</f>
         <v>0</v>
       </c>
       <c r="AH30" s="18">
@@ -8367,13 +8306,13 @@
         <v>0</v>
       </c>
       <c r="AI30" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AJ30" s="17">
-        <v>6884</v>
+        <v>7158</v>
       </c>
       <c r="AL30" s="18">
-        <f>iferror(lookup(if(AK30="",H30,AK30),{0,1,8500,100000},{0.0,0.148,0.162,0.136}),"")</f>
+        <f>iferror(lookup(if(AK30="",H30,AK30),{0,1,8500,100000},{0.0,0.157,0.172,0.144}),"")</f>
         <v>0</v>
       </c>
       <c r="AM30" s="18">
@@ -8381,24 +8320,10 @@
         <v>0</v>
       </c>
       <c r="AN30" s="19" t="s">
-        <v>307</v>
-      </c>
-      <c r="AT30" s="17">
-        <v>2865</v>
-      </c>
-      <c r="AV30" s="18">
-        <f>iferror(USD_GBP*lookup(if(AU30="",H30,AU30),{0,1,5,100,1000,3000,8500},{0.0,0.174,0.174,0.1425,0.0961,0.0831,0.0814}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="AW30" s="18">
-        <f>iferror(if(AU30="",H30,AU30)*AV30,"")</f>
-        <v>0</v>
-      </c>
-      <c r="AX30" s="19" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
     </row>
-    <row r="31" spans="1:50">
+    <row r="31" spans="1:45">
       <c r="A31" s="17" t="s">
         <v>121</v>
       </c>
@@ -8469,7 +8394,7 @@
         <v>0</v>
       </c>
       <c r="AI31" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AJ31" s="17">
         <v>1912</v>
@@ -8483,7 +8408,7 @@
         <v>0</v>
       </c>
       <c r="AN31" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AO31" s="17">
         <v>3000</v>
@@ -8497,10 +8422,10 @@
         <v>0</v>
       </c>
       <c r="AS31" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
-    <row r="32" spans="1:50">
+    <row r="32" spans="1:45">
       <c r="A32" s="17" t="s">
         <v>126</v>
       </c>
@@ -8571,7 +8496,7 @@
         <v>0</v>
       </c>
       <c r="AI32" s="19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AJ32" s="20" t="s">
         <v>196</v>
@@ -8585,7 +8510,7 @@
         <v>0</v>
       </c>
       <c r="AN32" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:50">
@@ -8659,7 +8584,7 @@
         <v>0</v>
       </c>
       <c r="AI33" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AJ33" s="20" t="s">
         <v>196</v>
@@ -8673,7 +8598,7 @@
         <v>0</v>
       </c>
       <c r="AN33" s="19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AO33" s="17">
         <v>12</v>
@@ -8687,7 +8612,7 @@
         <v>0</v>
       </c>
       <c r="AS33" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="34" spans="1:50">
@@ -8747,7 +8672,7 @@
         <v>0</v>
       </c>
       <c r="AD34" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AE34" s="17">
         <v>627</v>
@@ -8761,7 +8686,7 @@
         <v>0</v>
       </c>
       <c r="AI34" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:50">
@@ -8838,7 +8763,7 @@
         <v>0</v>
       </c>
       <c r="AI35" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AJ35" s="20" t="s">
         <v>196</v>
@@ -8852,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="AN35" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:50">
@@ -8926,7 +8851,7 @@
         <v>0</v>
       </c>
       <c r="AI36" s="19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AJ36" s="20" t="s">
         <v>196</v>
@@ -8940,7 +8865,7 @@
         <v>0</v>
       </c>
       <c r="AN36" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AO36" s="17">
         <v>2400</v>
@@ -8954,7 +8879,7 @@
         <v>0</v>
       </c>
       <c r="AS36" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AT36" s="20" t="s">
         <v>196</v>
@@ -9042,7 +8967,7 @@
         <v>0</v>
       </c>
       <c r="AI37" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AJ37" s="17">
         <v>2970</v>
@@ -9056,7 +8981,7 @@
         <v>0</v>
       </c>
       <c r="AN37" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AO37" s="17">
         <v>1660</v>
@@ -9070,7 +8995,7 @@
         <v>0</v>
       </c>
       <c r="AS37" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AT37" s="20" t="s">
         <v>196</v>
@@ -9084,7 +9009,7 @@
         <v>0</v>
       </c>
       <c r="AX37" s="19" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="38" spans="1:50">
@@ -9245,7 +9170,7 @@
         <v>0</v>
       </c>
       <c r="AI40" s="19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AJ40" s="17">
         <v>2945</v>
@@ -9259,7 +9184,7 @@
         <v>0</v>
       </c>
       <c r="AN40" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:50">
@@ -9457,7 +9382,7 @@
     </row>
     <row r="45" spans="1:50">
       <c r="A45" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="L45">
         <f t="array" ref="L45">IFERROR(CONCATENATE(INDEX(O7:O40,SMALL(IF(ISNUMBER(L7:L40),IF(L7:L40&gt;0,IF(O7:O40&lt;&gt;"",ROW(L7:L40)-MIN(ROW(L7:L40))+1))),ROW()-ROW(A$43)+1)),",",TEXT(INDEX(L7:L40,SMALL(IF(ISNUMBER(L7:L40),IF(L7:L40&gt;0,IF(O7:O40&lt;&gt;"",ROW(L7:L40)-MIN(ROW(L7:L40))+1))),ROW()-ROW(A$43)+1)),"##0"),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A40,SMALL(IF(ISNUMBER(L7:L40),IF(L7:L40&gt;0,IF(O7:O40&lt;&gt;"",ROW(L7:L40)-MIN(ROW(L7:L40))+1))),ROW()-ROW(A$43)+1)),",",";")),"")</f>
@@ -10865,13 +10790,8 @@
       <formula>Z29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA30">
+  <conditionalFormatting sqref="AA34">
     <cfRule type="cellIs" dxfId="1" priority="473" operator="greaterThan">
-      <formula>Z30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA34">
-    <cfRule type="cellIs" dxfId="1" priority="478" operator="greaterThan">
       <formula>Z34</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10913,13 +10833,8 @@
       <formula>I29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB30">
+  <conditionalFormatting sqref="AB34">
     <cfRule type="cellIs" dxfId="4" priority="475" operator="lessThanOrEqual">
-      <formula>I30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB34">
-    <cfRule type="cellIs" dxfId="4" priority="480" operator="lessThanOrEqual">
       <formula>I34</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10958,13 +10873,8 @@
       <formula>J29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC30">
+  <conditionalFormatting sqref="AC34">
     <cfRule type="cellIs" dxfId="4" priority="474" operator="lessThanOrEqual">
-      <formula>J30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC34">
-    <cfRule type="cellIs" dxfId="4" priority="479" operator="lessThanOrEqual">
       <formula>J34</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10974,1675 +10884,1649 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE10">
+    <cfRule type="cellIs" dxfId="1" priority="491" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="492" operator="lessThan">
+      <formula>H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE11">
     <cfRule type="cellIs" dxfId="1" priority="496" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="497" operator="lessThan">
-      <formula>H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE11">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE12">
     <cfRule type="cellIs" dxfId="1" priority="501" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="502" operator="lessThan">
-      <formula>H11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE12">
+      <formula>H12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE13">
     <cfRule type="cellIs" dxfId="1" priority="506" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="507" operator="lessThan">
-      <formula>H12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE13">
+      <formula>H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE14">
     <cfRule type="cellIs" dxfId="1" priority="511" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="512" operator="lessThan">
-      <formula>H13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE14">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE15">
     <cfRule type="cellIs" dxfId="1" priority="516" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="517" operator="lessThan">
-      <formula>H14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE15">
+      <formula>H15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE21">
     <cfRule type="cellIs" dxfId="1" priority="521" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="522" operator="lessThan">
-      <formula>H15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE21">
+      <formula>H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE22">
     <cfRule type="cellIs" dxfId="1" priority="526" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="527" operator="lessThan">
-      <formula>H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE22">
+      <formula>H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE23">
     <cfRule type="cellIs" dxfId="1" priority="531" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="532" operator="lessThan">
-      <formula>H22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE23">
+      <formula>H23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE24">
     <cfRule type="cellIs" dxfId="1" priority="536" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="537" operator="lessThan">
-      <formula>H23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE24">
+      <formula>H24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE25">
     <cfRule type="cellIs" dxfId="1" priority="541" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="542" operator="lessThan">
-      <formula>H24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE25">
+      <formula>H25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE26">
     <cfRule type="cellIs" dxfId="1" priority="546" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="547" operator="lessThan">
-      <formula>H25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE26">
+      <formula>H26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE27">
     <cfRule type="cellIs" dxfId="1" priority="551" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="552" operator="lessThan">
-      <formula>H26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE27">
+      <formula>H27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE28">
     <cfRule type="cellIs" dxfId="1" priority="556" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="557" operator="lessThan">
-      <formula>H27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE28">
+      <formula>H28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE29">
     <cfRule type="cellIs" dxfId="1" priority="561" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="562" operator="lessThan">
-      <formula>H28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE29">
+      <formula>H29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE30">
     <cfRule type="cellIs" dxfId="1" priority="566" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="567" operator="lessThan">
-      <formula>H29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE30">
+      <formula>H30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE31">
     <cfRule type="cellIs" dxfId="1" priority="571" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="572" operator="lessThan">
-      <formula>H30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE31">
+      <formula>H31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE32">
     <cfRule type="cellIs" dxfId="1" priority="576" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="577" operator="lessThan">
-      <formula>H31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE32">
+      <formula>H32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE33">
     <cfRule type="cellIs" dxfId="1" priority="581" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="582" operator="lessThan">
-      <formula>H32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE33">
+      <formula>H33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE34">
     <cfRule type="cellIs" dxfId="1" priority="586" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="587" operator="lessThan">
-      <formula>H33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE34">
+      <formula>H34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE35">
     <cfRule type="cellIs" dxfId="1" priority="591" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="592" operator="lessThan">
-      <formula>H34</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE35">
+      <formula>H35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE36">
     <cfRule type="cellIs" dxfId="1" priority="596" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="597" operator="lessThan">
-      <formula>H35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE36">
+      <formula>H36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE37">
     <cfRule type="cellIs" dxfId="1" priority="601" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="602" operator="lessThan">
-      <formula>H36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE37">
+      <formula>H37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE40">
     <cfRule type="cellIs" dxfId="1" priority="606" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="607" operator="lessThan">
+      <formula>H40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE7">
+    <cfRule type="cellIs" dxfId="1" priority="476" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="477" operator="lessThan">
+      <formula>H7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE8">
+    <cfRule type="cellIs" dxfId="1" priority="481" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="482" operator="lessThan">
+      <formula>H8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE9">
+    <cfRule type="cellIs" dxfId="1" priority="486" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="487" operator="lessThan">
+      <formula>H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF10">
+    <cfRule type="cellIs" dxfId="1" priority="493" operator="greaterThan">
+      <formula>AE10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF11">
+    <cfRule type="cellIs" dxfId="1" priority="498" operator="greaterThan">
+      <formula>AE11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF12">
+    <cfRule type="cellIs" dxfId="1" priority="503" operator="greaterThan">
+      <formula>AE12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF13">
+    <cfRule type="cellIs" dxfId="1" priority="508" operator="greaterThan">
+      <formula>AE13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF14">
+    <cfRule type="cellIs" dxfId="1" priority="513" operator="greaterThan">
+      <formula>AE14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF15">
+    <cfRule type="cellIs" dxfId="1" priority="518" operator="greaterThan">
+      <formula>AE15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF21">
+    <cfRule type="cellIs" dxfId="1" priority="523" operator="greaterThan">
+      <formula>AE21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF22">
+    <cfRule type="cellIs" dxfId="1" priority="528" operator="greaterThan">
+      <formula>AE22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF23">
+    <cfRule type="cellIs" dxfId="1" priority="533" operator="greaterThan">
+      <formula>AE23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF24">
+    <cfRule type="cellIs" dxfId="1" priority="538" operator="greaterThan">
+      <formula>AE24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF25">
+    <cfRule type="cellIs" dxfId="1" priority="543" operator="greaterThan">
+      <formula>AE25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF26">
+    <cfRule type="cellIs" dxfId="1" priority="548" operator="greaterThan">
+      <formula>AE26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF27">
+    <cfRule type="cellIs" dxfId="1" priority="553" operator="greaterThan">
+      <formula>AE27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF28">
+    <cfRule type="cellIs" dxfId="1" priority="558" operator="greaterThan">
+      <formula>AE28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF29">
+    <cfRule type="cellIs" dxfId="1" priority="563" operator="greaterThan">
+      <formula>AE29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF30">
+    <cfRule type="cellIs" dxfId="1" priority="568" operator="greaterThan">
+      <formula>AE30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF31">
+    <cfRule type="cellIs" dxfId="1" priority="573" operator="greaterThan">
+      <formula>AE31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF32">
+    <cfRule type="cellIs" dxfId="1" priority="578" operator="greaterThan">
+      <formula>AE32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF33">
+    <cfRule type="cellIs" dxfId="1" priority="583" operator="greaterThan">
+      <formula>AE33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF34">
+    <cfRule type="cellIs" dxfId="1" priority="588" operator="greaterThan">
+      <formula>AE34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF35">
+    <cfRule type="cellIs" dxfId="1" priority="593" operator="greaterThan">
+      <formula>AE35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF36">
+    <cfRule type="cellIs" dxfId="1" priority="598" operator="greaterThan">
+      <formula>AE36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF37">
+    <cfRule type="cellIs" dxfId="1" priority="603" operator="greaterThan">
+      <formula>AE37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF40">
+    <cfRule type="cellIs" dxfId="1" priority="608" operator="greaterThan">
+      <formula>AE40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF7">
+    <cfRule type="cellIs" dxfId="1" priority="478" operator="greaterThan">
+      <formula>AE7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF8">
+    <cfRule type="cellIs" dxfId="1" priority="483" operator="greaterThan">
+      <formula>AE8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF9">
+    <cfRule type="cellIs" dxfId="1" priority="488" operator="greaterThan">
+      <formula>AE9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG10">
+    <cfRule type="cellIs" dxfId="4" priority="495" operator="lessThanOrEqual">
+      <formula>I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG11">
+    <cfRule type="cellIs" dxfId="4" priority="500" operator="lessThanOrEqual">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG12">
+    <cfRule type="cellIs" dxfId="4" priority="505" operator="lessThanOrEqual">
+      <formula>I12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG13">
+    <cfRule type="cellIs" dxfId="4" priority="510" operator="lessThanOrEqual">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG14">
+    <cfRule type="cellIs" dxfId="4" priority="515" operator="lessThanOrEqual">
+      <formula>I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG15">
+    <cfRule type="cellIs" dxfId="4" priority="520" operator="lessThanOrEqual">
+      <formula>I15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG21">
+    <cfRule type="cellIs" dxfId="4" priority="525" operator="lessThanOrEqual">
+      <formula>I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG22">
+    <cfRule type="cellIs" dxfId="4" priority="530" operator="lessThanOrEqual">
+      <formula>I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG23">
+    <cfRule type="cellIs" dxfId="4" priority="535" operator="lessThanOrEqual">
+      <formula>I23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG24">
+    <cfRule type="cellIs" dxfId="4" priority="540" operator="lessThanOrEqual">
+      <formula>I24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG25">
+    <cfRule type="cellIs" dxfId="4" priority="545" operator="lessThanOrEqual">
+      <formula>I25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG26">
+    <cfRule type="cellIs" dxfId="4" priority="550" operator="lessThanOrEqual">
+      <formula>I26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG27">
+    <cfRule type="cellIs" dxfId="4" priority="555" operator="lessThanOrEqual">
+      <formula>I27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG28">
+    <cfRule type="cellIs" dxfId="4" priority="560" operator="lessThanOrEqual">
+      <formula>I28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG29">
+    <cfRule type="cellIs" dxfId="4" priority="565" operator="lessThanOrEqual">
+      <formula>I29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG30">
+    <cfRule type="cellIs" dxfId="4" priority="570" operator="lessThanOrEqual">
+      <formula>I30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG31">
+    <cfRule type="cellIs" dxfId="4" priority="575" operator="lessThanOrEqual">
+      <formula>I31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG32">
+    <cfRule type="cellIs" dxfId="4" priority="580" operator="lessThanOrEqual">
+      <formula>I32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG33">
+    <cfRule type="cellIs" dxfId="4" priority="585" operator="lessThanOrEqual">
+      <formula>I33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG34">
+    <cfRule type="cellIs" dxfId="4" priority="590" operator="lessThanOrEqual">
+      <formula>I34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG35">
+    <cfRule type="cellIs" dxfId="4" priority="595" operator="lessThanOrEqual">
+      <formula>I35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG36">
+    <cfRule type="cellIs" dxfId="4" priority="600" operator="lessThanOrEqual">
+      <formula>I36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG37">
+    <cfRule type="cellIs" dxfId="4" priority="605" operator="lessThanOrEqual">
+      <formula>I37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG40">
+    <cfRule type="cellIs" dxfId="4" priority="610" operator="lessThanOrEqual">
+      <formula>I40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG7">
+    <cfRule type="cellIs" dxfId="4" priority="480" operator="lessThanOrEqual">
+      <formula>I7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG8">
+    <cfRule type="cellIs" dxfId="4" priority="485" operator="lessThanOrEqual">
+      <formula>I8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG9">
+    <cfRule type="cellIs" dxfId="4" priority="490" operator="lessThanOrEqual">
+      <formula>I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH10">
+    <cfRule type="cellIs" dxfId="4" priority="494" operator="lessThanOrEqual">
+      <formula>J10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH11">
+    <cfRule type="cellIs" dxfId="4" priority="499" operator="lessThanOrEqual">
+      <formula>J11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH12">
+    <cfRule type="cellIs" dxfId="4" priority="504" operator="lessThanOrEqual">
+      <formula>J12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH13">
+    <cfRule type="cellIs" dxfId="4" priority="509" operator="lessThanOrEqual">
+      <formula>J13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH14">
+    <cfRule type="cellIs" dxfId="4" priority="514" operator="lessThanOrEqual">
+      <formula>J14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH15">
+    <cfRule type="cellIs" dxfId="4" priority="519" operator="lessThanOrEqual">
+      <formula>J15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH21">
+    <cfRule type="cellIs" dxfId="4" priority="524" operator="lessThanOrEqual">
+      <formula>J21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH22">
+    <cfRule type="cellIs" dxfId="4" priority="529" operator="lessThanOrEqual">
+      <formula>J22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH23">
+    <cfRule type="cellIs" dxfId="4" priority="534" operator="lessThanOrEqual">
+      <formula>J23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH24">
+    <cfRule type="cellIs" dxfId="4" priority="539" operator="lessThanOrEqual">
+      <formula>J24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH25">
+    <cfRule type="cellIs" dxfId="4" priority="544" operator="lessThanOrEqual">
+      <formula>J25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH26">
+    <cfRule type="cellIs" dxfId="4" priority="549" operator="lessThanOrEqual">
+      <formula>J26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH27">
+    <cfRule type="cellIs" dxfId="4" priority="554" operator="lessThanOrEqual">
+      <formula>J27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH28">
+    <cfRule type="cellIs" dxfId="4" priority="559" operator="lessThanOrEqual">
+      <formula>J28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH29">
+    <cfRule type="cellIs" dxfId="4" priority="564" operator="lessThanOrEqual">
+      <formula>J29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH30">
+    <cfRule type="cellIs" dxfId="4" priority="569" operator="lessThanOrEqual">
+      <formula>J30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH31">
+    <cfRule type="cellIs" dxfId="4" priority="574" operator="lessThanOrEqual">
+      <formula>J31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH32">
+    <cfRule type="cellIs" dxfId="4" priority="579" operator="lessThanOrEqual">
+      <formula>J32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH33">
+    <cfRule type="cellIs" dxfId="4" priority="584" operator="lessThanOrEqual">
+      <formula>J33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH34">
+    <cfRule type="cellIs" dxfId="4" priority="589" operator="lessThanOrEqual">
+      <formula>J34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH35">
+    <cfRule type="cellIs" dxfId="4" priority="594" operator="lessThanOrEqual">
+      <formula>J35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH36">
+    <cfRule type="cellIs" dxfId="4" priority="599" operator="lessThanOrEqual">
+      <formula>J36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH37">
+    <cfRule type="cellIs" dxfId="4" priority="604" operator="lessThanOrEqual">
+      <formula>J37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH40">
+    <cfRule type="cellIs" dxfId="4" priority="609" operator="lessThanOrEqual">
+      <formula>J40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH7">
+    <cfRule type="cellIs" dxfId="4" priority="479" operator="lessThanOrEqual">
+      <formula>J7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH8">
+    <cfRule type="cellIs" dxfId="4" priority="484" operator="lessThanOrEqual">
+      <formula>J8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH9">
+    <cfRule type="cellIs" dxfId="4" priority="489" operator="lessThanOrEqual">
+      <formula>J9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ10">
+    <cfRule type="cellIs" dxfId="1" priority="627" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="628" operator="lessThan">
+      <formula>H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ11">
+    <cfRule type="cellIs" dxfId="1" priority="633" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="634" operator="lessThan">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ12">
+    <cfRule type="cellIs" dxfId="1" priority="638" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="639" operator="lessThan">
+      <formula>H12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ13">
+    <cfRule type="cellIs" dxfId="1" priority="643" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="644" operator="lessThan">
+      <formula>H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ14">
+    <cfRule type="cellIs" dxfId="1" priority="648" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="649" operator="lessThan">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ15">
+    <cfRule type="cellIs" dxfId="1" priority="653" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="654" operator="lessThan">
+      <formula>H15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ21">
+    <cfRule type="cellIs" dxfId="1" priority="658" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="659" operator="lessThan">
+      <formula>H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ22">
+    <cfRule type="cellIs" dxfId="1" priority="664" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="665" operator="lessThan">
+      <formula>H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ23">
+    <cfRule type="cellIs" dxfId="1" priority="669" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="670" operator="lessThan">
+      <formula>H23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ24">
+    <cfRule type="cellIs" dxfId="1" priority="674" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="675" operator="lessThan">
+      <formula>H24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ25">
+    <cfRule type="cellIs" dxfId="1" priority="680" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="681" operator="lessThan">
+      <formula>H25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ26">
+    <cfRule type="cellIs" dxfId="1" priority="685" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="686" operator="lessThan">
+      <formula>H26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ27">
+    <cfRule type="cellIs" dxfId="1" priority="690" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="691" operator="lessThan">
+      <formula>H27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ28">
+    <cfRule type="cellIs" dxfId="1" priority="695" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="696" operator="lessThan">
+      <formula>H28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ29">
+    <cfRule type="cellIs" dxfId="1" priority="700" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="701" operator="lessThan">
+      <formula>H29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ30">
+    <cfRule type="cellIs" dxfId="1" priority="705" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="706" operator="lessThan">
+      <formula>H30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ31">
+    <cfRule type="cellIs" dxfId="1" priority="710" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="711" operator="lessThan">
+      <formula>H31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ32">
+    <cfRule type="cellIs" dxfId="1" priority="716" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="717" operator="lessThan">
+      <formula>H32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ33">
+    <cfRule type="cellIs" dxfId="1" priority="721" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="722" operator="lessThan">
+      <formula>H33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ35">
+    <cfRule type="cellIs" dxfId="1" priority="726" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="727" operator="lessThan">
+      <formula>H35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ36">
+    <cfRule type="cellIs" dxfId="1" priority="731" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="732" operator="lessThan">
+      <formula>H36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ37">
+    <cfRule type="cellIs" dxfId="1" priority="736" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="737" operator="lessThan">
       <formula>H37</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE40">
+  <conditionalFormatting sqref="AJ40">
+    <cfRule type="cellIs" dxfId="1" priority="741" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="742" operator="lessThan">
+      <formula>H40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ7">
     <cfRule type="cellIs" dxfId="1" priority="611" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="612" operator="lessThan">
-      <formula>H40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE7">
-    <cfRule type="cellIs" dxfId="1" priority="481" operator="equal">
+      <formula>H7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ8">
+    <cfRule type="cellIs" dxfId="1" priority="616" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="482" operator="lessThan">
-      <formula>H7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE8">
-    <cfRule type="cellIs" dxfId="1" priority="486" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="617" operator="lessThan">
+      <formula>H8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ9">
+    <cfRule type="cellIs" dxfId="1" priority="621" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="487" operator="lessThan">
-      <formula>H8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE9">
-    <cfRule type="cellIs" dxfId="1" priority="491" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="622" operator="lessThan">
+      <formula>H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK10">
+    <cfRule type="expression" dxfId="3" priority="629">
+      <formula>AND(AK10&gt;0,AK10&lt;10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="630" operator="greaterThan">
+      <formula>AJ10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK11">
+    <cfRule type="cellIs" dxfId="1" priority="635" operator="greaterThan">
+      <formula>AJ11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK12">
+    <cfRule type="cellIs" dxfId="1" priority="640" operator="greaterThan">
+      <formula>AJ12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK13">
+    <cfRule type="cellIs" dxfId="1" priority="645" operator="greaterThan">
+      <formula>AJ13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK14">
+    <cfRule type="cellIs" dxfId="1" priority="650" operator="greaterThan">
+      <formula>AJ14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK15">
+    <cfRule type="cellIs" dxfId="1" priority="655" operator="greaterThan">
+      <formula>AJ15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK21">
+    <cfRule type="expression" dxfId="3" priority="660">
+      <formula>AND(AK21&gt;0,AK21&lt;15000)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="661" operator="greaterThan">
+      <formula>AJ21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK22">
+    <cfRule type="cellIs" dxfId="1" priority="666" operator="greaterThan">
+      <formula>AJ22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK23">
+    <cfRule type="cellIs" dxfId="1" priority="671" operator="greaterThan">
+      <formula>AJ23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK24">
+    <cfRule type="expression" dxfId="3" priority="676">
+      <formula>AND(AK24&gt;0,AK24&lt;15000)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="677" operator="greaterThan">
+      <formula>AJ24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK25">
+    <cfRule type="cellIs" dxfId="1" priority="682" operator="greaterThan">
+      <formula>AJ25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK26">
+    <cfRule type="cellIs" dxfId="1" priority="687" operator="greaterThan">
+      <formula>AJ26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK27">
+    <cfRule type="cellIs" dxfId="1" priority="692" operator="greaterThan">
+      <formula>AJ27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK28">
+    <cfRule type="cellIs" dxfId="1" priority="697" operator="greaterThan">
+      <formula>AJ28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK29">
+    <cfRule type="cellIs" dxfId="1" priority="702" operator="greaterThan">
+      <formula>AJ29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK30">
+    <cfRule type="cellIs" dxfId="1" priority="707" operator="greaterThan">
+      <formula>AJ30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK31">
+    <cfRule type="expression" dxfId="3" priority="712">
+      <formula>AND(AK31&gt;0,AK31&lt;5)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="713" operator="greaterThan">
+      <formula>AJ31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK32">
+    <cfRule type="cellIs" dxfId="1" priority="718" operator="greaterThan">
+      <formula>AJ32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK33">
+    <cfRule type="cellIs" dxfId="1" priority="723" operator="greaterThan">
+      <formula>AJ33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK35">
+    <cfRule type="cellIs" dxfId="1" priority="728" operator="greaterThan">
+      <formula>AJ35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK36">
+    <cfRule type="cellIs" dxfId="1" priority="733" operator="greaterThan">
+      <formula>AJ36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK37">
+    <cfRule type="cellIs" dxfId="1" priority="738" operator="greaterThan">
+      <formula>AJ37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK40">
+    <cfRule type="cellIs" dxfId="1" priority="743" operator="greaterThan">
+      <formula>AJ40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK7">
+    <cfRule type="cellIs" dxfId="1" priority="613" operator="greaterThan">
+      <formula>AJ7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK8">
+    <cfRule type="cellIs" dxfId="1" priority="618" operator="greaterThan">
+      <formula>AJ8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK9">
+    <cfRule type="expression" dxfId="3" priority="623">
+      <formula>AND(AK9&gt;0,AK9&lt;10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="624" operator="greaterThan">
+      <formula>AJ9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL10">
+    <cfRule type="cellIs" dxfId="4" priority="632" operator="lessThanOrEqual">
+      <formula>I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL11">
+    <cfRule type="cellIs" dxfId="4" priority="637" operator="lessThanOrEqual">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL12">
+    <cfRule type="cellIs" dxfId="4" priority="642" operator="lessThanOrEqual">
+      <formula>I12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL13">
+    <cfRule type="cellIs" dxfId="4" priority="647" operator="lessThanOrEqual">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL14">
+    <cfRule type="cellIs" dxfId="4" priority="652" operator="lessThanOrEqual">
+      <formula>I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL15">
+    <cfRule type="cellIs" dxfId="4" priority="657" operator="lessThanOrEqual">
+      <formula>I15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL21">
+    <cfRule type="cellIs" dxfId="4" priority="663" operator="lessThanOrEqual">
+      <formula>I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL22">
+    <cfRule type="cellIs" dxfId="4" priority="668" operator="lessThanOrEqual">
+      <formula>I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL23">
+    <cfRule type="cellIs" dxfId="4" priority="673" operator="lessThanOrEqual">
+      <formula>I23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL24">
+    <cfRule type="cellIs" dxfId="4" priority="679" operator="lessThanOrEqual">
+      <formula>I24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL25">
+    <cfRule type="cellIs" dxfId="4" priority="684" operator="lessThanOrEqual">
+      <formula>I25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL26">
+    <cfRule type="cellIs" dxfId="4" priority="689" operator="lessThanOrEqual">
+      <formula>I26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL27">
+    <cfRule type="cellIs" dxfId="4" priority="694" operator="lessThanOrEqual">
+      <formula>I27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL28">
+    <cfRule type="cellIs" dxfId="4" priority="699" operator="lessThanOrEqual">
+      <formula>I28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL29">
+    <cfRule type="cellIs" dxfId="4" priority="704" operator="lessThanOrEqual">
+      <formula>I29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL30">
+    <cfRule type="cellIs" dxfId="4" priority="709" operator="lessThanOrEqual">
+      <formula>I30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL31">
+    <cfRule type="cellIs" dxfId="4" priority="715" operator="lessThanOrEqual">
+      <formula>I31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL32">
+    <cfRule type="cellIs" dxfId="4" priority="720" operator="lessThanOrEqual">
+      <formula>I32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL33">
+    <cfRule type="cellIs" dxfId="4" priority="725" operator="lessThanOrEqual">
+      <formula>I33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL35">
+    <cfRule type="cellIs" dxfId="4" priority="730" operator="lessThanOrEqual">
+      <formula>I35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL36">
+    <cfRule type="cellIs" dxfId="4" priority="735" operator="lessThanOrEqual">
+      <formula>I36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL37">
+    <cfRule type="cellIs" dxfId="4" priority="740" operator="lessThanOrEqual">
+      <formula>I37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL40">
+    <cfRule type="cellIs" dxfId="4" priority="745" operator="lessThanOrEqual">
+      <formula>I40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL7">
+    <cfRule type="cellIs" dxfId="4" priority="615" operator="lessThanOrEqual">
+      <formula>I7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL8">
+    <cfRule type="cellIs" dxfId="4" priority="620" operator="lessThanOrEqual">
+      <formula>I8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL9">
+    <cfRule type="cellIs" dxfId="4" priority="626" operator="lessThanOrEqual">
+      <formula>I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM10">
+    <cfRule type="cellIs" dxfId="4" priority="631" operator="lessThanOrEqual">
+      <formula>J10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM11">
+    <cfRule type="cellIs" dxfId="4" priority="636" operator="lessThanOrEqual">
+      <formula>J11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM12">
+    <cfRule type="cellIs" dxfId="4" priority="641" operator="lessThanOrEqual">
+      <formula>J12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM13">
+    <cfRule type="cellIs" dxfId="4" priority="646" operator="lessThanOrEqual">
+      <formula>J13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM14">
+    <cfRule type="cellIs" dxfId="4" priority="651" operator="lessThanOrEqual">
+      <formula>J14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM15">
+    <cfRule type="cellIs" dxfId="4" priority="656" operator="lessThanOrEqual">
+      <formula>J15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM21">
+    <cfRule type="cellIs" dxfId="4" priority="662" operator="lessThanOrEqual">
+      <formula>J21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM22">
+    <cfRule type="cellIs" dxfId="4" priority="667" operator="lessThanOrEqual">
+      <formula>J22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM23">
+    <cfRule type="cellIs" dxfId="4" priority="672" operator="lessThanOrEqual">
+      <formula>J23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM24">
+    <cfRule type="cellIs" dxfId="4" priority="678" operator="lessThanOrEqual">
+      <formula>J24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM25">
+    <cfRule type="cellIs" dxfId="4" priority="683" operator="lessThanOrEqual">
+      <formula>J25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM26">
+    <cfRule type="cellIs" dxfId="4" priority="688" operator="lessThanOrEqual">
+      <formula>J26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM27">
+    <cfRule type="cellIs" dxfId="4" priority="693" operator="lessThanOrEqual">
+      <formula>J27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM28">
+    <cfRule type="cellIs" dxfId="4" priority="698" operator="lessThanOrEqual">
+      <formula>J28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM29">
+    <cfRule type="cellIs" dxfId="4" priority="703" operator="lessThanOrEqual">
+      <formula>J29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM30">
+    <cfRule type="cellIs" dxfId="4" priority="708" operator="lessThanOrEqual">
+      <formula>J30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM31">
+    <cfRule type="cellIs" dxfId="4" priority="714" operator="lessThanOrEqual">
+      <formula>J31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM32">
+    <cfRule type="cellIs" dxfId="4" priority="719" operator="lessThanOrEqual">
+      <formula>J32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM33">
+    <cfRule type="cellIs" dxfId="4" priority="724" operator="lessThanOrEqual">
+      <formula>J33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM35">
+    <cfRule type="cellIs" dxfId="4" priority="729" operator="lessThanOrEqual">
+      <formula>J35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM36">
+    <cfRule type="cellIs" dxfId="4" priority="734" operator="lessThanOrEqual">
+      <formula>J36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM37">
+    <cfRule type="cellIs" dxfId="4" priority="739" operator="lessThanOrEqual">
+      <formula>J37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM40">
+    <cfRule type="cellIs" dxfId="4" priority="744" operator="lessThanOrEqual">
+      <formula>J40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM7">
+    <cfRule type="cellIs" dxfId="4" priority="614" operator="lessThanOrEqual">
+      <formula>J7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM8">
+    <cfRule type="cellIs" dxfId="4" priority="619" operator="lessThanOrEqual">
+      <formula>J8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM9">
+    <cfRule type="cellIs" dxfId="4" priority="625" operator="lessThanOrEqual">
+      <formula>J9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO12">
+    <cfRule type="cellIs" dxfId="1" priority="752" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="492" operator="lessThan">
-      <formula>H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF10">
-    <cfRule type="cellIs" dxfId="1" priority="498" operator="greaterThan">
-      <formula>AE10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF11">
-    <cfRule type="cellIs" dxfId="1" priority="503" operator="greaterThan">
-      <formula>AE11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF12">
-    <cfRule type="cellIs" dxfId="1" priority="508" operator="greaterThan">
-      <formula>AE12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF13">
-    <cfRule type="cellIs" dxfId="1" priority="513" operator="greaterThan">
-      <formula>AE13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF14">
-    <cfRule type="cellIs" dxfId="1" priority="518" operator="greaterThan">
-      <formula>AE14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF15">
-    <cfRule type="cellIs" dxfId="1" priority="523" operator="greaterThan">
-      <formula>AE15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF21">
-    <cfRule type="cellIs" dxfId="1" priority="528" operator="greaterThan">
-      <formula>AE21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF22">
-    <cfRule type="cellIs" dxfId="1" priority="533" operator="greaterThan">
-      <formula>AE22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF23">
-    <cfRule type="cellIs" dxfId="1" priority="538" operator="greaterThan">
-      <formula>AE23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF24">
-    <cfRule type="cellIs" dxfId="1" priority="543" operator="greaterThan">
-      <formula>AE24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF25">
-    <cfRule type="cellIs" dxfId="1" priority="548" operator="greaterThan">
-      <formula>AE25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF26">
-    <cfRule type="cellIs" dxfId="1" priority="553" operator="greaterThan">
-      <formula>AE26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF27">
-    <cfRule type="cellIs" dxfId="1" priority="558" operator="greaterThan">
-      <formula>AE27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF28">
-    <cfRule type="cellIs" dxfId="1" priority="563" operator="greaterThan">
-      <formula>AE28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF29">
-    <cfRule type="cellIs" dxfId="1" priority="568" operator="greaterThan">
-      <formula>AE29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF30">
-    <cfRule type="cellIs" dxfId="1" priority="573" operator="greaterThan">
-      <formula>AE30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF31">
-    <cfRule type="cellIs" dxfId="1" priority="578" operator="greaterThan">
-      <formula>AE31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF32">
-    <cfRule type="cellIs" dxfId="1" priority="583" operator="greaterThan">
-      <formula>AE32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF33">
-    <cfRule type="cellIs" dxfId="1" priority="588" operator="greaterThan">
-      <formula>AE33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF34">
-    <cfRule type="cellIs" dxfId="1" priority="593" operator="greaterThan">
-      <formula>AE34</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF35">
-    <cfRule type="cellIs" dxfId="1" priority="598" operator="greaterThan">
-      <formula>AE35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF36">
-    <cfRule type="cellIs" dxfId="1" priority="603" operator="greaterThan">
-      <formula>AE36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF37">
-    <cfRule type="cellIs" dxfId="1" priority="608" operator="greaterThan">
-      <formula>AE37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF40">
-    <cfRule type="cellIs" dxfId="1" priority="613" operator="greaterThan">
-      <formula>AE40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF7">
-    <cfRule type="cellIs" dxfId="1" priority="483" operator="greaterThan">
-      <formula>AE7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF8">
-    <cfRule type="cellIs" dxfId="1" priority="488" operator="greaterThan">
-      <formula>AE8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF9">
-    <cfRule type="cellIs" dxfId="1" priority="493" operator="greaterThan">
-      <formula>AE9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG10">
-    <cfRule type="cellIs" dxfId="4" priority="500" operator="lessThanOrEqual">
-      <formula>I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG11">
-    <cfRule type="cellIs" dxfId="4" priority="505" operator="lessThanOrEqual">
-      <formula>I11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG12">
-    <cfRule type="cellIs" dxfId="4" priority="510" operator="lessThanOrEqual">
-      <formula>I12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG13">
-    <cfRule type="cellIs" dxfId="4" priority="515" operator="lessThanOrEqual">
-      <formula>I13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG14">
-    <cfRule type="cellIs" dxfId="4" priority="520" operator="lessThanOrEqual">
-      <formula>I14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG15">
-    <cfRule type="cellIs" dxfId="4" priority="525" operator="lessThanOrEqual">
-      <formula>I15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG21">
-    <cfRule type="cellIs" dxfId="4" priority="530" operator="lessThanOrEqual">
-      <formula>I21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG22">
-    <cfRule type="cellIs" dxfId="4" priority="535" operator="lessThanOrEqual">
-      <formula>I22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG23">
-    <cfRule type="cellIs" dxfId="4" priority="540" operator="lessThanOrEqual">
-      <formula>I23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG24">
-    <cfRule type="cellIs" dxfId="4" priority="545" operator="lessThanOrEqual">
-      <formula>I24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG25">
-    <cfRule type="cellIs" dxfId="4" priority="550" operator="lessThanOrEqual">
-      <formula>I25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG26">
-    <cfRule type="cellIs" dxfId="4" priority="555" operator="lessThanOrEqual">
-      <formula>I26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG27">
-    <cfRule type="cellIs" dxfId="4" priority="560" operator="lessThanOrEqual">
-      <formula>I27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG28">
-    <cfRule type="cellIs" dxfId="4" priority="565" operator="lessThanOrEqual">
-      <formula>I28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG29">
-    <cfRule type="cellIs" dxfId="4" priority="570" operator="lessThanOrEqual">
-      <formula>I29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG30">
-    <cfRule type="cellIs" dxfId="4" priority="575" operator="lessThanOrEqual">
-      <formula>I30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG31">
-    <cfRule type="cellIs" dxfId="4" priority="580" operator="lessThanOrEqual">
-      <formula>I31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG32">
-    <cfRule type="cellIs" dxfId="4" priority="585" operator="lessThanOrEqual">
-      <formula>I32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG33">
-    <cfRule type="cellIs" dxfId="4" priority="590" operator="lessThanOrEqual">
-      <formula>I33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG34">
-    <cfRule type="cellIs" dxfId="4" priority="595" operator="lessThanOrEqual">
-      <formula>I34</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG35">
-    <cfRule type="cellIs" dxfId="4" priority="600" operator="lessThanOrEqual">
-      <formula>I35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG36">
-    <cfRule type="cellIs" dxfId="4" priority="605" operator="lessThanOrEqual">
-      <formula>I36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG37">
-    <cfRule type="cellIs" dxfId="4" priority="610" operator="lessThanOrEqual">
-      <formula>I37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG40">
-    <cfRule type="cellIs" dxfId="4" priority="615" operator="lessThanOrEqual">
-      <formula>I40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG7">
-    <cfRule type="cellIs" dxfId="4" priority="485" operator="lessThanOrEqual">
-      <formula>I7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG8">
-    <cfRule type="cellIs" dxfId="4" priority="490" operator="lessThanOrEqual">
-      <formula>I8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG9">
-    <cfRule type="cellIs" dxfId="4" priority="495" operator="lessThanOrEqual">
-      <formula>I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH10">
-    <cfRule type="cellIs" dxfId="4" priority="499" operator="lessThanOrEqual">
-      <formula>J10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH11">
-    <cfRule type="cellIs" dxfId="4" priority="504" operator="lessThanOrEqual">
-      <formula>J11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH12">
-    <cfRule type="cellIs" dxfId="4" priority="509" operator="lessThanOrEqual">
-      <formula>J12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH13">
-    <cfRule type="cellIs" dxfId="4" priority="514" operator="lessThanOrEqual">
-      <formula>J13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH14">
-    <cfRule type="cellIs" dxfId="4" priority="519" operator="lessThanOrEqual">
-      <formula>J14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH15">
-    <cfRule type="cellIs" dxfId="4" priority="524" operator="lessThanOrEqual">
-      <formula>J15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH21">
-    <cfRule type="cellIs" dxfId="4" priority="529" operator="lessThanOrEqual">
-      <formula>J21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH22">
-    <cfRule type="cellIs" dxfId="4" priority="534" operator="lessThanOrEqual">
-      <formula>J22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH23">
-    <cfRule type="cellIs" dxfId="4" priority="539" operator="lessThanOrEqual">
-      <formula>J23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH24">
-    <cfRule type="cellIs" dxfId="4" priority="544" operator="lessThanOrEqual">
-      <formula>J24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH25">
-    <cfRule type="cellIs" dxfId="4" priority="549" operator="lessThanOrEqual">
-      <formula>J25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH26">
-    <cfRule type="cellIs" dxfId="4" priority="554" operator="lessThanOrEqual">
-      <formula>J26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH27">
-    <cfRule type="cellIs" dxfId="4" priority="559" operator="lessThanOrEqual">
-      <formula>J27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH28">
-    <cfRule type="cellIs" dxfId="4" priority="564" operator="lessThanOrEqual">
-      <formula>J28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH29">
-    <cfRule type="cellIs" dxfId="4" priority="569" operator="lessThanOrEqual">
-      <formula>J29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH30">
-    <cfRule type="cellIs" dxfId="4" priority="574" operator="lessThanOrEqual">
-      <formula>J30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH31">
-    <cfRule type="cellIs" dxfId="4" priority="579" operator="lessThanOrEqual">
-      <formula>J31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH32">
-    <cfRule type="cellIs" dxfId="4" priority="584" operator="lessThanOrEqual">
-      <formula>J32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH33">
-    <cfRule type="cellIs" dxfId="4" priority="589" operator="lessThanOrEqual">
-      <formula>J33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH34">
-    <cfRule type="cellIs" dxfId="4" priority="594" operator="lessThanOrEqual">
-      <formula>J34</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH35">
-    <cfRule type="cellIs" dxfId="4" priority="599" operator="lessThanOrEqual">
-      <formula>J35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH36">
-    <cfRule type="cellIs" dxfId="4" priority="604" operator="lessThanOrEqual">
-      <formula>J36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH37">
-    <cfRule type="cellIs" dxfId="4" priority="609" operator="lessThanOrEqual">
-      <formula>J37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH40">
-    <cfRule type="cellIs" dxfId="4" priority="614" operator="lessThanOrEqual">
-      <formula>J40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH7">
-    <cfRule type="cellIs" dxfId="4" priority="484" operator="lessThanOrEqual">
-      <formula>J7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH8">
-    <cfRule type="cellIs" dxfId="4" priority="489" operator="lessThanOrEqual">
-      <formula>J8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH9">
-    <cfRule type="cellIs" dxfId="4" priority="494" operator="lessThanOrEqual">
-      <formula>J9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ10">
-    <cfRule type="cellIs" dxfId="1" priority="632" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="753" operator="lessThan">
+      <formula>H12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO21">
+    <cfRule type="cellIs" dxfId="1" priority="758" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="633" operator="lessThan">
-      <formula>H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ11">
-    <cfRule type="cellIs" dxfId="1" priority="638" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="759" operator="lessThan">
+      <formula>H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO22">
+    <cfRule type="cellIs" dxfId="1" priority="764" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="639" operator="lessThan">
-      <formula>H11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ12">
-    <cfRule type="cellIs" dxfId="1" priority="643" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="765" operator="lessThan">
+      <formula>H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO23">
+    <cfRule type="cellIs" dxfId="1" priority="770" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="644" operator="lessThan">
-      <formula>H12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ13">
-    <cfRule type="cellIs" dxfId="1" priority="648" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="771" operator="lessThan">
+      <formula>H23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO25">
+    <cfRule type="cellIs" dxfId="1" priority="776" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="649" operator="lessThan">
-      <formula>H13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ14">
-    <cfRule type="cellIs" dxfId="1" priority="653" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="777" operator="lessThan">
+      <formula>H25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO27">
+    <cfRule type="cellIs" dxfId="1" priority="782" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="654" operator="lessThan">
-      <formula>H14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ15">
-    <cfRule type="cellIs" dxfId="1" priority="658" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="783" operator="lessThan">
+      <formula>H27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO29">
+    <cfRule type="cellIs" dxfId="1" priority="788" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="659" operator="lessThan">
-      <formula>H15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="1" priority="663" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="789" operator="lessThan">
+      <formula>H29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO31">
+    <cfRule type="cellIs" dxfId="1" priority="794" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="664" operator="lessThan">
-      <formula>H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ22">
-    <cfRule type="cellIs" dxfId="1" priority="669" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="795" operator="lessThan">
+      <formula>H31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO33">
+    <cfRule type="cellIs" dxfId="1" priority="800" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="670" operator="lessThan">
-      <formula>H22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ23">
-    <cfRule type="cellIs" dxfId="1" priority="674" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="801" operator="lessThan">
+      <formula>H33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO36">
+    <cfRule type="cellIs" dxfId="1" priority="806" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="675" operator="lessThan">
-      <formula>H23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ24">
-    <cfRule type="cellIs" dxfId="1" priority="679" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="807" operator="lessThan">
+      <formula>H36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO37">
+    <cfRule type="cellIs" dxfId="1" priority="812" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="680" operator="lessThan">
-      <formula>H24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ25">
-    <cfRule type="cellIs" dxfId="1" priority="685" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="686" operator="lessThan">
-      <formula>H25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ26">
-    <cfRule type="cellIs" dxfId="1" priority="690" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="691" operator="lessThan">
-      <formula>H26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ27">
-    <cfRule type="cellIs" dxfId="1" priority="695" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="696" operator="lessThan">
-      <formula>H27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ28">
-    <cfRule type="cellIs" dxfId="1" priority="700" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="701" operator="lessThan">
-      <formula>H28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ29">
-    <cfRule type="cellIs" dxfId="1" priority="705" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="706" operator="lessThan">
-      <formula>H29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ30">
-    <cfRule type="cellIs" dxfId="1" priority="710" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="711" operator="lessThan">
-      <formula>H30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ31">
-    <cfRule type="cellIs" dxfId="1" priority="715" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="716" operator="lessThan">
-      <formula>H31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ32">
-    <cfRule type="cellIs" dxfId="1" priority="721" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="722" operator="lessThan">
-      <formula>H32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ33">
-    <cfRule type="cellIs" dxfId="1" priority="726" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="727" operator="lessThan">
-      <formula>H33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ35">
-    <cfRule type="cellIs" dxfId="1" priority="731" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="732" operator="lessThan">
-      <formula>H35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ36">
-    <cfRule type="cellIs" dxfId="1" priority="736" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="737" operator="lessThan">
-      <formula>H36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ37">
-    <cfRule type="cellIs" dxfId="1" priority="741" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="742" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="813" operator="lessThan">
       <formula>H37</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ40">
+  <conditionalFormatting sqref="AO9">
     <cfRule type="cellIs" dxfId="1" priority="746" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="747" operator="lessThan">
-      <formula>H40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ7">
-    <cfRule type="cellIs" dxfId="1" priority="616" operator="equal">
+      <formula>H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP12">
+    <cfRule type="expression" dxfId="3" priority="754">
+      <formula>AND(AP12&gt;0,AP12&lt;1000)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="755" operator="greaterThan">
+      <formula>AO12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP21">
+    <cfRule type="expression" dxfId="3" priority="760">
+      <formula>AND(AP21&gt;0,AP21&lt;1000)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="761" operator="greaterThan">
+      <formula>AO21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP22">
+    <cfRule type="expression" dxfId="3" priority="766">
+      <formula>AND(AP22&gt;0,AP22&lt;1000)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="767" operator="greaterThan">
+      <formula>AO22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP23">
+    <cfRule type="expression" dxfId="3" priority="772">
+      <formula>AND(AP23&gt;0,AP23&lt;1000)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="773" operator="greaterThan">
+      <formula>AO23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP25">
+    <cfRule type="expression" dxfId="3" priority="778">
+      <formula>AND(AP25&gt;0,AP25&lt;1000)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="779" operator="greaterThan">
+      <formula>AO25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP27">
+    <cfRule type="expression" dxfId="3" priority="784">
+      <formula>AND(AP27&gt;0,AP27&lt;1000)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="785" operator="greaterThan">
+      <formula>AO27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP29">
+    <cfRule type="expression" dxfId="3" priority="790">
+      <formula>AND(AP29&gt;0,AP29&lt;1000)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="791" operator="greaterThan">
+      <formula>AO29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP31">
+    <cfRule type="expression" dxfId="3" priority="796">
+      <formula>AND(AP31&gt;0,AP31&lt;30)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="797" operator="greaterThan">
+      <formula>AO31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP33">
+    <cfRule type="expression" dxfId="3" priority="802">
+      <formula>AND(AP33&gt;0,AP33&lt;18)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="803" operator="greaterThan">
+      <formula>AO33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP36">
+    <cfRule type="expression" dxfId="3" priority="808">
+      <formula>AND(AP36&gt;0,AP36&lt;50)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="809" operator="greaterThan">
+      <formula>AO36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP37">
+    <cfRule type="expression" dxfId="3" priority="814">
+      <formula>AND(AP37&gt;0,AP37&lt;20)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="815" operator="greaterThan">
+      <formula>AO37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP9">
+    <cfRule type="expression" dxfId="3" priority="748">
+      <formula>AND(AP9&gt;0,AP9&lt;20)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="749" operator="greaterThan">
+      <formula>AO9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ12">
+    <cfRule type="cellIs" dxfId="4" priority="757" operator="lessThanOrEqual">
+      <formula>I12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ21">
+    <cfRule type="cellIs" dxfId="4" priority="763" operator="lessThanOrEqual">
+      <formula>I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ22">
+    <cfRule type="cellIs" dxfId="4" priority="769" operator="lessThanOrEqual">
+      <formula>I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ23">
+    <cfRule type="cellIs" dxfId="4" priority="775" operator="lessThanOrEqual">
+      <formula>I23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ25">
+    <cfRule type="cellIs" dxfId="4" priority="781" operator="lessThanOrEqual">
+      <formula>I25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ27">
+    <cfRule type="cellIs" dxfId="4" priority="787" operator="lessThanOrEqual">
+      <formula>I27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ29">
+    <cfRule type="cellIs" dxfId="4" priority="793" operator="lessThanOrEqual">
+      <formula>I29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ31">
+    <cfRule type="cellIs" dxfId="4" priority="799" operator="lessThanOrEqual">
+      <formula>I31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ33">
+    <cfRule type="cellIs" dxfId="4" priority="805" operator="lessThanOrEqual">
+      <formula>I33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ36">
+    <cfRule type="cellIs" dxfId="4" priority="811" operator="lessThanOrEqual">
+      <formula>I36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ37">
+    <cfRule type="cellIs" dxfId="4" priority="817" operator="lessThanOrEqual">
+      <formula>I37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ9">
+    <cfRule type="cellIs" dxfId="4" priority="751" operator="lessThanOrEqual">
+      <formula>I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR12">
+    <cfRule type="cellIs" dxfId="4" priority="756" operator="lessThanOrEqual">
+      <formula>J12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR21">
+    <cfRule type="cellIs" dxfId="4" priority="762" operator="lessThanOrEqual">
+      <formula>J21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR22">
+    <cfRule type="cellIs" dxfId="4" priority="768" operator="lessThanOrEqual">
+      <formula>J22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR23">
+    <cfRule type="cellIs" dxfId="4" priority="774" operator="lessThanOrEqual">
+      <formula>J23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR25">
+    <cfRule type="cellIs" dxfId="4" priority="780" operator="lessThanOrEqual">
+      <formula>J25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR27">
+    <cfRule type="cellIs" dxfId="4" priority="786" operator="lessThanOrEqual">
+      <formula>J27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR29">
+    <cfRule type="cellIs" dxfId="4" priority="792" operator="lessThanOrEqual">
+      <formula>J29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR31">
+    <cfRule type="cellIs" dxfId="4" priority="798" operator="lessThanOrEqual">
+      <formula>J31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR33">
+    <cfRule type="cellIs" dxfId="4" priority="804" operator="lessThanOrEqual">
+      <formula>J33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR36">
+    <cfRule type="cellIs" dxfId="4" priority="810" operator="lessThanOrEqual">
+      <formula>J36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR37">
+    <cfRule type="cellIs" dxfId="4" priority="816" operator="lessThanOrEqual">
+      <formula>J37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR9">
+    <cfRule type="cellIs" dxfId="4" priority="750" operator="lessThanOrEqual">
+      <formula>J9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT14">
+    <cfRule type="cellIs" dxfId="1" priority="818" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="617" operator="lessThan">
-      <formula>H7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ8">
-    <cfRule type="cellIs" dxfId="1" priority="621" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="819" operator="lessThan">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT15">
+    <cfRule type="cellIs" dxfId="1" priority="824" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="622" operator="lessThan">
-      <formula>H8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ9">
-    <cfRule type="cellIs" dxfId="1" priority="626" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="825" operator="lessThan">
+      <formula>H15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT36">
+    <cfRule type="cellIs" dxfId="1" priority="830" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="627" operator="lessThan">
-      <formula>H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK10">
-    <cfRule type="expression" dxfId="3" priority="634">
-      <formula>AND(AK10&gt;0,AK10&lt;10)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="635" operator="greaterThan">
-      <formula>AJ10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK11">
-    <cfRule type="cellIs" dxfId="1" priority="640" operator="greaterThan">
-      <formula>AJ11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK12">
-    <cfRule type="cellIs" dxfId="1" priority="645" operator="greaterThan">
-      <formula>AJ12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK13">
-    <cfRule type="cellIs" dxfId="1" priority="650" operator="greaterThan">
-      <formula>AJ13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK14">
-    <cfRule type="cellIs" dxfId="1" priority="655" operator="greaterThan">
-      <formula>AJ14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK15">
-    <cfRule type="cellIs" dxfId="1" priority="660" operator="greaterThan">
-      <formula>AJ15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK21">
-    <cfRule type="expression" dxfId="3" priority="665">
-      <formula>AND(AK21&gt;0,AK21&lt;15000)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="666" operator="greaterThan">
-      <formula>AJ21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK22">
-    <cfRule type="cellIs" dxfId="1" priority="671" operator="greaterThan">
-      <formula>AJ22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK23">
-    <cfRule type="cellIs" dxfId="1" priority="676" operator="greaterThan">
-      <formula>AJ23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK24">
-    <cfRule type="expression" dxfId="3" priority="681">
-      <formula>AND(AK24&gt;0,AK24&lt;15000)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="682" operator="greaterThan">
-      <formula>AJ24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK25">
-    <cfRule type="cellIs" dxfId="1" priority="687" operator="greaterThan">
-      <formula>AJ25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK26">
-    <cfRule type="cellIs" dxfId="1" priority="692" operator="greaterThan">
-      <formula>AJ26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK27">
-    <cfRule type="cellIs" dxfId="1" priority="697" operator="greaterThan">
-      <formula>AJ27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK28">
-    <cfRule type="cellIs" dxfId="1" priority="702" operator="greaterThan">
-      <formula>AJ28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK29">
-    <cfRule type="cellIs" dxfId="1" priority="707" operator="greaterThan">
-      <formula>AJ29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK30">
-    <cfRule type="cellIs" dxfId="1" priority="712" operator="greaterThan">
-      <formula>AJ30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK31">
-    <cfRule type="expression" dxfId="3" priority="717">
-      <formula>AND(AK31&gt;0,AK31&lt;5)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="718" operator="greaterThan">
-      <formula>AJ31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK32">
-    <cfRule type="cellIs" dxfId="1" priority="723" operator="greaterThan">
-      <formula>AJ32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK33">
-    <cfRule type="cellIs" dxfId="1" priority="728" operator="greaterThan">
-      <formula>AJ33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK35">
-    <cfRule type="cellIs" dxfId="1" priority="733" operator="greaterThan">
-      <formula>AJ35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK36">
-    <cfRule type="cellIs" dxfId="1" priority="738" operator="greaterThan">
-      <formula>AJ36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK37">
-    <cfRule type="cellIs" dxfId="1" priority="743" operator="greaterThan">
-      <formula>AJ37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK40">
-    <cfRule type="cellIs" dxfId="1" priority="748" operator="greaterThan">
-      <formula>AJ40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK7">
-    <cfRule type="cellIs" dxfId="1" priority="618" operator="greaterThan">
-      <formula>AJ7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK8">
-    <cfRule type="cellIs" dxfId="1" priority="623" operator="greaterThan">
-      <formula>AJ8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK9">
-    <cfRule type="expression" dxfId="3" priority="628">
-      <formula>AND(AK9&gt;0,AK9&lt;10)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="629" operator="greaterThan">
-      <formula>AJ9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL10">
-    <cfRule type="cellIs" dxfId="4" priority="637" operator="lessThanOrEqual">
-      <formula>I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL11">
-    <cfRule type="cellIs" dxfId="4" priority="642" operator="lessThanOrEqual">
-      <formula>I11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL12">
-    <cfRule type="cellIs" dxfId="4" priority="647" operator="lessThanOrEqual">
-      <formula>I12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL13">
-    <cfRule type="cellIs" dxfId="4" priority="652" operator="lessThanOrEqual">
-      <formula>I13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL14">
-    <cfRule type="cellIs" dxfId="4" priority="657" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="831" operator="lessThan">
+      <formula>H36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT37">
+    <cfRule type="cellIs" dxfId="1" priority="836" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="837" operator="lessThan">
+      <formula>H37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU14">
+    <cfRule type="expression" dxfId="3" priority="820">
+      <formula>AND(AU14&gt;0,AU14&lt;5)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="821" operator="greaterThan">
+      <formula>AT14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU15">
+    <cfRule type="expression" dxfId="3" priority="826">
+      <formula>AND(AU15&gt;0,AU15&lt;5)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="827" operator="greaterThan">
+      <formula>AT15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU36">
+    <cfRule type="expression" dxfId="3" priority="832">
+      <formula>AND(AU36&gt;0,AU36&lt;5)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="833" operator="greaterThan">
+      <formula>AT36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU37">
+    <cfRule type="cellIs" dxfId="1" priority="838" operator="greaterThan">
+      <formula>AT37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AV14">
+    <cfRule type="cellIs" dxfId="4" priority="823" operator="lessThanOrEqual">
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL15">
-    <cfRule type="cellIs" dxfId="4" priority="662" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AV15">
+    <cfRule type="cellIs" dxfId="4" priority="829" operator="lessThanOrEqual">
       <formula>I15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL21">
-    <cfRule type="cellIs" dxfId="4" priority="668" operator="lessThanOrEqual">
-      <formula>I21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL22">
-    <cfRule type="cellIs" dxfId="4" priority="673" operator="lessThanOrEqual">
-      <formula>I22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL23">
-    <cfRule type="cellIs" dxfId="4" priority="678" operator="lessThanOrEqual">
-      <formula>I23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL24">
-    <cfRule type="cellIs" dxfId="4" priority="684" operator="lessThanOrEqual">
-      <formula>I24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL25">
-    <cfRule type="cellIs" dxfId="4" priority="689" operator="lessThanOrEqual">
-      <formula>I25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL26">
-    <cfRule type="cellIs" dxfId="4" priority="694" operator="lessThanOrEqual">
-      <formula>I26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL27">
-    <cfRule type="cellIs" dxfId="4" priority="699" operator="lessThanOrEqual">
-      <formula>I27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL28">
-    <cfRule type="cellIs" dxfId="4" priority="704" operator="lessThanOrEqual">
-      <formula>I28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL29">
-    <cfRule type="cellIs" dxfId="4" priority="709" operator="lessThanOrEqual">
-      <formula>I29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL30">
-    <cfRule type="cellIs" dxfId="4" priority="714" operator="lessThanOrEqual">
-      <formula>I30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL31">
-    <cfRule type="cellIs" dxfId="4" priority="720" operator="lessThanOrEqual">
-      <formula>I31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL32">
-    <cfRule type="cellIs" dxfId="4" priority="725" operator="lessThanOrEqual">
-      <formula>I32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL33">
-    <cfRule type="cellIs" dxfId="4" priority="730" operator="lessThanOrEqual">
-      <formula>I33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL35">
-    <cfRule type="cellIs" dxfId="4" priority="735" operator="lessThanOrEqual">
-      <formula>I35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL36">
-    <cfRule type="cellIs" dxfId="4" priority="740" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AV36">
+    <cfRule type="cellIs" dxfId="4" priority="835" operator="lessThanOrEqual">
       <formula>I36</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL37">
-    <cfRule type="cellIs" dxfId="4" priority="745" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AV37">
+    <cfRule type="cellIs" dxfId="4" priority="840" operator="lessThanOrEqual">
       <formula>I37</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL40">
-    <cfRule type="cellIs" dxfId="4" priority="750" operator="lessThanOrEqual">
-      <formula>I40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL7">
-    <cfRule type="cellIs" dxfId="4" priority="620" operator="lessThanOrEqual">
-      <formula>I7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL8">
-    <cfRule type="cellIs" dxfId="4" priority="625" operator="lessThanOrEqual">
-      <formula>I8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL9">
-    <cfRule type="cellIs" dxfId="4" priority="631" operator="lessThanOrEqual">
-      <formula>I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM10">
-    <cfRule type="cellIs" dxfId="4" priority="636" operator="lessThanOrEqual">
-      <formula>J10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM11">
-    <cfRule type="cellIs" dxfId="4" priority="641" operator="lessThanOrEqual">
-      <formula>J11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM12">
-    <cfRule type="cellIs" dxfId="4" priority="646" operator="lessThanOrEqual">
-      <formula>J12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM13">
-    <cfRule type="cellIs" dxfId="4" priority="651" operator="lessThanOrEqual">
-      <formula>J13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM14">
-    <cfRule type="cellIs" dxfId="4" priority="656" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AW14">
+    <cfRule type="cellIs" dxfId="4" priority="822" operator="lessThanOrEqual">
       <formula>J14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM15">
-    <cfRule type="cellIs" dxfId="4" priority="661" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AW15">
+    <cfRule type="cellIs" dxfId="4" priority="828" operator="lessThanOrEqual">
       <formula>J15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM21">
-    <cfRule type="cellIs" dxfId="4" priority="667" operator="lessThanOrEqual">
-      <formula>J21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM22">
-    <cfRule type="cellIs" dxfId="4" priority="672" operator="lessThanOrEqual">
-      <formula>J22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM23">
-    <cfRule type="cellIs" dxfId="4" priority="677" operator="lessThanOrEqual">
-      <formula>J23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM24">
-    <cfRule type="cellIs" dxfId="4" priority="683" operator="lessThanOrEqual">
-      <formula>J24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM25">
-    <cfRule type="cellIs" dxfId="4" priority="688" operator="lessThanOrEqual">
-      <formula>J25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM26">
-    <cfRule type="cellIs" dxfId="4" priority="693" operator="lessThanOrEqual">
-      <formula>J26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM27">
-    <cfRule type="cellIs" dxfId="4" priority="698" operator="lessThanOrEqual">
-      <formula>J27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM28">
-    <cfRule type="cellIs" dxfId="4" priority="703" operator="lessThanOrEqual">
-      <formula>J28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM29">
-    <cfRule type="cellIs" dxfId="4" priority="708" operator="lessThanOrEqual">
-      <formula>J29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM30">
-    <cfRule type="cellIs" dxfId="4" priority="713" operator="lessThanOrEqual">
-      <formula>J30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM31">
-    <cfRule type="cellIs" dxfId="4" priority="719" operator="lessThanOrEqual">
-      <formula>J31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM32">
-    <cfRule type="cellIs" dxfId="4" priority="724" operator="lessThanOrEqual">
-      <formula>J32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM33">
-    <cfRule type="cellIs" dxfId="4" priority="729" operator="lessThanOrEqual">
-      <formula>J33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM35">
-    <cfRule type="cellIs" dxfId="4" priority="734" operator="lessThanOrEqual">
-      <formula>J35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM36">
-    <cfRule type="cellIs" dxfId="4" priority="739" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AW36">
+    <cfRule type="cellIs" dxfId="4" priority="834" operator="lessThanOrEqual">
       <formula>J36</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM37">
-    <cfRule type="cellIs" dxfId="4" priority="744" operator="lessThanOrEqual">
-      <formula>J37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM40">
-    <cfRule type="cellIs" dxfId="4" priority="749" operator="lessThanOrEqual">
-      <formula>J40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM7">
-    <cfRule type="cellIs" dxfId="4" priority="619" operator="lessThanOrEqual">
-      <formula>J7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM8">
-    <cfRule type="cellIs" dxfId="4" priority="624" operator="lessThanOrEqual">
-      <formula>J8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM9">
-    <cfRule type="cellIs" dxfId="4" priority="630" operator="lessThanOrEqual">
-      <formula>J9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO12">
-    <cfRule type="cellIs" dxfId="1" priority="757" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="758" operator="lessThan">
-      <formula>H12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO21">
-    <cfRule type="cellIs" dxfId="1" priority="763" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="764" operator="lessThan">
-      <formula>H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO22">
-    <cfRule type="cellIs" dxfId="1" priority="769" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="770" operator="lessThan">
-      <formula>H22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO23">
-    <cfRule type="cellIs" dxfId="1" priority="775" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="776" operator="lessThan">
-      <formula>H23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO25">
-    <cfRule type="cellIs" dxfId="1" priority="781" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="782" operator="lessThan">
-      <formula>H25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO27">
-    <cfRule type="cellIs" dxfId="1" priority="787" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="788" operator="lessThan">
-      <formula>H27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO29">
-    <cfRule type="cellIs" dxfId="1" priority="793" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="794" operator="lessThan">
-      <formula>H29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO31">
-    <cfRule type="cellIs" dxfId="1" priority="799" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="800" operator="lessThan">
-      <formula>H31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO33">
-    <cfRule type="cellIs" dxfId="1" priority="805" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="806" operator="lessThan">
-      <formula>H33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO36">
-    <cfRule type="cellIs" dxfId="1" priority="811" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="812" operator="lessThan">
-      <formula>H36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO37">
-    <cfRule type="cellIs" dxfId="1" priority="817" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="818" operator="lessThan">
-      <formula>H37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO9">
-    <cfRule type="cellIs" dxfId="1" priority="751" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="752" operator="lessThan">
-      <formula>H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP12">
-    <cfRule type="expression" dxfId="3" priority="759">
-      <formula>AND(AP12&gt;0,AP12&lt;1000)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="760" operator="greaterThan">
-      <formula>AO12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP21">
-    <cfRule type="expression" dxfId="3" priority="765">
-      <formula>AND(AP21&gt;0,AP21&lt;1000)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="766" operator="greaterThan">
-      <formula>AO21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP22">
-    <cfRule type="expression" dxfId="3" priority="771">
-      <formula>AND(AP22&gt;0,AP22&lt;1000)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="772" operator="greaterThan">
-      <formula>AO22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP23">
-    <cfRule type="expression" dxfId="3" priority="777">
-      <formula>AND(AP23&gt;0,AP23&lt;1000)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="778" operator="greaterThan">
-      <formula>AO23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP25">
-    <cfRule type="expression" dxfId="3" priority="783">
-      <formula>AND(AP25&gt;0,AP25&lt;1000)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="784" operator="greaterThan">
-      <formula>AO25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP27">
-    <cfRule type="expression" dxfId="3" priority="789">
-      <formula>AND(AP27&gt;0,AP27&lt;1000)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="790" operator="greaterThan">
-      <formula>AO27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP29">
-    <cfRule type="expression" dxfId="3" priority="795">
-      <formula>AND(AP29&gt;0,AP29&lt;1000)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="796" operator="greaterThan">
-      <formula>AO29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP31">
-    <cfRule type="expression" dxfId="3" priority="801">
-      <formula>AND(AP31&gt;0,AP31&lt;30)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="802" operator="greaterThan">
-      <formula>AO31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP33">
-    <cfRule type="expression" dxfId="3" priority="807">
-      <formula>AND(AP33&gt;0,AP33&lt;18)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="808" operator="greaterThan">
-      <formula>AO33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP36">
-    <cfRule type="expression" dxfId="3" priority="813">
-      <formula>AND(AP36&gt;0,AP36&lt;50)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="814" operator="greaterThan">
-      <formula>AO36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP37">
-    <cfRule type="expression" dxfId="3" priority="819">
-      <formula>AND(AP37&gt;0,AP37&lt;20)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="820" operator="greaterThan">
-      <formula>AO37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP9">
-    <cfRule type="expression" dxfId="3" priority="753">
-      <formula>AND(AP9&gt;0,AP9&lt;20)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="754" operator="greaterThan">
-      <formula>AO9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ12">
-    <cfRule type="cellIs" dxfId="4" priority="762" operator="lessThanOrEqual">
-      <formula>I12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ21">
-    <cfRule type="cellIs" dxfId="4" priority="768" operator="lessThanOrEqual">
-      <formula>I21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ22">
-    <cfRule type="cellIs" dxfId="4" priority="774" operator="lessThanOrEqual">
-      <formula>I22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ23">
-    <cfRule type="cellIs" dxfId="4" priority="780" operator="lessThanOrEqual">
-      <formula>I23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ25">
-    <cfRule type="cellIs" dxfId="4" priority="786" operator="lessThanOrEqual">
-      <formula>I25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ27">
-    <cfRule type="cellIs" dxfId="4" priority="792" operator="lessThanOrEqual">
-      <formula>I27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ29">
-    <cfRule type="cellIs" dxfId="4" priority="798" operator="lessThanOrEqual">
-      <formula>I29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ31">
-    <cfRule type="cellIs" dxfId="4" priority="804" operator="lessThanOrEqual">
-      <formula>I31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ33">
-    <cfRule type="cellIs" dxfId="4" priority="810" operator="lessThanOrEqual">
-      <formula>I33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ36">
-    <cfRule type="cellIs" dxfId="4" priority="816" operator="lessThanOrEqual">
-      <formula>I36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ37">
-    <cfRule type="cellIs" dxfId="4" priority="822" operator="lessThanOrEqual">
-      <formula>I37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ9">
-    <cfRule type="cellIs" dxfId="4" priority="756" operator="lessThanOrEqual">
-      <formula>I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR12">
-    <cfRule type="cellIs" dxfId="4" priority="761" operator="lessThanOrEqual">
-      <formula>J12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR21">
-    <cfRule type="cellIs" dxfId="4" priority="767" operator="lessThanOrEqual">
-      <formula>J21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR22">
-    <cfRule type="cellIs" dxfId="4" priority="773" operator="lessThanOrEqual">
-      <formula>J22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR23">
-    <cfRule type="cellIs" dxfId="4" priority="779" operator="lessThanOrEqual">
-      <formula>J23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR25">
-    <cfRule type="cellIs" dxfId="4" priority="785" operator="lessThanOrEqual">
-      <formula>J25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR27">
-    <cfRule type="cellIs" dxfId="4" priority="791" operator="lessThanOrEqual">
-      <formula>J27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR29">
-    <cfRule type="cellIs" dxfId="4" priority="797" operator="lessThanOrEqual">
-      <formula>J29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR31">
-    <cfRule type="cellIs" dxfId="4" priority="803" operator="lessThanOrEqual">
-      <formula>J31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR33">
-    <cfRule type="cellIs" dxfId="4" priority="809" operator="lessThanOrEqual">
-      <formula>J33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR36">
-    <cfRule type="cellIs" dxfId="4" priority="815" operator="lessThanOrEqual">
-      <formula>J36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR37">
-    <cfRule type="cellIs" dxfId="4" priority="821" operator="lessThanOrEqual">
-      <formula>J37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR9">
-    <cfRule type="cellIs" dxfId="4" priority="755" operator="lessThanOrEqual">
-      <formula>J9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT14">
-    <cfRule type="cellIs" dxfId="1" priority="823" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="824" operator="lessThan">
-      <formula>H14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT15">
-    <cfRule type="cellIs" dxfId="1" priority="829" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="830" operator="lessThan">
-      <formula>H15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT30">
-    <cfRule type="cellIs" dxfId="1" priority="835" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="836" operator="lessThan">
-      <formula>H30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT36">
-    <cfRule type="cellIs" dxfId="1" priority="841" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="842" operator="lessThan">
-      <formula>H36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT37">
-    <cfRule type="cellIs" dxfId="1" priority="847" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="848" operator="lessThan">
-      <formula>H37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU14">
-    <cfRule type="expression" dxfId="3" priority="825">
-      <formula>AND(AU14&gt;0,AU14&lt;5)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="826" operator="greaterThan">
-      <formula>AT14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU15">
-    <cfRule type="expression" dxfId="3" priority="831">
-      <formula>AND(AU15&gt;0,AU15&lt;5)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="832" operator="greaterThan">
-      <formula>AT15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU30">
-    <cfRule type="expression" dxfId="3" priority="837">
-      <formula>AND(AU30&gt;0,AU30&lt;5)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="838" operator="greaterThan">
-      <formula>AT30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU36">
-    <cfRule type="expression" dxfId="3" priority="843">
-      <formula>AND(AU36&gt;0,AU36&lt;5)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="844" operator="greaterThan">
-      <formula>AT36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU37">
-    <cfRule type="cellIs" dxfId="1" priority="849" operator="greaterThan">
-      <formula>AT37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV14">
-    <cfRule type="cellIs" dxfId="4" priority="828" operator="lessThanOrEqual">
-      <formula>I14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV15">
-    <cfRule type="cellIs" dxfId="4" priority="834" operator="lessThanOrEqual">
-      <formula>I15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV30">
-    <cfRule type="cellIs" dxfId="4" priority="840" operator="lessThanOrEqual">
-      <formula>I30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV36">
-    <cfRule type="cellIs" dxfId="4" priority="846" operator="lessThanOrEqual">
-      <formula>I36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV37">
-    <cfRule type="cellIs" dxfId="4" priority="851" operator="lessThanOrEqual">
-      <formula>I37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW14">
-    <cfRule type="cellIs" dxfId="4" priority="827" operator="lessThanOrEqual">
-      <formula>J14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW15">
-    <cfRule type="cellIs" dxfId="4" priority="833" operator="lessThanOrEqual">
-      <formula>J15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW30">
+  <conditionalFormatting sqref="AW37">
     <cfRule type="cellIs" dxfId="4" priority="839" operator="lessThanOrEqual">
-      <formula>J30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW36">
-    <cfRule type="cellIs" dxfId="4" priority="845" operator="lessThanOrEqual">
-      <formula>J36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW37">
-    <cfRule type="cellIs" dxfId="4" priority="850" operator="lessThanOrEqual">
       <formula>J37</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14481,19 +14365,11 @@
       <formula>H29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z30">
+  <conditionalFormatting sqref="Z34">
     <cfRule type="cellIs" dxfId="1" priority="471" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="472" operator="lessThan">
-      <formula>H30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z34">
-    <cfRule type="cellIs" dxfId="1" priority="476" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="477" operator="lessThan">
       <formula>H34</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14617,68 +14493,66 @@
     <hyperlink ref="G30" r:id="rId109"/>
     <hyperlink ref="T30" r:id="rId110"/>
     <hyperlink ref="Y30" r:id="rId111"/>
-    <hyperlink ref="AD30" r:id="rId112"/>
-    <hyperlink ref="AI30" r:id="rId113"/>
-    <hyperlink ref="AN30" r:id="rId114"/>
-    <hyperlink ref="AX30" r:id="rId115"/>
-    <hyperlink ref="G31" r:id="rId116"/>
-    <hyperlink ref="T31" r:id="rId117"/>
-    <hyperlink ref="Y31" r:id="rId118"/>
-    <hyperlink ref="AI31" r:id="rId119"/>
-    <hyperlink ref="AN31" r:id="rId120"/>
-    <hyperlink ref="AS31" r:id="rId121"/>
-    <hyperlink ref="G32" r:id="rId122"/>
-    <hyperlink ref="T32" r:id="rId123"/>
-    <hyperlink ref="Y32" r:id="rId124"/>
-    <hyperlink ref="AI32" r:id="rId125"/>
-    <hyperlink ref="AN32" r:id="rId126"/>
-    <hyperlink ref="G33" r:id="rId127"/>
-    <hyperlink ref="T33" r:id="rId128"/>
-    <hyperlink ref="Y33" r:id="rId129"/>
-    <hyperlink ref="AI33" r:id="rId130"/>
-    <hyperlink ref="AN33" r:id="rId131"/>
-    <hyperlink ref="AS33" r:id="rId132"/>
-    <hyperlink ref="G34" r:id="rId133"/>
-    <hyperlink ref="T34" r:id="rId134"/>
-    <hyperlink ref="AD34" r:id="rId135"/>
-    <hyperlink ref="AI34" r:id="rId136"/>
-    <hyperlink ref="G35" r:id="rId137"/>
-    <hyperlink ref="T35" r:id="rId138"/>
-    <hyperlink ref="Y35" r:id="rId139"/>
-    <hyperlink ref="AI35" r:id="rId140"/>
-    <hyperlink ref="AN35" r:id="rId141"/>
-    <hyperlink ref="G36" r:id="rId142"/>
-    <hyperlink ref="T36" r:id="rId143"/>
-    <hyperlink ref="Y36" r:id="rId144"/>
-    <hyperlink ref="AI36" r:id="rId145"/>
-    <hyperlink ref="AN36" r:id="rId146"/>
-    <hyperlink ref="AS36" r:id="rId147"/>
-    <hyperlink ref="AX36" r:id="rId148"/>
-    <hyperlink ref="G37" r:id="rId149"/>
-    <hyperlink ref="T37" r:id="rId150"/>
-    <hyperlink ref="Y37" r:id="rId151"/>
-    <hyperlink ref="AI37" r:id="rId152"/>
-    <hyperlink ref="AN37" r:id="rId153"/>
-    <hyperlink ref="AS37" r:id="rId154"/>
-    <hyperlink ref="AX37" r:id="rId155"/>
-    <hyperlink ref="G38" r:id="rId156"/>
-    <hyperlink ref="G39" r:id="rId157"/>
-    <hyperlink ref="T39" r:id="rId158"/>
-    <hyperlink ref="G40" r:id="rId159"/>
-    <hyperlink ref="T40" r:id="rId160"/>
-    <hyperlink ref="Y40" r:id="rId161"/>
-    <hyperlink ref="AI40" r:id="rId162"/>
-    <hyperlink ref="AN40" r:id="rId163"/>
-    <hyperlink ref="K42" r:id="rId164"/>
-    <hyperlink ref="P42" r:id="rId165"/>
-    <hyperlink ref="U42" r:id="rId166"/>
-    <hyperlink ref="Z42" r:id="rId167"/>
-    <hyperlink ref="AE42" r:id="rId168"/>
-    <hyperlink ref="AJ42" r:id="rId169"/>
-    <hyperlink ref="AO42" r:id="rId170"/>
-    <hyperlink ref="AT42" r:id="rId171"/>
+    <hyperlink ref="AI30" r:id="rId112"/>
+    <hyperlink ref="AN30" r:id="rId113"/>
+    <hyperlink ref="G31" r:id="rId114"/>
+    <hyperlink ref="T31" r:id="rId115"/>
+    <hyperlink ref="Y31" r:id="rId116"/>
+    <hyperlink ref="AI31" r:id="rId117"/>
+    <hyperlink ref="AN31" r:id="rId118"/>
+    <hyperlink ref="AS31" r:id="rId119"/>
+    <hyperlink ref="G32" r:id="rId120"/>
+    <hyperlink ref="T32" r:id="rId121"/>
+    <hyperlink ref="Y32" r:id="rId122"/>
+    <hyperlink ref="AI32" r:id="rId123"/>
+    <hyperlink ref="AN32" r:id="rId124"/>
+    <hyperlink ref="G33" r:id="rId125"/>
+    <hyperlink ref="T33" r:id="rId126"/>
+    <hyperlink ref="Y33" r:id="rId127"/>
+    <hyperlink ref="AI33" r:id="rId128"/>
+    <hyperlink ref="AN33" r:id="rId129"/>
+    <hyperlink ref="AS33" r:id="rId130"/>
+    <hyperlink ref="G34" r:id="rId131"/>
+    <hyperlink ref="T34" r:id="rId132"/>
+    <hyperlink ref="AD34" r:id="rId133"/>
+    <hyperlink ref="AI34" r:id="rId134"/>
+    <hyperlink ref="G35" r:id="rId135"/>
+    <hyperlink ref="T35" r:id="rId136"/>
+    <hyperlink ref="Y35" r:id="rId137"/>
+    <hyperlink ref="AI35" r:id="rId138"/>
+    <hyperlink ref="AN35" r:id="rId139"/>
+    <hyperlink ref="G36" r:id="rId140"/>
+    <hyperlink ref="T36" r:id="rId141"/>
+    <hyperlink ref="Y36" r:id="rId142"/>
+    <hyperlink ref="AI36" r:id="rId143"/>
+    <hyperlink ref="AN36" r:id="rId144"/>
+    <hyperlink ref="AS36" r:id="rId145"/>
+    <hyperlink ref="AX36" r:id="rId146"/>
+    <hyperlink ref="G37" r:id="rId147"/>
+    <hyperlink ref="T37" r:id="rId148"/>
+    <hyperlink ref="Y37" r:id="rId149"/>
+    <hyperlink ref="AI37" r:id="rId150"/>
+    <hyperlink ref="AN37" r:id="rId151"/>
+    <hyperlink ref="AS37" r:id="rId152"/>
+    <hyperlink ref="AX37" r:id="rId153"/>
+    <hyperlink ref="G38" r:id="rId154"/>
+    <hyperlink ref="G39" r:id="rId155"/>
+    <hyperlink ref="T39" r:id="rId156"/>
+    <hyperlink ref="G40" r:id="rId157"/>
+    <hyperlink ref="T40" r:id="rId158"/>
+    <hyperlink ref="Y40" r:id="rId159"/>
+    <hyperlink ref="AI40" r:id="rId160"/>
+    <hyperlink ref="AN40" r:id="rId161"/>
+    <hyperlink ref="K42" r:id="rId162"/>
+    <hyperlink ref="P42" r:id="rId163"/>
+    <hyperlink ref="U42" r:id="rId164"/>
+    <hyperlink ref="Z42" r:id="rId165"/>
+    <hyperlink ref="AE42" r:id="rId166"/>
+    <hyperlink ref="AJ42" r:id="rId167"/>
+    <hyperlink ref="AO42" r:id="rId168"/>
+    <hyperlink ref="AT42" r:id="rId169"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId172"/>
+  <legacyDrawing r:id="rId170"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Board support for CBT, CBTD, and CB3T bus switches
</commit_message>
<xml_diff>
--- a/documentation/reDIP-SID-BOM.xlsx
+++ b/documentation/reDIP-SID-BOM.xlsx
@@ -1239,12 +1239,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.29      $0.29
-    10   $0.13      $1.32
-    25   $0.13      $3.15
-    50   $0.12      $5.95
-   100   $0.11     $11.30
- 15000   $0.06    $930.00</t>
+     1   $0.05      $0.05
+    10   $0.12      $1.19
+    25   $0.11      $2.77
+    50   $0.10      $5.10
+   100   $0.09      $9.40
+ 15000   $0.05    $780.00</t>
         </r>
       </text>
     </comment>
@@ -1263,15 +1263,15 @@
      1   $0.37      $0.37
     10   $0.22      $2.17
     25   $0.21      $5.37
-   100   $0.18     $17.77
-   250   $0.17     $43.60
-   500   $0.16     $81.55
-  1000   $0.10     $98.80
-  3000   $0.10    $293.40
-  6000   $0.09    $561.60
- 15000   $0.09  $1,390.50
- 30000   $0.09  $2,661.00
- 75000   $0.08  $6,165.00</t>
+   100   $0.18     $18.27
+   250   $0.17     $42.92
+   500   $0.16     $80.55
+  1000   $0.10     $96.40
+  3000   $0.10    $286.20
+  6000   $0.09    $552.00
+ 15000   $0.09  $1,365.00
+ 30000   $0.09  $2,649.00
+ 75000   $0.08  $6,127.50</t>
         </r>
       </text>
     </comment>
@@ -1337,12 +1337,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     5   $0.12      $0.61
-    50   $0.10      $5.04
-   150   $0.09     $12.79
-   500   $0.06     $29.05
-  2500   $0.06    $141.00
-  5000   $0.06    $277.50</t>
+     5   $0.12      $0.59
+    50   $0.10      $4.91
+   150   $0.08     $12.46
+   500   $0.06     $28.30
+  2500   $0.05    $137.25
+  5000   $0.05    $270.50</t>
         </r>
       </text>
     </comment>
@@ -1392,13 +1392,13 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.50      $0.50
-    10   $0.25      $2.47
-    25   $0.24      $5.90
-    50   $0.22     $11.20
-   100   $0.21     $21.20
- 10000   $0.11  $1,110.00
- 20000   $0.11  $2,180.00</t>
+     1   $0.09      $0.09
+    10   $0.21      $2.06
+    25   $0.20      $4.90
+    50   $0.19      $9.35
+   100   $0.18     $17.70
+ 10000   $0.09    $930.00
+ 20000   $0.09  $1,820.00</t>
         </r>
       </text>
     </comment>
@@ -1564,13 +1564,13 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.33      $0.33
-    10   $0.24      $2.41
-    25   $0.24      $5.97
-    50   $0.17      $8.50
-   100   $0.14     $14.45
-   250   $0.14     $35.77
-   500   $0.12     $58.20</t>
+     1   $0.32      $0.32
+    10   $0.24      $2.37
+    25   $0.23      $5.87
+    50   $0.17      $8.49
+   100   $0.14     $14.35
+   250   $0.14     $35.52
+   500   $0.11     $57.45</t>
         </r>
       </text>
     </comment>
@@ -1595,8 +1595,7 @@
   4000   $0.06    $249.08
   8000   $0.06    $471.28
  12000   $0.06    $670.56
- 28000   $0.05  $1,508.08
-100000   $0.04  $4,460.00</t>
+ 40000   $0.05  $2,154.40</t>
         </r>
       </text>
     </comment>
@@ -1676,11 +1675,11 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.44      $0.44
-    10   $0.31      $3.10
-    25   $0.27      $6.70
-    50   $0.23     $11.30
-   100   $0.18     $18.50</t>
+     1   $0.37      $0.37
+    10   $0.26      $2.58
+    25   $0.22      $5.58
+    50   $0.19      $9.45
+   100   $0.15     $15.40</t>
         </r>
       </text>
     </comment>
@@ -1813,6 +1812,7 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
+     1   $0.11      $0.11
     10   $0.27      $2.70
     25   $0.23      $5.85
     50   $0.20      $9.85
@@ -1857,14 +1857,14 @@
   Qty  -  Unit$  -  Ext$
 ================
      1   $0.33      $0.33
-    10   $0.28      $2.85
-    25   $0.24      $6.06
-    50   $0.23     $11.25
-   100   $0.14     $13.50
-   250   $0.11     $26.47
+    10   $0.28      $2.78
+    25   $0.24      $6.04
+    50   $0.22     $11.24
+   100   $0.13     $13.48
+   250   $0.11     $26.58
    500   $0.09     $47.25
-  1000   $0.08     $79.90
-  3000   $0.07    $220.20
+  1000   $0.08     $79.80
+  3000   $0.07    $219.90
   6000   $0.07    $406.20</t>
         </r>
       </text>
@@ -1993,10 +1993,10 @@
   Qty  -  Unit£  -  Ext£
 ================
      5   £0.15      £0.74
-    25   £0.13      £3.20
-   100   £0.08      £7.93
-   500   £0.06     £30.20
-  4000   £0.05    £181.20</t>
+    25   £0.13      £3.23
+   100   £0.08      £8.00
+   500   £0.06     £30.45
+  4000   £0.05    £182.80</t>
         </r>
       </text>
     </comment>
@@ -2102,10 +2102,10 @@
   Qty  -  Unit£  -  Ext£
 ================
      5   £0.15      £0.74
-    25   £0.11      £2.80
-   100   £0.08      £7.93
-   500   £0.06     £28.60
-  4000   £0.04    £164.80</t>
+    25   £0.11      £2.82
+   100   £0.08      £8.00
+   500   £0.06     £28.85
+  4000   £0.04    £166.00</t>
         </r>
       </text>
     </comment>
@@ -2166,9 +2166,9 @@
    160   £0.62     £99.04
    400   £0.58    £231.20
    800   £0.34    £273.60
-  4000   £0.31  £1,232.00
-  8000   £0.28  £2,264.00
- 16000   £0.28  £4,432.00</t>
+  4000   £0.31  £1,240.00
+  8000   £0.29  £2,336.00
+ 16000   £0.28  £4,544.00</t>
         </r>
       </text>
     </comment>
@@ -2205,13 +2205,13 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.81      $0.81
-    10   $0.71      $7.09
-    25   $0.67     $16.70
-    50   $0.64     $32.00
-   100   $0.61     $61.20
-   250   $0.56    $139.00
-   500   $0.50    $250.50
+     1   $0.75      $0.75
+    10   $0.68      $6.82
+    25   $0.64     $16.00
+    50   $0.61     $30.60
+   100   $0.58     $58.40
+   250   $0.53    $132.25
+   500   $0.49    $243.50
    800   $0.50    $400.80</t>
         </r>
       </text>
@@ -2884,17 +2884,15 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.12      $0.12
-    10   $0.07      $0.66
-    25   $0.05      $1.32
-    50   $0.04      $2.00
-   100   $0.03      $2.80
+     1   $0.11      $0.11
+    10   $0.06      $0.60
+    25   $0.05      $1.20
+    50   $0.04      $1.85
+   100   $0.03      $2.50
    250   $0.02      $5.50
    500   $0.02      $8.50
   1000   $0.01     $12.00
   2500   $0.01     $22.50
-  5000   $0.02     $90.00
- 10000   $0.01    $150.00
  15000   $0.01    $225.00
  20000   $0.01    $200.00</t>
         </r>
@@ -3109,21 +3107,8 @@
 ================
      1   $0.08      $0.08
     10   $0.07      $0.68
-    25   $0.05      $1.33
-   100   $0.04      $3.53</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q26" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This part is listed but is not stocked.</t>
+    25   $0.05      $1.32
+   100   $0.04      $3.50</t>
         </r>
       </text>
     </comment>
@@ -3225,11 +3210,11 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.12      $0.12
-    10   $0.07      $0.66
-    25   $0.05      $1.32
-    50   $0.04      $2.00
-   100   $0.03      $2.80
+     1   $0.13      $0.13
+    10   $0.06      $0.60
+    25   $0.07      $1.85
+    50   $0.04      $1.85
+   100   $0.03      $3.00
    250   $0.03      $6.25
    500   $0.02      $9.00
   1000   $0.01     $12.00
@@ -3377,7 +3362,7 @@
    100   $0.01      $1.15
    250   $0.01      $2.85
    500   $0.01      $5.60
-  1000   $0.01      $6.70
+  1000   $0.01      $6.80
   3000   $0.00      $8.40
  30000   $0.00     $81.00</t>
         </r>
@@ -3610,7 +3595,7 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.01      $0.01
+     1   $0.24      $0.24
     25   $0.02      $0.57
    100   $0.01      $1.00
    250   $0.01      $2.25
@@ -3618,7 +3603,7 @@
   1000   $0.01      $7.00
   2500   $0.01     $12.50
   5000   $0.00     $20.00
- 15000   $0.01    $120.00</t>
+ 15000   $0.01     $90.00</t>
         </r>
       </text>
     </comment>
@@ -3662,6 +3647,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="W30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="Y30" authorId="0">
       <text>
         <r>
@@ -3738,15 +3736,17 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.12      $0.12
-    10   $0.07      $0.66
-    25   $0.05      $1.32
-    50   $0.04      $2.00
-   100   $0.03      $2.80
-   250   $0.03      $6.25
-   500   $0.02      $9.50
-  1000   $0.02     $16.00
-  2500   $0.01     $27.50
+     1   $0.00      $0.00
+    10   $0.06      $0.60
+    25   $0.00      $0.05
+    50   $0.04      $1.85
+   100   $0.00      $0.20
+   250   $0.00      $0.50
+   500   $0.00      $1.00
+  1000   $0.00      $2.00
+  2500   $0.00      $5.00
+  5000   $0.02    $105.00
+ 10000   $0.02    $160.00
  15000   $0.02    $240.00</t>
         </r>
       </text>
@@ -3911,14 +3911,14 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-     5   £0.44      £2.19
-    10   £0.33      £3.29
-   100   £0.17     £16.50
-   500   £0.10     £47.85
-  3000   £0.07    £221.10
-  9000   £0.07    £649.80
- 24000   £0.07  £1,699.20
- 45000   £0.07  £3,118.50</t>
+     5   £0.34      £1.70
+    10   £0.25      £2.54
+   100   £0.13     £12.80
+   500   £0.06     £28.50
+  6000   £0.06    £335.40
+ 18000   £0.05    £984.60
+ 48000   £0.05  £2,572.80
+ 90000   £0.05  £4,716.00</t>
         </r>
       </text>
     </comment>
@@ -3955,13 +3955,14 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
+     1   $0.54      $0.54
      5   $0.54      $2.68
     10   $0.41      $4.09
    100   $0.26     $25.50
-  6000   $0.10    $576.00
- 18000   $0.09  $1,530.00
- 48000   $0.07  $3,312.00
- 90000   $0.06  $5,400.00</t>
+  6000   $0.09    $522.00
+ 18000   $0.08  $1,386.00
+ 48000   $0.06  $3,024.00
+ 90000   $0.06  $4,950.00</t>
         </r>
       </text>
     </comment>
@@ -3990,11 +3991,11 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-     5   £0.14      £0.68
-    25   £0.09      £2.16
-   100   £0.07      £7.50
-   500   £0.07     £32.70
-  3000   £0.06    £183.00</t>
+     5   £0.13      £0.67
+    25   £0.09      £2.15
+   100   £0.07      £7.46
+   500   £0.07     £32.55
+  3000   £0.06    £182.10</t>
         </r>
       </text>
     </comment>
@@ -4023,14 +4024,14 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.47      $0.47
-    10   $0.40      $4.02
-    25   $0.38      $9.39
-   100   $0.30     $30.04
-   250   $0.28     $69.73
-   500   $0.24    $118.00
-  1000   $0.18    $182.36
-  3000   $0.18    $531.30</t>
+     1   $0.61      $0.61
+    10   $0.53      $5.25
+    25   $0.49     $12.25
+   100   $0.39     $39.21
+   250   $0.36     $91.02
+   500   $0.31    $154.03
+  1000   $0.24    $238.04
+  3000   $0.23    $693.51</t>
         </r>
       </text>
     </comment>
@@ -4059,10 +4060,10 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-     5   £0.55      £2.77
-    10   £0.46      £4.64
-   100   £0.29     £28.60
-   500   £0.19     £94.50</t>
+     5   £0.48      £2.40
+    10   £0.38      £3.82
+   100   £0.28     £28.30
+   500   £0.19     £93.00</t>
         </r>
       </text>
     </comment>
@@ -4091,12 +4092,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.47      $0.47
-    10   $0.38      $3.76
-    50   $0.38     $18.80
-   100   $0.28     $27.90
-  1000   $0.18    $183.00
- 10000   $0.17  $1,660.00</t>
+     1   $0.62      $0.62
+    10   $0.53      $5.26
+    50   $0.53     $26.30
+   100   $0.36     $36.50
+  1000   $0.24    $239.00
+ 10000   $0.20  $2,040.00</t>
         </r>
       </text>
     </comment>
@@ -4412,18 +4413,18 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.26      $0.26
-    10   $0.24      $2.42
-    25   $0.23      $5.76
-    50   $0.22     $11.15
-   100   $0.22     $21.56
-   250   $0.20     $51.11
-   500   $0.17     $85.49
-  1000   $0.13    $132.69
-  4000   $0.13    $505.48
-  8000   $0.12    $951.52
- 12000   $0.11  $1,338.00
- 28000   $0.10  $2,913.96</t>
+     1   $0.47      $0.47
+    10   $0.43      $4.32
+    25   $0.41     $10.31
+    50   $0.40     $19.95
+   100   $0.39     $38.57
+   250   $0.37     $91.45
+   500   $0.31    $152.97
+  1000   $0.24    $237.44
+  4000   $0.23    $904.52
+  8000   $0.21  $1,702.64
+ 12000   $0.20  $2,394.36
+ 28000   $0.19  $5,214.16</t>
         </r>
       </text>
     </comment>
@@ -4452,9 +4453,9 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-     5   £0.53      £2.66
-    10   £0.42      £4.24
-   100   £0.26     £25.80
+     5   £0.46      £2.30
+    10   £0.38      £3.75
+   100   £0.26     £25.50
    500   £0.14     £72.00</t>
         </r>
       </text>
@@ -4484,12 +4485,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.45      $0.45
-    10   $0.37      $3.67
-    50   $0.37     $18.35
-   100   $0.25     $25.00
-  1000   $0.14    $141.00
- 10000   $0.12  $1,200.00</t>
+     1   $0.61      $0.61
+    10   $0.52      $5.24
+    50   $0.52     $26.20
+   100   $0.39     $39.10
+  1000   $0.24    $238.00
+ 10000   $0.20  $2,040.00</t>
         </r>
       </text>
     </comment>
@@ -4505,9 +4506,9 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.27      $0.27
-    10   $0.26      $2.55
-   100   $0.23     $22.90
+     1   $0.26      $0.26
+    10   $0.25      $2.48
+   100   $0.22     $22.30
   3000   $0.13    $393.00
   4000   $0.13    $524.00
   6000   $0.12    $702.00
@@ -4578,11 +4579,11 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-     5   £0.17      £0.86
-    25   £0.15      £3.74
-   100   £0.13     £12.96
-   500   £0.11     £56.59
-  2000   £0.11    £211.28</t>
+     5   £0.17      £0.85
+    25   £0.15      £3.73
+   100   £0.13     £12.92
+   500   £0.11     £56.42
+  2000   £0.11    £210.64</t>
         </r>
       </text>
     </comment>
@@ -4618,19 +4619,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="W38" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This part is listed but is not stocked.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="Y38" authorId="0">
       <text>
         <r>
@@ -4643,9 +4631,9 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-     1   £0.80      £0.80
-    25   £0.67     £16.85
-   100   £0.62     £62.00</t>
+     1   £0.85      £0.85
+    25   £0.72     £17.90
+   100   £0.66     £65.80</t>
         </r>
       </text>
     </comment>
@@ -4775,8 +4763,8 @@
   Qty  -  Unit£  -  Ext£
 ================
      1   £0.76      £0.76
-     5   £0.70      £3.50
-    25   £0.64     £16.00
+     5   £0.71      £3.55
+    25   £0.65     £16.25
    100   £0.58     £58.00</t>
         </r>
       </text>
@@ -4850,19 +4838,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q41" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This part is listed but is not stocked.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="S41" authorId="0">
       <text>
         <r>
@@ -4878,7 +4853,7 @@
      1   $9.15      $9.15
     25   $7.95    $198.75
    100   $7.67    $767.00
-  2000   $6.95 $13,900.04</t>
+  2000   $7.67 $15,340.00</t>
         </r>
       </text>
     </comment>
@@ -4907,11 +4882,11 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-     1   £5.87      £5.87
-    10   £5.27     £52.70
-    25   £4.66    £116.50
-    50   £4.57    £228.50
-   100   £4.57    £457.00</t>
+     1   £5.67      £5.67
+    10   £5.33     £53.30
+    25   £4.98    £124.50
+    50   £4.88    £244.00
+   100   £4.88    £488.00</t>
         </r>
       </text>
     </comment>
@@ -5077,11 +5052,11 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $1.18      $1.18
-    10   $1.18     $11.80
-    25   $1.18     $29.50
-    50   $1.18     $59.00
-   100   $1.18    $118.00
+     1   $1.15      $1.15
+    10   $1.15     $11.50
+    25   $1.15     $28.75
+    50   $1.15     $57.50
+   100   $1.15    $115.00
   1000   $1.34  $1,340.00
   2000   $1.28  $2,560.00
   3000   $1.28  $3,840.00
@@ -5277,7 +5252,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="360">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -5521,7 +5496,7 @@
     <t>ERJ1GNF1001C</t>
   </si>
   <si>
-    <t>R2</t>
+    <t>R3</t>
   </si>
   <si>
     <t>6.2k</t>
@@ -5533,7 +5508,7 @@
     <t>ERJ1GNF6201C</t>
   </si>
   <si>
-    <t>R3,R4,R15,R16</t>
+    <t>R4,R5,R16,R17</t>
   </si>
   <si>
     <t>2.2k</t>
@@ -5545,7 +5520,7 @@
     <t>ERJ1GNJ222C</t>
   </si>
   <si>
-    <t>R5</t>
+    <t>R6</t>
   </si>
   <si>
     <t>1.5k</t>
@@ -5557,7 +5532,7 @@
     <t>ERJ1GNJ152C</t>
   </si>
   <si>
-    <t>R6</t>
+    <t>R7</t>
   </si>
   <si>
     <t>100k</t>
@@ -5569,7 +5544,7 @@
     <t>ERJ1GNF1003C</t>
   </si>
   <si>
-    <t>R7-R9</t>
+    <t>R8-R10</t>
   </si>
   <si>
     <t>20k</t>
@@ -5581,7 +5556,7 @@
     <t>ERJ1GNF2002C</t>
   </si>
   <si>
-    <t>R10,R14,R17,R18</t>
+    <t>R11,R15,R18,R19</t>
   </si>
   <si>
     <t>10k</t>
@@ -5593,7 +5568,7 @@
     <t>ERJ1GNF1002C</t>
   </si>
   <si>
-    <t>R11,R12</t>
+    <t>R12,R13</t>
   </si>
   <si>
     <t>5.1k</t>
@@ -5605,7 +5580,7 @@
     <t>ERJ1GNJ512C</t>
   </si>
   <si>
-    <t>R13</t>
+    <t>R14</t>
   </si>
   <si>
     <t>100</t>
@@ -5617,7 +5592,7 @@
     <t>ERJ1GNJ101C</t>
   </si>
   <si>
-    <t>R19,R20</t>
+    <t>R20,R21</t>
   </si>
   <si>
     <t>0</t>
@@ -5629,7 +5604,7 @@
     <t>ERJ1GN0R00C</t>
   </si>
   <si>
-    <t>R21</t>
+    <t>R22</t>
   </si>
   <si>
     <t>22</t>
@@ -6220,7 +6195,7 @@
     <t>36AJ9148</t>
   </si>
   <si>
-    <t>85Y7484</t>
+    <t>05X8796</t>
   </si>
   <si>
     <t>51W5889</t>
@@ -6232,7 +6207,7 @@
     <t>51W5934</t>
   </si>
   <si>
-    <t>85Y7497</t>
+    <t>05X8814</t>
   </si>
   <si>
     <t>39AH6819</t>
@@ -6340,7 +6315,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>fr. 08. april 2022 kl. 12.00 +0200</t>
+    <t>fr. 15. april 2022 kl. 11.06 +0200</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -6355,7 +6330,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2022-04-08 12:00:56</t>
+    <t>2022-04-15 11:07:06</t>
   </si>
   <si>
     <t>KiCost® v1.1.6</t>
@@ -7037,7 +7012,7 @@
       </c>
       <c r="J2" s="4">
         <f>TotalCost/BoardQty</f>
-        <v>18.8149</v>
+        <v>19.2805</v>
       </c>
     </row>
     <row r="3" spans="1:58">
@@ -7052,11 +7027,11 @@
       </c>
       <c r="J3" s="5">
         <f>SUM(J7:J42)</f>
-        <v>1881.4907</v>
+        <v>1928.0548</v>
       </c>
       <c r="O3" s="5">
         <f>SUM(O7:O42)</f>
-        <v>299.46</v>
+        <v>298.42</v>
       </c>
       <c r="P3" s="6" t="str">
         <f>(COUNTA(O7:O42)&amp;" of "&amp;ROWS(O7:O42)&amp;" parts found")</f>
@@ -7064,7 +7039,7 @@
       </c>
       <c r="U3" s="5">
         <f>SUM(U7:U42)</f>
-        <v>2171.164</v>
+        <v>2197.344</v>
       </c>
       <c r="V3" s="6" t="str">
         <f>(COUNTA(U7:U42)&amp;" of "&amp;ROWS(U7:U42)&amp;" parts found")</f>
@@ -7072,7 +7047,7 @@
       </c>
       <c r="AA3" s="5">
         <f>SUM(AA7:AA42)</f>
-        <v>1757.6788</v>
+        <v>1798.1738</v>
       </c>
       <c r="AB3" s="6" t="str">
         <f>(COUNTA(AA7:AA42)&amp;" of "&amp;ROWS(AA7:AA42)&amp;" parts found")</f>
@@ -7080,7 +7055,7 @@
       </c>
       <c r="AG3" s="5">
         <f>SUM(AG7:AG42)</f>
-        <v>82.15</v>
+        <v>81.49</v>
       </c>
       <c r="AH3" s="6" t="str">
         <f>(COUNTA(AG7:AG42)&amp;" of "&amp;ROWS(AG7:AG42)&amp;" parts found")</f>
@@ -7088,7 +7063,7 @@
       </c>
       <c r="AM3" s="5">
         <f>SUM(AM7:AM42)</f>
-        <v>2090.6</v>
+        <v>2113.3</v>
       </c>
       <c r="AN3" s="6" t="str">
         <f>(COUNTA(AM7:AM42)&amp;" of "&amp;ROWS(AM7:AM42)&amp;" parts found")</f>
@@ -7096,7 +7071,7 @@
       </c>
       <c r="AS3" s="5">
         <f>SUM(AS7:AS42)</f>
-        <v>1776.1</v>
+        <v>1747.5</v>
       </c>
       <c r="AT3" s="6" t="str">
         <f>(COUNTA(AS7:AS42)&amp;" of "&amp;ROWS(AS7:AS42)&amp;" parts found")</f>
@@ -7104,7 +7079,7 @@
       </c>
       <c r="AY3" s="5">
         <f>SUM(AY7:AY42)</f>
-        <v>364.1719</v>
+        <v>365.2766</v>
       </c>
       <c r="AZ3" s="6" t="str">
         <f>(COUNTA(AY7:AY42)&amp;" of "&amp;ROWS(AY7:AY42)&amp;" parts found")</f>
@@ -7112,7 +7087,7 @@
       </c>
       <c r="BE3" s="5">
         <f>SUM(BE7:BE42)</f>
-        <v>133.1896</v>
+        <v>133.6199</v>
       </c>
       <c r="BF3" s="6" t="str">
         <f>(COUNTA(BE7:BE42)&amp;" of "&amp;ROWS(BE7:BE42)&amp;" parts found")</f>
@@ -7457,14 +7432,14 @@
       <c r="X7" s="17"/>
       <c r="Y7" s="18">
         <f>IFERROR(IF(OR(X7&gt;=Z7,H7&gt;=Z7),USD_GBP*LOOKUP(IF(X7="",H7,X7),{0,1,10,100,500,2500,5000,10000,50000},{0.0,0.088,0.088,0.075,0.046,0.043,0.04,0.034,0.0333}),"MOQ="&amp;Z7),"")</f>
-        <v>0.09810665068903535</v>
+        <v>0.09840425531914895</v>
       </c>
       <c r="Z7" s="17">
         <v>10</v>
       </c>
       <c r="AA7" s="19">
         <f>IFERROR(IF(X7="",H7,X7)*Y7,"")</f>
-        <v>39.2427</v>
+        <v>39.3617</v>
       </c>
       <c r="AB7" s="17" t="s">
         <v>224</v>
@@ -7577,7 +7552,7 @@
         <v>22</v>
       </c>
       <c r="Q8" s="17">
-        <v>1214472</v>
+        <v>1147032</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="18">
@@ -7600,20 +7575,20 @@
       <c r="X8" s="17"/>
       <c r="Y8" s="18">
         <f>IFERROR(IF(OR(X8&gt;=Z8,H8&gt;=Z8),USD_GBP*LOOKUP(IF(X8="",H8,X8),{0,1,10,100,500,2500,7500,15000,75000},{0.0,0.0857,0.0857,0.0735,0.0459,0.0408,0.0398,0.039,0.0382}),"MOQ="&amp;Z8),"")</f>
-        <v>0.09614451767525463</v>
+        <v>0.09643617021276597</v>
       </c>
       <c r="Z8" s="17">
         <v>10</v>
       </c>
       <c r="AA8" s="19">
         <f>IFERROR(IF(X8="",H8,X8)*Y8,"")</f>
-        <v>28.8434</v>
+        <v>28.9309</v>
       </c>
       <c r="AB8" s="17" t="s">
         <v>225</v>
       </c>
       <c r="AC8" s="17">
-        <v>19250</v>
+        <v>10250</v>
       </c>
       <c r="AD8" s="17"/>
       <c r="AE8" s="18">
@@ -7631,7 +7606,7 @@
         <v>254</v>
       </c>
       <c r="AI8" s="17">
-        <v>1198227</v>
+        <v>1197677</v>
       </c>
       <c r="AJ8" s="17"/>
       <c r="AK8" s="18">
@@ -7653,15 +7628,15 @@
       </c>
       <c r="AP8" s="17"/>
       <c r="AQ8" s="18">
-        <f>IFERROR(IF(OR(AP8&gt;=AR8,H8&gt;=AR8),LOOKUP(IF(AP8="",H8,AP8),{0,1,10,25,50,100,15000},{0.0,0.288,0.132,0.126,0.119,0.113,0.062}),"MOQ="&amp;AR8),"")</f>
-        <v>0.113</v>
+        <f>IFERROR(IF(OR(AP8&gt;=AR8,H8&gt;=AR8),LOOKUP(IF(AP8="",H8,AP8),{0,1,10,25,50,100,15000},{0.0,0.052,0.119,0.111,0.102,0.094,0.052}),"MOQ="&amp;AR8),"")</f>
+        <v>0.094</v>
       </c>
       <c r="AR8" s="17">
         <v>1</v>
       </c>
       <c r="AS8" s="19">
         <f>IFERROR(IF(AP8="",H8,AP8)*AQ8,"")</f>
-        <v>33.9</v>
+        <v>28.2</v>
       </c>
       <c r="AT8" s="17" t="s">
         <v>299</v>
@@ -7695,32 +7670,32 @@
       </c>
       <c r="I9" s="18">
         <f>IF(MIN(M9,S9,Y9,AE9,AK9,AQ9,AW9,BC9)&lt;&gt;0,MIN(M9,S9,Y9,AE9,AK9,AQ9,AW9,BC9),"")</f>
-        <v>0.0853</v>
+        <v>0.0831</v>
       </c>
       <c r="J9" s="19">
         <f>IF(AND(ISNUMBER(H9),ISNUMBER(I9)),H9*I9,"")</f>
-        <v>25.59</v>
+        <v>24.93</v>
       </c>
       <c r="K9" s="17">
-        <v>90074</v>
+        <v>89814</v>
       </c>
       <c r="L9" s="17"/>
       <c r="M9" s="18">
-        <f>IFERROR(IF(OR(L9&gt;=N9,H9&gt;=N9),LOOKUP(IF(L9="",H9,L9),{0,1,10,25,100,250,500,1000,3000,6000,15000,30000,75000},{0.0,0.3745,0.2169,0.2147,0.1777,0.1744,0.1631,0.0988,0.0978,0.0936,0.0927,0.0887,0.0822}),"MOQ="&amp;N9),"")</f>
-        <v>0.1744</v>
+        <f>IFERROR(IF(OR(L9&gt;=N9,H9&gt;=N9),LOOKUP(IF(L9="",H9,L9),{0,1,10,25,100,250,500,1000,3000,6000,15000,30000,75000},{0.0,0.368,0.2167,0.2146,0.1827,0.1717,0.1611,0.0964,0.0954,0.092,0.091,0.0883,0.0817}),"MOQ="&amp;N9),"")</f>
+        <v>0.1717</v>
       </c>
       <c r="N9" s="17">
         <v>1</v>
       </c>
       <c r="O9" s="19">
         <f>IFERROR(IF(L9="",H9,L9)*M9,"")</f>
-        <v>52.32</v>
+        <v>51.51</v>
       </c>
       <c r="P9" s="17" t="s">
         <v>26</v>
       </c>
       <c r="Q9" s="17">
-        <v>1639292</v>
+        <v>1314071</v>
       </c>
       <c r="R9" s="17"/>
       <c r="S9" s="18">
@@ -7743,38 +7718,38 @@
       <c r="X9" s="17"/>
       <c r="Y9" s="18">
         <f>IFERROR(IF(OR(X9&gt;=Z9,H9&gt;=Z9),USD_GBP*LOOKUP(IF(X9="",H9,X9),{0,1,10,100,500,2500,5000,10000,50000},{0.0,0.158,0.158,0.136,0.086,0.082,0.077,0.0836,0.0716}),"MOQ="&amp;Z9),"")</f>
-        <v>0.17790005991611743</v>
+        <v>0.1784397163120568</v>
       </c>
       <c r="Z9" s="17">
         <v>10</v>
       </c>
       <c r="AA9" s="19">
         <f>IFERROR(IF(X9="",H9,X9)*Y9,"")</f>
-        <v>53.37</v>
+        <v>53.5319</v>
       </c>
       <c r="AB9" s="17" t="s">
         <v>226</v>
       </c>
       <c r="AC9" s="17">
-        <v>29450</v>
+        <v>57620</v>
       </c>
       <c r="AD9" s="17"/>
       <c r="AE9" s="18">
-        <f>IFERROR(IF(OR(AD9&gt;=AF9,H9&gt;=AF9),LOOKUP(IF(AD9="",H9,AD9),{0,1,5,50,150,500,2500,5000},{0.0,0.122,0.122,0.1007,0.0853,0.0581,0.0564,0.0555}),"MOQ="&amp;AF9),"")</f>
-        <v>0.0853</v>
+        <f>IFERROR(IF(OR(AD9&gt;=AF9,H9&gt;=AF9),LOOKUP(IF(AD9="",H9,AD9),{0,1,5,50,150,500,2500,5000},{0.0,0.1189,0.1189,0.0981,0.0831,0.0566,0.0549,0.0541}),"MOQ="&amp;AF9),"")</f>
+        <v>0.0831</v>
       </c>
       <c r="AF9" s="17">
         <v>5</v>
       </c>
       <c r="AG9" s="19">
         <f>IFERROR(IF(AD9="",H9,AD9)*AE9,"")</f>
-        <v>25.59</v>
+        <v>24.93</v>
       </c>
       <c r="AH9" s="17" t="s">
         <v>255</v>
       </c>
       <c r="AI9" s="17">
-        <v>612544</v>
+        <v>644771</v>
       </c>
       <c r="AJ9" s="17"/>
       <c r="AK9" s="18">
@@ -7796,15 +7771,15 @@
       </c>
       <c r="AP9" s="17"/>
       <c r="AQ9" s="18">
-        <f>IFERROR(IF(OR(AP9&gt;=AR9,H9&gt;=AR9),LOOKUP(IF(AP9="",H9,AP9),{0,1,10,25,50,100,10000,20000},{0.0,0.504,0.247,0.236,0.224,0.212,0.111,0.109}),"MOQ="&amp;AR9),"")</f>
-        <v>0.212</v>
+        <f>IFERROR(IF(OR(AP9&gt;=AR9,H9&gt;=AR9),LOOKUP(IF(AP9="",H9,AP9),{0,1,10,25,50,100,10000,20000},{0.0,0.094,0.206,0.196,0.187,0.177,0.093,0.091}),"MOQ="&amp;AR9),"")</f>
+        <v>0.177</v>
       </c>
       <c r="AR9" s="17">
         <v>1</v>
       </c>
       <c r="AS9" s="19">
         <f>IFERROR(IF(AP9="",H9,AP9)*AQ9,"")</f>
-        <v>63.6</v>
+        <v>53.1</v>
       </c>
       <c r="AT9" s="17" t="s">
         <v>300</v>
@@ -7886,14 +7861,14 @@
       <c r="X10" s="17"/>
       <c r="Y10" s="18">
         <f>IFERROR(IF(OR(X10&gt;=Z10,H10&gt;=Z10),USD_GBP*LOOKUP(IF(X10="",H10,X10),{0,1,10,100,500,2500,7500,15000,75000},{0.0,0.0271,0.0271,0.0114,0.0073,0.0052,0.0051,0.0054,0.0047}),"MOQ="&amp;Z10),"")</f>
-        <v>0.009549047333732774</v>
+        <v>0.009578014184397165</v>
       </c>
       <c r="Z10" s="17">
         <v>10</v>
       </c>
       <c r="AA10" s="19">
         <f>IFERROR(IF(X10="",H10,X10)*Y10,"")</f>
-        <v>11.4589</v>
+        <v>11.4936</v>
       </c>
       <c r="AB10" s="17" t="s">
         <v>227</v>
@@ -7958,14 +7933,14 @@
       <c r="AV10" s="17"/>
       <c r="AW10" s="18">
         <f>IFERROR(IF(OR(AV10&gt;=AX10,H10&gt;=AX10),USD_GBP*LOOKUP(IF(AV10="",H10,AV10),{0,1,1000,5000,10000,15000,60000},{0.0,0.007,0.007,0.006,0.006,0.004,0.004}),"MOQ="&amp;AX10),"")</f>
-        <v>0.009156620730976632</v>
+        <v>0.00918439716312057</v>
       </c>
       <c r="AX10" s="17">
         <v>1000</v>
       </c>
       <c r="AY10" s="19">
         <f>IFERROR(IF(AV10="",H10,AV10)*AW10,"")</f>
-        <v>10.9879</v>
+        <v>11.0213</v>
       </c>
       <c r="AZ10" s="17" t="s">
         <v>327</v>
@@ -8010,15 +7985,15 @@
       </c>
       <c r="L11" s="17"/>
       <c r="M11" s="18">
-        <f>IFERROR(IF(OR(L11&gt;=N11,H11&gt;=N11),LOOKUP(IF(L11="",H11,L11),{0,1,10,25,50,100,250,500},{0.0,0.3276,0.2414,0.2389,0.17,0.1445,0.1431,0.1164}),"MOQ="&amp;N11),"")</f>
-        <v>0.1445</v>
+        <f>IFERROR(IF(OR(L11&gt;=N11,H11&gt;=N11),LOOKUP(IF(L11="",H11,L11),{0,1,10,25,50,100,250,500},{0.0,0.3216,0.2372,0.2348,0.1699,0.1435,0.1421,0.1149}),"MOQ="&amp;N11),"")</f>
+        <v>0.1435</v>
       </c>
       <c r="N11" s="17">
         <v>1</v>
       </c>
       <c r="O11" s="19">
         <f>IFERROR(IF(L11="",H11,L11)*M11,"")</f>
-        <v>14.45</v>
+        <v>14.35</v>
       </c>
       <c r="P11" s="17" t="s">
         <v>36</v>
@@ -8028,7 +8003,7 @@
       </c>
       <c r="R11" s="17"/>
       <c r="S11" s="18">
-        <f>IFERROR(IF(OR(R11&gt;=T11,H11&gt;=T11),LOOKUP(IF(R11="",H11,R11),{0,1,10,50,100,500,1000,4000,8000,12000,28000,100000},{0.0,0.29,0.202,0.1346,0.1144,0.08078,0.07069,0.06227,0.05891,0.05588,0.05386,0.0446}),"MOQ="&amp;T11),"")</f>
+        <f>IFERROR(IF(OR(R11&gt;=T11,H11&gt;=T11),LOOKUP(IF(R11="",H11,R11),{0,1,10,50,100,500,1000,4000,8000,12000,40000},{0.0,0.29,0.202,0.1346,0.1144,0.08078,0.07069,0.06227,0.05891,0.05588,0.05386}),"MOQ="&amp;T11),"")</f>
         <v>0.1144</v>
       </c>
       <c r="T11" s="17">
@@ -8047,14 +8022,14 @@
       <c r="X11" s="17"/>
       <c r="Y11" s="18">
         <f>IFERROR(IF(OR(X11&gt;=Z11,H11&gt;=Z11),USD_GBP*LOOKUP(IF(X11="",H11,X11),{0,1,10,100,500,1000,2000,4000,20000},{0.0,0.198,0.198,0.119,0.09,0.076,0.07,0.064,0.0627}),"MOQ="&amp;Z11),"")</f>
-        <v>0.15566255242660273</v>
+        <v>0.15613475177304967</v>
       </c>
       <c r="Z11" s="17">
         <v>10</v>
       </c>
       <c r="AA11" s="19">
         <f>IFERROR(IF(X11="",H11,X11)*Y11,"")</f>
-        <v>15.5663</v>
+        <v>15.6135</v>
       </c>
       <c r="AB11" s="17" t="s">
         <v>228</v>
@@ -8100,15 +8075,15 @@
       </c>
       <c r="AP11" s="17"/>
       <c r="AQ11" s="18">
-        <f>IFERROR(IF(OR(AP11&gt;=AR11,H11&gt;=AR11),LOOKUP(IF(AP11="",H11,AP11),{0,1,10,25,50,100},{0.0,0.444,0.31,0.268,0.226,0.185}),"MOQ="&amp;AR11),"")</f>
-        <v>0.185</v>
+        <f>IFERROR(IF(OR(AP11&gt;=AR11,H11&gt;=AR11),LOOKUP(IF(AP11="",H11,AP11),{0,1,10,25,50,100},{0.0,0.37,0.258,0.223,0.189,0.154}),"MOQ="&amp;AR11),"")</f>
+        <v>0.154</v>
       </c>
       <c r="AR11" s="17">
         <v>1</v>
       </c>
       <c r="AS11" s="19">
         <f>IFERROR(IF(AP11="",H11,AP11)*AQ11,"")</f>
-        <v>18.5</v>
+        <v>15.4</v>
       </c>
       <c r="AT11" s="17" t="s">
         <v>302</v>
@@ -8142,11 +8117,11 @@
       </c>
       <c r="I12" s="18">
         <f>IF(MIN(M12,S12,Y12,AE12,AK12,AQ12,AW12,BC12)&lt;&gt;0,MIN(M12,S12,Y12,AE12,AK12,AQ12,AW12,BC12),"")</f>
-        <v>0.15566255242660273</v>
+        <v>0.15613475177304967</v>
       </c>
       <c r="J12" s="19">
         <f>IF(AND(ISNUMBER(H12),ISNUMBER(I12)),H12*I12,"")</f>
-        <v>31.1325</v>
+        <v>31.227</v>
       </c>
       <c r="Q12" s="20" t="s">
         <v>197</v>
@@ -8172,14 +8147,14 @@
       <c r="X12" s="17"/>
       <c r="Y12" s="18">
         <f>IFERROR(IF(OR(X12&gt;=Z12,H12&gt;=Z12),USD_GBP*LOOKUP(IF(X12="",H12,X12),{0,1,10,100,500,1000,2000,4000,20000},{0.0,0.216,0.216,0.129,0.0969,0.0813,0.0796,0.0741,0.0614}),"MOQ="&amp;Z12),"")</f>
-        <v>0.1687434391851408</v>
+        <v>0.1692553191489362</v>
       </c>
       <c r="Z12" s="17">
         <v>10</v>
       </c>
       <c r="AA12" s="19">
         <f>IFERROR(IF(X12="",H12,X12)*Y12,"")</f>
-        <v>33.7487</v>
+        <v>33.8511</v>
       </c>
       <c r="AB12" s="17" t="s">
         <v>229</v>
@@ -8207,11 +8182,11 @@
       </c>
       <c r="AP12" s="17"/>
       <c r="AQ12" s="18">
-        <f>IFERROR(IF(OR(AP12&gt;=AR12,H12&gt;=AR12),LOOKUP(IF(AP12="",H12,AP12),{0,1,10,25,50,100,4000,8000},{0.0,0.27,0.27,0.234,0.197,0.161,0.101,0.094}),"MOQ="&amp;AR12),"")</f>
+        <f>IFERROR(IF(OR(AP12&gt;=AR12,H12&gt;=AR12),LOOKUP(IF(AP12="",H12,AP12),{0,1,10,25,50,100,4000,8000},{0.0,0.109,0.27,0.234,0.197,0.161,0.101,0.094}),"MOQ="&amp;AR12),"")</f>
         <v>0.161</v>
       </c>
       <c r="AR12" s="17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AS12" s="19">
         <f>IFERROR(IF(AP12="",H12,AP12)*AQ12,"")</f>
@@ -8226,14 +8201,14 @@
       <c r="AV12" s="17"/>
       <c r="AW12" s="18">
         <f>IFERROR(IF(OR(AV12&gt;=AX12,H12&gt;=AX12),USD_GBP*LOOKUP(IF(AV12="",H12,AV12),{0,1,20,100,500,1000,2000,4000,16000},{0.0,0.216,0.216,0.119,0.097,0.086,0.084,0.063,0.06}),"MOQ="&amp;AX12),"")</f>
-        <v>0.15566255242660273</v>
+        <v>0.15613475177304967</v>
       </c>
       <c r="AX12" s="17">
         <v>20</v>
       </c>
       <c r="AY12" s="19">
         <f>IFERROR(IF(AV12="",H12,AV12)*AW12,"")</f>
-        <v>31.1325</v>
+        <v>31.227</v>
       </c>
       <c r="AZ12" s="17" t="s">
         <v>328</v>
@@ -8264,26 +8239,26 @@
       </c>
       <c r="I13" s="18">
         <f>IF(MIN(M13,S13,Y13,AE13,AK13,AQ13,AW13,BC13)&lt;&gt;0,MIN(M13,S13,Y13,AE13,AK13,AQ13,AW13,BC13),"")</f>
-        <v>0.1037314319952067</v>
+        <v>0.10496453900709223</v>
       </c>
       <c r="J13" s="19">
         <f>IF(AND(ISNUMBER(H13),ISNUMBER(I13)),H13*I13,"")</f>
-        <v>10.3731</v>
+        <v>10.4965</v>
       </c>
       <c r="K13" s="17">
         <v>8037</v>
       </c>
       <c r="L13" s="17"/>
       <c r="M13" s="18">
-        <f>IFERROR(IF(OR(L13&gt;=N13,H13&gt;=N13),LOOKUP(IF(L13="",H13,L13),{0,1,10,25,50,100,250,500,1000,3000,6000},{0.0,0.3336,0.2848,0.2423,0.225,0.135,0.1059,0.0945,0.0799,0.0734,0.0677}),"MOQ="&amp;N13),"")</f>
-        <v>0.135</v>
+        <f>IFERROR(IF(OR(L13&gt;=N13,H13&gt;=N13),LOOKUP(IF(L13="",H13,L13),{0,1,10,25,50,100,250,500,1000,3000,6000},{0.0,0.3335,0.2784,0.2417,0.2247,0.1348,0.1063,0.0945,0.0798,0.0733,0.0677}),"MOQ="&amp;N13),"")</f>
+        <v>0.1348</v>
       </c>
       <c r="N13" s="17">
         <v>1</v>
       </c>
       <c r="O13" s="19">
         <f>IFERROR(IF(L13="",H13,L13)*M13,"")</f>
-        <v>13.5</v>
+        <v>13.48</v>
       </c>
       <c r="P13" s="17" t="s">
         <v>187</v>
@@ -8325,7 +8300,7 @@
         <v>230</v>
       </c>
       <c r="AI13" s="17">
-        <v>2404</v>
+        <v>2204</v>
       </c>
       <c r="AJ13" s="17"/>
       <c r="AK13" s="18">
@@ -8365,15 +8340,15 @@
       </c>
       <c r="BB13" s="17"/>
       <c r="BC13" s="18">
-        <f>IFERROR(IF(OR(BB13&gt;=BD13,H13&gt;=BD13),USD_GBP*LOOKUP(IF(BB13="",H13,BB13),{0,1,5,25,100,500,4000},{0.0,0.148,0.148,0.128,0.0793,0.0604,0.0453}),"MOQ="&amp;BD13),"")</f>
-        <v>0.1037314319952067</v>
+        <f>IFERROR(IF(OR(BB13&gt;=BD13,H13&gt;=BD13),USD_GBP*LOOKUP(IF(BB13="",H13,BB13),{0,1,5,25,100,500,4000},{0.0,0.148,0.148,0.1292,0.08,0.0609,0.0457}),"MOQ="&amp;BD13),"")</f>
+        <v>0.10496453900709223</v>
       </c>
       <c r="BD13" s="17">
         <v>5</v>
       </c>
       <c r="BE13" s="19">
         <f>IFERROR(IF(BB13="",H13,BB13)*BC13,"")</f>
-        <v>10.3731</v>
+        <v>10.4965</v>
       </c>
       <c r="BF13" s="17" t="s">
         <v>187</v>
@@ -8411,7 +8386,7 @@
         <v>3.9</v>
       </c>
       <c r="Q14" s="17">
-        <v>12478</v>
+        <v>12378</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="18">
@@ -8434,20 +8409,20 @@
       <c r="X14" s="17"/>
       <c r="Y14" s="18">
         <f>IFERROR(IF(OR(X14&gt;=Z14,H14&gt;=Z14),USD_GBP*LOOKUP(IF(X14="",H14,X14),{0,1,25,50,100,250,500},{0.0,0.277,0.22,0.161,0.0993,0.0942,0.0891}),"MOQ="&amp;Z14),"")</f>
-        <v>0.1298932055122828</v>
+        <v>0.1302872340425532</v>
       </c>
       <c r="Z14" s="17">
         <v>1</v>
       </c>
       <c r="AA14" s="19">
         <f>IFERROR(IF(X14="",H14,X14)*Y14,"")</f>
-        <v>12.9893</v>
+        <v>13.0287</v>
       </c>
       <c r="AB14" s="17" t="s">
         <v>231</v>
       </c>
       <c r="AI14" s="17">
-        <v>11240</v>
+        <v>10840</v>
       </c>
       <c r="AJ14" s="17"/>
       <c r="AK14" s="18">
@@ -8487,15 +8462,15 @@
       </c>
       <c r="BB14" s="17"/>
       <c r="BC14" s="18">
-        <f>IFERROR(IF(OR(BB14&gt;=BD14,H14&gt;=BD14),USD_GBP*LOOKUP(IF(BB14="",H14,BB14),{0,1,5,25,100,500,4000},{0.0,0.148,0.148,0.112,0.0793,0.0572,0.0412}),"MOQ="&amp;BD14),"")</f>
-        <v>0.1037314319952067</v>
+        <f>IFERROR(IF(OR(BB14&gt;=BD14,H14&gt;=BD14),USD_GBP*LOOKUP(IF(BB14="",H14,BB14),{0,1,5,25,100,500,4000},{0.0,0.148,0.148,0.1128,0.08,0.0577,0.0415}),"MOQ="&amp;BD14),"")</f>
+        <v>0.10496453900709223</v>
       </c>
       <c r="BD14" s="17">
         <v>5</v>
       </c>
       <c r="BE14" s="19">
         <f>IFERROR(IF(BB14="",H14,BB14)*BC14,"")</f>
-        <v>10.3731</v>
+        <v>10.4965</v>
       </c>
       <c r="BF14" s="17" t="s">
         <v>342</v>
@@ -8640,7 +8615,7 @@
         <v>56.2</v>
       </c>
       <c r="Q19" s="17">
-        <v>35835</v>
+        <v>33259</v>
       </c>
       <c r="R19" s="17"/>
       <c r="S19" s="18">
@@ -8662,21 +8637,21 @@
       </c>
       <c r="X19" s="17"/>
       <c r="Y19" s="18">
-        <f>IFERROR(IF(OR(X19&gt;=Z19,H19&gt;=Z19),USD_GBP*LOOKUP(IF(X19="",H19,X19),{0,1,20,60,160,400,800,4000,8000,16000},{0.0,0.903,0.748,0.671,0.619,0.578,0.342,0.308,0.283,0.277}),"MOQ="&amp;Z19),"")</f>
-        <v>0.8777275014979029</v>
+        <f>IFERROR(IF(OR(X19&gt;=Z19,H19&gt;=Z19),USD_GBP*LOOKUP(IF(X19="",H19,X19),{0,1,20,60,160,400,800,4000,8000,16000},{0.0,0.903,0.748,0.671,0.619,0.578,0.342,0.31,0.292,0.284}),"MOQ="&amp;Z19),"")</f>
+        <v>0.8803900709219861</v>
       </c>
       <c r="Z19" s="17">
         <v>1</v>
       </c>
       <c r="AA19" s="19">
         <f>IFERROR(IF(X19="",H19,X19)*Y19,"")</f>
-        <v>87.7728</v>
+        <v>88.039</v>
       </c>
       <c r="AB19" s="17" t="s">
         <v>232</v>
       </c>
       <c r="AI19" s="17">
-        <v>85163</v>
+        <v>81710</v>
       </c>
       <c r="AJ19" s="17"/>
       <c r="AK19" s="18">
@@ -8698,15 +8673,15 @@
       </c>
       <c r="AP19" s="17"/>
       <c r="AQ19" s="18">
-        <f>IFERROR(IF(OR(AP19&gt;=AR19,H19&gt;=AR19),LOOKUP(IF(AP19="",H19,AP19),{0,1,10,25,50,100,250,500,800},{0.0,0.807,0.709,0.668,0.64,0.612,0.556,0.501,0.501}),"MOQ="&amp;AR19),"")</f>
-        <v>0.612</v>
+        <f>IFERROR(IF(OR(AP19&gt;=AR19,H19&gt;=AR19),LOOKUP(IF(AP19="",H19,AP19),{0,1,10,25,50,100,250,500,800},{0.0,0.754,0.682,0.64,0.612,0.584,0.529,0.487,0.501}),"MOQ="&amp;AR19),"")</f>
+        <v>0.584</v>
       </c>
       <c r="AR19" s="17">
         <v>1</v>
       </c>
       <c r="AS19" s="19">
         <f>IFERROR(IF(AP19="",H19,AP19)*AQ19,"")</f>
-        <v>61.2</v>
+        <v>58.4</v>
       </c>
       <c r="AT19" s="17" t="s">
         <v>306</v>
@@ -8767,14 +8742,14 @@
       <c r="X20" s="17"/>
       <c r="Y20" s="18">
         <f>IFERROR(IF(OR(X20&gt;=Z20,H20&gt;=Z20),USD_GBP*LOOKUP(IF(X20="",H20,X20),{0,1,10,100,500,2500,7500,15000,75000},{0.0,0.0533,0.0533,0.0215,0.0102,0.0068,0.0067,0.0066,0.0065}),"MOQ="&amp;Z20),"")</f>
-        <v>0.028123906530856797</v>
+        <v>0.02820921985815603</v>
       </c>
       <c r="Z20" s="17">
         <v>10</v>
       </c>
       <c r="AA20" s="19">
         <f>IFERROR(IF(X20="",H20,X20)*Y20,"")</f>
-        <v>2.8124</v>
+        <v>2.8209</v>
       </c>
       <c r="AB20" s="17" t="s">
         <v>233</v>
@@ -8877,11 +8852,11 @@
       </c>
       <c r="I21" s="18">
         <f>IF(MIN(M21,S21,Y21,AE21,AK21,AQ21,AW21,BC21)&lt;&gt;0,MIN(M21,S21,Y21,AE21,AK21,AQ21,AW21,BC21),"")</f>
-        <v>0.018444050329538646</v>
+        <v>0.018500000000000003</v>
       </c>
       <c r="J21" s="19">
         <f>IF(AND(ISNUMBER(H21),ISNUMBER(I21)),H21*I21,"")</f>
-        <v>1.8444</v>
+        <v>1.85</v>
       </c>
       <c r="Q21" s="17">
         <v>28274</v>
@@ -8907,14 +8882,14 @@
       <c r="X21" s="17"/>
       <c r="Y21" s="18">
         <f>IFERROR(IF(OR(X21&gt;=Z21,H21&gt;=Z21),USD_GBP*LOOKUP(IF(X21="",H21,X21),{0,1,10,100,150,500,2500,7500,15000,75000},{0.0,0.0257,0.0257,0.0141,0.0141,0.0087,0.0079,0.0041,0.0068,0.0056}),"MOQ="&amp;Z21),"")</f>
-        <v>0.018444050329538646</v>
+        <v>0.018500000000000003</v>
       </c>
       <c r="Z21" s="17">
         <v>10</v>
       </c>
       <c r="AA21" s="19">
         <f>IFERROR(IF(X21="",H21,X21)*Y21,"")</f>
-        <v>1.8444</v>
+        <v>1.85</v>
       </c>
       <c r="AB21" s="17" t="s">
         <v>234</v>
@@ -9268,25 +9243,25 @@
         <v>1.33</v>
       </c>
       <c r="K24" s="17">
-        <v>285000</v>
+        <v>330000</v>
       </c>
       <c r="L24" s="17"/>
       <c r="M24" s="18">
-        <f>IFERROR(IF(OR(L24&gt;=N24,H24&gt;=N24),LOOKUP(IF(L24="",H24,L24),{0,1,10,25},{0.0,0.0803,0.0593,0.0587}),"MOQ="&amp;N24),"")</f>
-        <v>0.0587</v>
+        <f>IFERROR(IF(OR(L24&gt;=N24,H24&gt;=N24),LOOKUP(IF(L24="",H24,L24),{0,1,10,25},{0.0,0.0804,0.0594,0.0588}),"MOQ="&amp;N24),"")</f>
+        <v>0.0588</v>
       </c>
       <c r="N24" s="17">
         <v>1</v>
       </c>
       <c r="O24" s="19">
         <f>IFERROR(IF(L24="",H24,L24)*M24,"")</f>
-        <v>5.87</v>
+        <v>5.88</v>
       </c>
       <c r="P24" s="17" t="s">
         <v>95</v>
       </c>
       <c r="Q24" s="17">
-        <v>504427</v>
+        <v>240905</v>
       </c>
       <c r="R24" s="17"/>
       <c r="S24" s="18">
@@ -9304,19 +9279,19 @@
         <v>205</v>
       </c>
       <c r="W24" s="17">
-        <v>49201</v>
+        <v>47201</v>
       </c>
       <c r="X24" s="17"/>
       <c r="Y24" s="18">
         <f>IFERROR(IF(OR(X24&gt;=Z24,H24&gt;=Z24),USD_GBP*LOOKUP(IF(X24="",H24,X24),{0,1,10,100,500,2500,7500,15000,75000},{0.0,0.0533,0.0533,0.0215,0.0102,0.0068,0.0067,0.0066,0.0065}),"MOQ="&amp;Z24),"")</f>
-        <v>0.028123906530856797</v>
+        <v>0.02820921985815603</v>
       </c>
       <c r="Z24" s="17">
         <v>10</v>
       </c>
       <c r="AA24" s="19">
         <f>IFERROR(IF(X24="",H24,X24)*Y24,"")</f>
-        <v>2.8124</v>
+        <v>2.8209</v>
       </c>
       <c r="AB24" s="17" t="s">
         <v>237</v>
@@ -9340,7 +9315,7 @@
         <v>259</v>
       </c>
       <c r="AI24" s="17">
-        <v>923836</v>
+        <v>919640</v>
       </c>
       <c r="AJ24" s="17"/>
       <c r="AK24" s="18">
@@ -9362,15 +9337,15 @@
       </c>
       <c r="AP24" s="17"/>
       <c r="AQ24" s="18">
-        <f>IFERROR(IF(OR(AP24&gt;=AR24,H24&gt;=AR24),LOOKUP(IF(AP24="",H24,AP24),{0,1,10,25,50,100,250,500,1000,2500,5000,10000,15000,20000},{0.0,0.121,0.066,0.053,0.04,0.028,0.022,0.017,0.012,0.009,0.018,0.015,0.015,0.01}),"MOQ="&amp;AR24),"")</f>
-        <v>0.028</v>
+        <f>IFERROR(IF(OR(AP24&gt;=AR24,H24&gt;=AR24),LOOKUP(IF(AP24="",H24,AP24),{0,1,10,25,50,100,250,500,1000,2500,15000,20000},{0.0,0.11,0.06,0.048,0.037,0.025,0.022,0.017,0.012,0.009,0.015,0.01}),"MOQ="&amp;AR24),"")</f>
+        <v>0.025</v>
       </c>
       <c r="AR24" s="17">
         <v>1</v>
       </c>
       <c r="AS24" s="19">
         <f>IFERROR(IF(AP24="",H24,AP24)*AQ24,"")</f>
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="AT24" s="17" t="s">
         <v>311</v>
@@ -9426,7 +9401,7 @@
         <v>3.99</v>
       </c>
       <c r="K25" s="17">
-        <v>90000</v>
+        <v>45000</v>
       </c>
       <c r="L25" s="17"/>
       <c r="M25" s="18">
@@ -9467,20 +9442,20 @@
       <c r="X25" s="17"/>
       <c r="Y25" s="18">
         <f>IFERROR(IF(OR(X25&gt;=Z25,H25&gt;=Z25),USD_GBP*LOOKUP(IF(X25="",H25,X25),{0,1,10,100,150,500,2500,7500,15000,75000},{0.0,0.0257,0.0257,0.0141,0.0141,0.0087,0.0046,0.0041,0.0066,0.0055}),"MOQ="&amp;Z25),"")</f>
-        <v>0.018444050329538646</v>
+        <v>0.018500000000000003</v>
       </c>
       <c r="Z25" s="17">
         <v>10</v>
       </c>
       <c r="AA25" s="19">
         <f>IFERROR(IF(X25="",H25,X25)*Y25,"")</f>
-        <v>5.5332</v>
+        <v>5.55</v>
       </c>
       <c r="AB25" s="17" t="s">
         <v>238</v>
       </c>
       <c r="AC25" s="17">
-        <v>5750</v>
+        <v>5700</v>
       </c>
       <c r="AD25" s="17"/>
       <c r="AE25" s="18">
@@ -9566,25 +9541,25 @@
         <v>5.56</v>
       </c>
       <c r="K26" s="17">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="L26" s="17"/>
       <c r="M26" s="18">
-        <f>IFERROR(IF(OR(L26&gt;=N26,H26&gt;=N26),LOOKUP(IF(L26="",H26,L26),{0,1,10,25,100},{0.0,0.0817,0.0678,0.0533,0.0353}),"MOQ="&amp;N26),"")</f>
-        <v>0.0353</v>
+        <f>IFERROR(IF(OR(L26&gt;=N26,H26&gt;=N26),LOOKUP(IF(L26="",H26,L26),{0,1,10,25,100},{0.0,0.0816,0.0677,0.053,0.035}),"MOQ="&amp;N26),"")</f>
+        <v>0.035</v>
       </c>
       <c r="N26" s="17">
         <v>1</v>
       </c>
       <c r="O26" s="19">
         <f>IFERROR(IF(L26="",H26,L26)*M26,"")</f>
-        <v>14.12</v>
+        <v>14.0</v>
       </c>
       <c r="P26" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="Q26" s="20" t="s">
-        <v>197</v>
+      <c r="Q26" s="17">
+        <v>8076</v>
       </c>
       <c r="R26" s="17"/>
       <c r="S26" s="18">
@@ -9602,19 +9577,19 @@
         <v>207</v>
       </c>
       <c r="W26" s="17">
-        <v>405000</v>
+        <v>345000</v>
       </c>
       <c r="X26" s="17"/>
       <c r="Y26" s="18">
         <f>IFERROR(IF(OR(X26&gt;=Z26,H26&gt;=Z26),USD_GBP*LOOKUP(IF(X26="",H26,X26),{0,1,10,100,500,2500,7500,15000,75000},{0.0,0.0533,0.0533,0.0215,0.0102,0.0068,0.0067,0.0066,0.0065}),"MOQ="&amp;Z26),"")</f>
-        <v>0.028123906530856797</v>
+        <v>0.02820921985815603</v>
       </c>
       <c r="Z26" s="17">
         <v>10</v>
       </c>
       <c r="AA26" s="19">
         <f>IFERROR(IF(X26="",H26,X26)*Y26,"")</f>
-        <v>11.2496</v>
+        <v>11.2837</v>
       </c>
       <c r="AB26" s="17" t="s">
         <v>239</v>
@@ -9638,7 +9613,7 @@
         <v>261</v>
       </c>
       <c r="AI26" s="17">
-        <v>582049</v>
+        <v>536590</v>
       </c>
       <c r="AJ26" s="17"/>
       <c r="AK26" s="18">
@@ -9656,11 +9631,11 @@
         <v>281</v>
       </c>
       <c r="AO26" s="17">
-        <v>360000</v>
+        <v>345000</v>
       </c>
       <c r="AP26" s="17"/>
       <c r="AQ26" s="18">
-        <f>IFERROR(IF(OR(AP26&gt;=AR26,H26&gt;=AR26),LOOKUP(IF(AP26="",H26,AP26),{0,1,10,25,50,100,250,500,1000,2500,5000,15000,20000},{0.0,0.121,0.066,0.053,0.04,0.028,0.025,0.018,0.012,0.011,0.01,0.009,0.01}),"MOQ="&amp;AR26),"")</f>
+        <f>IFERROR(IF(OR(AP26&gt;=AR26,H26&gt;=AR26),LOOKUP(IF(AP26="",H26,AP26),{0,1,10,25,50,100,250,500,1000,2500,5000,15000,20000},{0.0,0.128,0.06,0.074,0.037,0.03,0.025,0.018,0.012,0.011,0.01,0.009,0.01}),"MOQ="&amp;AR26),"")</f>
         <v>0.025</v>
       </c>
       <c r="AR26" s="17">
@@ -9724,7 +9699,7 @@
         <v>2.6</v>
       </c>
       <c r="Q27" s="17">
-        <v>148810</v>
+        <v>148710</v>
       </c>
       <c r="R27" s="17"/>
       <c r="S27" s="18">
@@ -9760,7 +9735,7 @@
         <v>240</v>
       </c>
       <c r="AI27" s="17">
-        <v>66957</v>
+        <v>65447</v>
       </c>
       <c r="AJ27" s="17"/>
       <c r="AK27" s="18">
@@ -9832,7 +9807,7 @@
       </c>
       <c r="L28" s="17"/>
       <c r="M28" s="18">
-        <f>IFERROR(IF(OR(L28&gt;=N28,H28&gt;=N28),LOOKUP(IF(L28="",H28,L28),{0,1,10,25,100,250,500,1000,3000,30000},{0.0,0.0689,0.0266,0.0264,0.0115,0.0114,0.0112,0.0067,0.0028,0.0027}),"MOQ="&amp;N28),"")</f>
+        <f>IFERROR(IF(OR(L28&gt;=N28,H28&gt;=N28),LOOKUP(IF(L28="",H28,L28),{0,1,10,25,100,250,500,1000,3000,30000},{0.0,0.0689,0.0267,0.0265,0.0115,0.0114,0.0112,0.0068,0.0028,0.0027}),"MOQ="&amp;N28),"")</f>
         <v>0.0115</v>
       </c>
       <c r="N28" s="17">
@@ -9846,7 +9821,7 @@
         <v>111</v>
       </c>
       <c r="Q28" s="17">
-        <v>480293</v>
+        <v>479993</v>
       </c>
       <c r="R28" s="17"/>
       <c r="S28" s="18">
@@ -9900,7 +9875,7 @@
         <v>262</v>
       </c>
       <c r="AI28" s="17">
-        <v>108726</v>
+        <v>107426</v>
       </c>
       <c r="AJ28" s="17"/>
       <c r="AK28" s="18">
@@ -9986,7 +9961,7 @@
         <v>2.0</v>
       </c>
       <c r="Q29" s="17">
-        <v>6317632</v>
+        <v>6183512</v>
       </c>
       <c r="R29" s="17"/>
       <c r="S29" s="18">
@@ -10004,25 +9979,25 @@
         <v>210</v>
       </c>
       <c r="W29" s="17">
-        <v>240000</v>
+        <v>225000</v>
       </c>
       <c r="X29" s="17"/>
       <c r="Y29" s="18">
         <f>IFERROR(IF(OR(X29&gt;=Z29,H29&gt;=Z29),USD_GBP*LOOKUP(IF(X29="",H29,X29),{0,1,10,100,500,2500,7500,15000,75000},{0.0,0.0339,0.0339,0.0136,0.0113,0.0091,0.0069,0.0068,0.0056}),"MOQ="&amp;Z29),"")</f>
-        <v>0.01779000599161174</v>
+        <v>0.017843971631205675</v>
       </c>
       <c r="Z29" s="17">
         <v>10</v>
       </c>
       <c r="AA29" s="19">
         <f>IFERROR(IF(X29="",H29,X29)*Y29,"")</f>
-        <v>3.558</v>
+        <v>3.5688</v>
       </c>
       <c r="AB29" s="17" t="s">
         <v>242</v>
       </c>
       <c r="AI29" s="17">
-        <v>7284611</v>
+        <v>7249011</v>
       </c>
       <c r="AJ29" s="17"/>
       <c r="AK29" s="18">
@@ -10044,7 +10019,7 @@
       </c>
       <c r="AP29" s="17"/>
       <c r="AQ29" s="18">
-        <f>IFERROR(IF(OR(AP29&gt;=AR29,H29&gt;=AR29),LOOKUP(IF(AP29="",H29,AP29),{0,1,25,100,250,500,1000,2500,5000,15000},{0.0,0.008,0.023,0.01,0.009,0.008,0.007,0.005,0.004,0.008}),"MOQ="&amp;AR29),"")</f>
+        <f>IFERROR(IF(OR(AP29&gt;=AR29,H29&gt;=AR29),LOOKUP(IF(AP29="",H29,AP29),{0,1,25,100,250,500,1000,2500,5000,15000},{0.0,0.236,0.023,0.01,0.009,0.008,0.007,0.005,0.004,0.006}),"MOQ="&amp;AR29),"")</f>
         <v>0.01</v>
       </c>
       <c r="AR29" s="17">
@@ -10101,14 +10076,14 @@
       </c>
       <c r="I30" s="18">
         <f>IF(MIN(M30,S30,Y30,AE30,AK30,AQ30,AW30,BC30)&lt;&gt;0,MIN(M30,S30,Y30,AE30,AK30,AQ30,AW30,BC30),"")</f>
-        <v>0.0124</v>
+        <v>0.002</v>
       </c>
       <c r="J30" s="19">
         <f>IF(AND(ISNUMBER(H30),ISNUMBER(I30)),H30*I30,"")</f>
-        <v>1.24</v>
+        <v>0.2</v>
       </c>
       <c r="Q30" s="17">
-        <v>556386</v>
+        <v>553636</v>
       </c>
       <c r="R30" s="17"/>
       <c r="S30" s="18">
@@ -10125,20 +10100,20 @@
       <c r="V30" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="W30" s="17">
-        <v>104</v>
+      <c r="W30" s="20" t="s">
+        <v>197</v>
       </c>
       <c r="X30" s="17"/>
       <c r="Y30" s="18">
         <f>IFERROR(IF(OR(X30&gt;=Z30,H30&gt;=Z30),USD_GBP*LOOKUP(IF(X30="",H30,X30),{0,1,10,100,500,2500,7500,15000,75000},{0.0,0.0619,0.0619,0.025,0.0118,0.0079,0.0067,0.0066,0.0055}),"MOQ="&amp;Z30),"")</f>
-        <v>0.032702216896345115</v>
+        <v>0.03280141843971632</v>
       </c>
       <c r="Z30" s="17">
         <v>10</v>
       </c>
       <c r="AA30" s="19">
         <f>IFERROR(IF(X30="",H30,X30)*Y30,"")</f>
-        <v>3.2702</v>
+        <v>3.2801</v>
       </c>
       <c r="AB30" s="17" t="s">
         <v>243</v>
@@ -10162,7 +10137,7 @@
         <v>263</v>
       </c>
       <c r="AI30" s="17">
-        <v>267080</v>
+        <v>254080</v>
       </c>
       <c r="AJ30" s="17"/>
       <c r="AK30" s="18">
@@ -10180,19 +10155,19 @@
         <v>285</v>
       </c>
       <c r="AO30" s="17">
-        <v>41</v>
+        <v>15000</v>
       </c>
       <c r="AP30" s="17"/>
       <c r="AQ30" s="18">
-        <f>IFERROR(IF(OR(AP30&gt;=AR30,H30&gt;=AR30),LOOKUP(IF(AP30="",H30,AP30),{0,1,10,25,50,100,250,500,1000,2500,15000},{0.0,0.121,0.066,0.053,0.04,0.028,0.025,0.019,0.016,0.011,0.016}),"MOQ="&amp;AR30),"")</f>
-        <v>0.028</v>
+        <f>IFERROR(IF(OR(AP30&gt;=AR30,H30&gt;=AR30),LOOKUP(IF(AP30="",H30,AP30),{0,1,10,25,50,100,250,500,1000,2500,5000,10000,15000},{0.0,0.002,0.06,0.002,0.037,0.002,0.002,0.002,0.002,0.002,0.021,0.016,0.016}),"MOQ="&amp;AR30),"")</f>
+        <v>0.002</v>
       </c>
       <c r="AR30" s="17">
         <v>1</v>
       </c>
       <c r="AS30" s="19">
         <f>IFERROR(IF(AP30="",H30,AP30)*AQ30,"")</f>
-        <v>2.8</v>
+        <v>0.2</v>
       </c>
       <c r="AT30" s="17" t="s">
         <v>317</v>
@@ -10271,14 +10246,14 @@
       <c r="X31" s="17"/>
       <c r="Y31" s="18">
         <f>IFERROR(IF(OR(X31&gt;=Z31,H31&gt;=Z31),USD_GBP*LOOKUP(IF(X31="",H31,X31),{0,1,10,50,100,500},{0.0,0.165,0.165,0.156,0.142,0.12}),"MOQ="&amp;Z31),"")</f>
-        <v>0.18574859197124025</v>
+        <v>0.18631205673758866</v>
       </c>
       <c r="Z31" s="17">
         <v>10</v>
       </c>
       <c r="AA31" s="19">
         <f>IFERROR(IF(X31="",H31,X31)*Y31,"")</f>
-        <v>18.5749</v>
+        <v>18.6312</v>
       </c>
       <c r="AB31" s="17" t="s">
         <v>244</v>
@@ -10363,14 +10338,14 @@
       </c>
       <c r="I32" s="18">
         <f>IF(MIN(M32,S32,Y32,AE32,AK32,AQ32,AW32,BC32)&lt;&gt;0,MIN(M32,S32,Y32,AE32,AK32,AQ32,AW32,BC32),"")</f>
-        <v>0.09810665068903535</v>
+        <v>0.09787943262411349</v>
       </c>
       <c r="J32" s="19">
         <f>IF(AND(ISNUMBER(H32),ISNUMBER(I32)),H32*I32,"")</f>
-        <v>19.6213</v>
+        <v>19.5759</v>
       </c>
       <c r="Q32" s="17">
-        <v>298</v>
+        <v>188</v>
       </c>
       <c r="R32" s="17"/>
       <c r="S32" s="18">
@@ -10392,21 +10367,21 @@
       </c>
       <c r="X32" s="17"/>
       <c r="Y32" s="18">
-        <f>IFERROR(IF(OR(X32&gt;=Z32,H32&gt;=Z32),USD_GBP*LOOKUP(IF(X32="",H32,X32),{0,1,5,10,100,500,3000,9000,24000,45000},{0.0,0.439,0.439,0.329,0.165,0.0957,0.0737,0.0722,0.0708,0.0693}),"MOQ="&amp;Z32),"")</f>
-        <v>0.21583463151587778</v>
+        <f>IFERROR(IF(OR(X32&gt;=Z32,H32&gt;=Z32),USD_GBP*LOOKUP(IF(X32="",H32,X32),{0,1,5,10,100,500,6000,18000,48000,90000},{0.0,0.339,0.339,0.254,0.128,0.057,0.0559,0.0547,0.0536,0.0524}),"MOQ="&amp;Z32),"")</f>
+        <v>0.16794326241134755</v>
       </c>
       <c r="Z32" s="17">
         <v>5</v>
       </c>
       <c r="AA32" s="19">
         <f>IFERROR(IF(X32="",H32,X32)*Y32,"")</f>
-        <v>43.1669</v>
+        <v>33.5887</v>
       </c>
       <c r="AB32" s="17" t="s">
         <v>245</v>
       </c>
       <c r="AI32" s="17">
-        <v>10729</v>
+        <v>10673</v>
       </c>
       <c r="AJ32" s="17"/>
       <c r="AK32" s="18">
@@ -10428,11 +10403,11 @@
       </c>
       <c r="AP32" s="17"/>
       <c r="AQ32" s="18">
-        <f>IFERROR(IF(OR(AP32&gt;=AR32,H32&gt;=AR32),LOOKUP(IF(AP32="",H32,AP32),{0,1,5,10,100,6000,18000,48000,90000},{0.0,0.536,0.536,0.409,0.255,0.096,0.085,0.069,0.06}),"MOQ="&amp;AR32),"")</f>
+        <f>IFERROR(IF(OR(AP32&gt;=AR32,H32&gt;=AR32),LOOKUP(IF(AP32="",H32,AP32),{0,1,5,10,100,6000,18000,48000,90000},{0.0,0.536,0.536,0.409,0.255,0.087,0.077,0.063,0.055}),"MOQ="&amp;AR32),"")</f>
         <v>0.255</v>
       </c>
       <c r="AR32" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AS32" s="19">
         <f>IFERROR(IF(AP32="",H32,AP32)*AQ32,"")</f>
@@ -10446,15 +10421,15 @@
       </c>
       <c r="BB32" s="17"/>
       <c r="BC32" s="18">
-        <f>IFERROR(IF(OR(BB32&gt;=BD32,H32&gt;=BD32),USD_GBP*LOOKUP(IF(BB32="",H32,BB32),{0,1,5,25,100,500,3000},{0.0,0.136,0.136,0.0864,0.075,0.0654,0.061}),"MOQ="&amp;BD32),"")</f>
-        <v>0.09810665068903535</v>
+        <f>IFERROR(IF(OR(BB32&gt;=BD32,H32&gt;=BD32),USD_GBP*LOOKUP(IF(BB32="",H32,BB32),{0,1,5,25,100,500,3000},{0.0,0.134,0.134,0.086,0.0746,0.0651,0.0607}),"MOQ="&amp;BD32),"")</f>
+        <v>0.09787943262411349</v>
       </c>
       <c r="BD32" s="17">
         <v>5</v>
       </c>
       <c r="BE32" s="19">
         <f>IFERROR(IF(BB32="",H32,BB32)*BC32,"")</f>
-        <v>19.6213</v>
+        <v>19.5759</v>
       </c>
       <c r="BF32" s="17" t="s">
         <v>126</v>
@@ -10485,26 +10460,26 @@
       </c>
       <c r="I33" s="18">
         <f>IF(MIN(M33,S33,Y33,AE33,AK33,AQ33,AW33,BC33)&lt;&gt;0,MIN(M33,S33,Y33,AE33,AK33,AQ33,AW33,BC33),"")</f>
-        <v>0.279</v>
+        <v>0.365</v>
       </c>
       <c r="J33" s="19">
         <f>IF(AND(ISNUMBER(H33),ISNUMBER(I33)),H33*I33,"")</f>
-        <v>27.9</v>
+        <v>36.5</v>
       </c>
       <c r="Q33" s="20" t="s">
         <v>197</v>
       </c>
       <c r="R33" s="17"/>
       <c r="S33" s="18">
-        <f>IFERROR(IF(OR(R33&gt;=T33,H33&gt;=T33),LOOKUP(IF(R33="",H33,R33),{0,1,10,25,100,250,500,1000,3000},{0.0,0.47,0.402,0.3756,0.3004,0.27892,0.236,0.18236,0.1771}),"MOQ="&amp;T33),"")</f>
-        <v>0.3004</v>
+        <f>IFERROR(IF(OR(R33&gt;=T33,H33&gt;=T33),LOOKUP(IF(R33="",H33,R33),{0,1,10,25,100,250,500,1000,3000},{0.0,0.61,0.525,0.49,0.3921,0.36408,0.30806,0.23804,0.23117}),"MOQ="&amp;T33),"")</f>
+        <v>0.3921</v>
       </c>
       <c r="T33" s="17">
         <v>1</v>
       </c>
       <c r="U33" s="19">
         <f>IFERROR(IF(R33="",H33,R33)*S33,"")</f>
-        <v>30.04</v>
+        <v>39.21</v>
       </c>
       <c r="V33" s="17" t="s">
         <v>214</v>
@@ -10514,15 +10489,15 @@
       </c>
       <c r="X33" s="17"/>
       <c r="Y33" s="18">
-        <f>IFERROR(IF(OR(X33&gt;=Z33,H33&gt;=Z33),USD_GBP*LOOKUP(IF(X33="",H33,X33),{0,1,5,10,100,500},{0.0,0.554,0.554,0.464,0.286,0.189}),"MOQ="&amp;Z33),"")</f>
-        <v>0.3741133612941881</v>
+        <f>IFERROR(IF(OR(X33&gt;=Z33,H33&gt;=Z33),USD_GBP*LOOKUP(IF(X33="",H33,X33),{0,1,5,10,100,500},{0.0,0.479,0.479,0.382,0.283,0.186}),"MOQ="&amp;Z33),"")</f>
+        <v>0.37131205673758866</v>
       </c>
       <c r="Z33" s="17">
         <v>5</v>
       </c>
       <c r="AA33" s="19">
         <f>IFERROR(IF(X33="",H33,X33)*Y33,"")</f>
-        <v>37.4113</v>
+        <v>37.1312</v>
       </c>
       <c r="AB33" s="17" t="s">
         <v>246</v>
@@ -10532,15 +10507,15 @@
       </c>
       <c r="AJ33" s="17"/>
       <c r="AK33" s="18">
-        <f>IFERROR(IF(OR(AJ33&gt;=AL33,H33&gt;=AL33),LOOKUP(IF(AJ33="",H33,AJ33),{0,1,10,50,100,1000,10000},{0.0,0.47,0.376,0.376,0.279,0.183,0.166}),"MOQ="&amp;AL33),"")</f>
-        <v>0.279</v>
+        <f>IFERROR(IF(OR(AJ33&gt;=AL33,H33&gt;=AL33),LOOKUP(IF(AJ33="",H33,AJ33),{0,1,10,50,100,1000,10000},{0.0,0.62,0.526,0.526,0.365,0.239,0.204}),"MOQ="&amp;AL33),"")</f>
+        <v>0.365</v>
       </c>
       <c r="AL33" s="17">
         <v>1</v>
       </c>
       <c r="AM33" s="19">
         <f>IFERROR(IF(AJ33="",H33,AJ33)*AK33,"")</f>
-        <v>27.9</v>
+        <v>36.5</v>
       </c>
       <c r="AN33" s="17" t="s">
         <v>288</v>
@@ -10569,14 +10544,14 @@
       <c r="AV33" s="17"/>
       <c r="AW33" s="18">
         <f>IFERROR(IF(OR(AV33&gt;=AX33,H33&gt;=AX33),USD_GBP*LOOKUP(IF(AV33="",H33,AV33),{0,1,18,108,1008,3000,3006,9000},{0.0,0.314,0.314,0.161,0.121,0.146,0.099,0.147}),"MOQ="&amp;AX33),"")</f>
-        <v>0.4107398442180947</v>
+        <v>0.411985815602837</v>
       </c>
       <c r="AX33" s="17">
         <v>18</v>
       </c>
       <c r="AY33" s="19">
         <f>IFERROR(IF(AV33="",H33,AV33)*AW33,"")</f>
-        <v>41.074</v>
+        <v>41.1986</v>
       </c>
       <c r="AZ33" s="17" t="s">
         <v>337</v>
@@ -10776,14 +10751,14 @@
       <c r="X36" s="17"/>
       <c r="Y36" s="18">
         <f>IFERROR(IF(OR(X36&gt;=Z36,H36&gt;=Z36),USD_GBP*LOOKUP(IF(X36="",H36,X36),{0,1,10,25,50},{0.0,4.35,3.91,3.69,3.62}),"MOQ="&amp;Z36),"")</f>
-        <v>4.735281006590773</v>
+        <v>4.749645390070923</v>
       </c>
       <c r="Z36" s="17">
         <v>1</v>
       </c>
       <c r="AA36" s="19">
         <f>IFERROR(IF(X36="",H36,X36)*Y36,"")</f>
-        <v>473.5281</v>
+        <v>474.9645</v>
       </c>
       <c r="AB36" s="17" t="s">
         <v>247</v>
@@ -10850,26 +10825,26 @@
       </c>
       <c r="I37" s="18">
         <f>IF(MIN(M37,S37,Y37,AE37,AK37,AQ37,AW37,BC37)&lt;&gt;0,MIN(M37,S37,Y37,AE37,AK37,AQ37,AW37,BC37),"")</f>
-        <v>0.16952829239065306</v>
+        <v>0.16951773049645394</v>
       </c>
       <c r="J37" s="19">
         <f>IF(AND(ISNUMBER(H37),ISNUMBER(I37)),H37*I37,"")</f>
-        <v>16.9528</v>
+        <v>16.9518</v>
       </c>
       <c r="Q37" s="20" t="s">
         <v>197</v>
       </c>
       <c r="R37" s="17"/>
       <c r="S37" s="18">
-        <f>IFERROR(IF(OR(R37&gt;=T37,H37&gt;=T37),LOOKUP(IF(R37="",H37,R37),{0,1,10,25,50,100,250,500,1000,4000,8000,12000,28000},{0.0,0.26,0.242,0.2304,0.223,0.2156,0.20444,0.17098,0.13269,0.12637,0.11894,0.1115,0.10407}),"MOQ="&amp;T37),"")</f>
-        <v>0.2156</v>
+        <f>IFERROR(IF(OR(R37&gt;=T37,H37&gt;=T37),LOOKUP(IF(R37="",H37,R37),{0,1,10,25,50,100,250,500,1000,4000,8000,12000,28000},{0.0,0.47,0.432,0.4124,0.399,0.3857,0.3658,0.30594,0.23744,0.22613,0.21283,0.19953,0.18622}),"MOQ="&amp;T37),"")</f>
+        <v>0.3857</v>
       </c>
       <c r="T37" s="17">
         <v>1</v>
       </c>
       <c r="U37" s="19">
         <f>IFERROR(IF(R37="",H37,R37)*S37,"")</f>
-        <v>21.56</v>
+        <v>38.57</v>
       </c>
       <c r="V37" s="17" t="s">
         <v>218</v>
@@ -10879,15 +10854,15 @@
       </c>
       <c r="X37" s="17"/>
       <c r="Y37" s="18">
-        <f>IFERROR(IF(OR(X37&gt;=Z37,H37&gt;=Z37),USD_GBP*LOOKUP(IF(X37="",H37,X37),{0,1,5,10,100,500},{0.0,0.531,0.531,0.424,0.258,0.144}),"MOQ="&amp;Z37),"")</f>
-        <v>0.3374868783702816</v>
+        <f>IFERROR(IF(OR(X37&gt;=Z37,H37&gt;=Z37),USD_GBP*LOOKUP(IF(X37="",H37,X37),{0,1,5,10,100,500},{0.0,0.46,0.46,0.375,0.255,0.144}),"MOQ="&amp;Z37),"")</f>
+        <v>0.33457446808510644</v>
       </c>
       <c r="Z37" s="17">
         <v>5</v>
       </c>
       <c r="AA37" s="19">
         <f>IFERROR(IF(X37="",H37,X37)*Y37,"")</f>
-        <v>33.7487</v>
+        <v>33.4574</v>
       </c>
       <c r="AB37" s="17" t="s">
         <v>248</v>
@@ -10897,15 +10872,15 @@
       </c>
       <c r="AJ37" s="17"/>
       <c r="AK37" s="18">
-        <f>IFERROR(IF(OR(AJ37&gt;=AL37,H37&gt;=AL37),LOOKUP(IF(AJ37="",H37,AJ37),{0,1,10,50,100,1000,10000},{0.0,0.45,0.367,0.367,0.25,0.141,0.12}),"MOQ="&amp;AL37),"")</f>
-        <v>0.25</v>
+        <f>IFERROR(IF(OR(AJ37&gt;=AL37,H37&gt;=AL37),LOOKUP(IF(AJ37="",H37,AJ37),{0,1,10,50,100,1000,10000},{0.0,0.61,0.524,0.524,0.391,0.238,0.204}),"MOQ="&amp;AL37),"")</f>
+        <v>0.391</v>
       </c>
       <c r="AL37" s="17">
         <v>1</v>
       </c>
       <c r="AM37" s="19">
         <f>IFERROR(IF(AJ37="",H37,AJ37)*AK37,"")</f>
-        <v>25.0</v>
+        <v>39.1</v>
       </c>
       <c r="AN37" s="17" t="s">
         <v>292</v>
@@ -10915,15 +10890,15 @@
       </c>
       <c r="AP37" s="17"/>
       <c r="AQ37" s="18">
-        <f>IFERROR(IF(OR(AP37&gt;=AR37,H37&gt;=AR37),LOOKUP(IF(AP37="",H37,AP37),{0,1,10,100,3000,4000,6000,12000,18000,30000},{0.0,0.268,0.255,0.229,0.131,0.131,0.117,0.106,0.098,0.091}),"MOQ="&amp;AR37),"")</f>
-        <v>0.229</v>
+        <f>IFERROR(IF(OR(AP37&gt;=AR37,H37&gt;=AR37),LOOKUP(IF(AP37="",H37,AP37),{0,1,10,100,3000,4000,6000,12000,18000,30000},{0.0,0.262,0.248,0.223,0.131,0.131,0.117,0.106,0.098,0.091}),"MOQ="&amp;AR37),"")</f>
+        <v>0.223</v>
       </c>
       <c r="AR37" s="17">
         <v>1</v>
       </c>
       <c r="AS37" s="19">
         <f>IFERROR(IF(AP37="",H37,AP37)*AQ37,"")</f>
-        <v>22.9</v>
+        <v>22.3</v>
       </c>
       <c r="AT37" s="17" t="s">
         <v>322</v>
@@ -10934,14 +10909,14 @@
       <c r="AV37" s="17"/>
       <c r="AW37" s="18">
         <f>IFERROR(IF(OR(AV37&gt;=AX37,H37&gt;=AX37),USD_GBP*LOOKUP(IF(AV37="",H37,AV37),{0,1,50,100,1000,4000,8000,24000,48000,100000},{0.0,0.295,0.295,0.227,0.219,0.205,0.185,0.083,0.076,0.073}),"MOQ="&amp;AX37),"")</f>
-        <v>0.29693612941881364</v>
+        <v>0.29783687943262416</v>
       </c>
       <c r="AX37" s="17">
         <v>50</v>
       </c>
       <c r="AY37" s="19">
         <f>IFERROR(IF(AV37="",H37,AV37)*AW37,"")</f>
-        <v>29.6936</v>
+        <v>29.7837</v>
       </c>
       <c r="AZ37" s="17" t="s">
         <v>338</v>
@@ -10951,15 +10926,15 @@
       </c>
       <c r="BB37" s="17"/>
       <c r="BC37" s="18">
-        <f>IFERROR(IF(OR(BB37&gt;=BD37,H37&gt;=BD37),USD_GBP*LOOKUP(IF(BB37="",H37,BB37),{0,1,5,25,100,500,2000},{0.0,0.172,0.172,0.1496,0.1296,0.11318,0.10564}),"MOQ="&amp;BD37),"")</f>
-        <v>0.16952829239065306</v>
+        <f>IFERROR(IF(OR(BB37&gt;=BD37,H37&gt;=BD37),USD_GBP*LOOKUP(IF(BB37="",H37,BB37),{0,1,5,25,100,500,2000},{0.0,0.17,0.17,0.1492,0.1292,0.11284,0.10532}),"MOQ="&amp;BD37),"")</f>
+        <v>0.16951773049645394</v>
       </c>
       <c r="BD37" s="17">
         <v>5</v>
       </c>
       <c r="BE37" s="19">
         <f>IFERROR(IF(BB37="",H37,BB37)*BC37,"")</f>
-        <v>16.9528</v>
+        <v>16.9518</v>
       </c>
       <c r="BF37" s="17" t="s">
         <v>152</v>
@@ -11014,20 +10989,20 @@
       <c r="V38" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="W38" s="20" t="s">
-        <v>197</v>
+      <c r="W38" s="17">
+        <v>465</v>
       </c>
       <c r="X38" s="17"/>
       <c r="Y38" s="18">
-        <f>IFERROR(IF(OR(X38&gt;=Z38,H38&gt;=Z38),USD_GBP*LOOKUP(IF(X38="",H38,X38),{0,1,25,100},{0.0,0.798,0.674,0.62}),"MOQ="&amp;Z38),"")</f>
-        <v>0.8110149790293588</v>
+        <f>IFERROR(IF(OR(X38&gt;=Z38,H38&gt;=Z38),USD_GBP*LOOKUP(IF(X38="",H38,X38),{0,1,25,100},{0.0,0.846,0.716,0.658}),"MOQ="&amp;Z38),"")</f>
+        <v>0.8633333333333335</v>
       </c>
       <c r="Z38" s="17">
         <v>1</v>
       </c>
       <c r="AA38" s="19">
         <f>IFERROR(IF(X38="",H38,X38)*Y38,"")</f>
-        <v>81.1015</v>
+        <v>86.3333</v>
       </c>
       <c r="AB38" s="17" t="s">
         <v>249</v>
@@ -11074,14 +11049,14 @@
       <c r="AV38" s="17"/>
       <c r="AW38" s="18">
         <f>IFERROR(IF(OR(AV38&gt;=AX38,H38&gt;=AX38),USD_GBP*LOOKUP(IF(AV38="",H38,AV38),{0,1,20,40,100,3000},{0.0,0.718,0.718,0.686,0.619,0.558}),"MOQ="&amp;AX38),"")</f>
-        <v>0.8097068903535051</v>
+        <v>0.812163120567376</v>
       </c>
       <c r="AX38" s="17">
         <v>20</v>
       </c>
       <c r="AY38" s="19">
         <f>IFERROR(IF(AV38="",H38,AV38)*AW38,"")</f>
-        <v>80.9707</v>
+        <v>81.2163</v>
       </c>
       <c r="AZ38" s="17" t="s">
         <v>339</v>
@@ -11091,15 +11066,15 @@
       </c>
       <c r="BB38" s="17"/>
       <c r="BC38" s="18">
-        <f>IFERROR(IF(OR(BB38&gt;=BD38,H38&gt;=BD38),USD_GBP*LOOKUP(IF(BB38="",H38,BB38),{0,1,5,25,100},{0.0,0.76,0.7,0.64,0.58}),"MOQ="&amp;BD38),"")</f>
-        <v>0.7586914319952066</v>
+        <f>IFERROR(IF(OR(BB38&gt;=BD38,H38&gt;=BD38),USD_GBP*LOOKUP(IF(BB38="",H38,BB38),{0,1,5,25,100},{0.0,0.76,0.71,0.65,0.58}),"MOQ="&amp;BD38),"")</f>
+        <v>0.7609929078014185</v>
       </c>
       <c r="BD38" s="17">
         <v>1</v>
       </c>
       <c r="BE38" s="19">
         <f>IFERROR(IF(BB38="",H38,BB38)*BC38,"")</f>
-        <v>75.8691</v>
+        <v>76.0993</v>
       </c>
       <c r="BF38" s="17" t="s">
         <v>343</v>
@@ -11140,7 +11115,7 @@
         <v>138.0</v>
       </c>
       <c r="AI39" s="17">
-        <v>52667</v>
+        <v>52038</v>
       </c>
       <c r="AJ39" s="17"/>
       <c r="AK39" s="18">
@@ -11254,18 +11229,18 @@
       </c>
       <c r="I41" s="18">
         <f>IF(MIN(M41,S41,Y41,AE41,AK41,AQ41,AW41,BC41)&lt;&gt;0,MIN(M41,S41,Y41,AE41,AK41,AQ41,AW41,BC41),"")</f>
-        <v>5.977965248651888</v>
+        <v>6.402836879432625</v>
       </c>
       <c r="J41" s="19">
         <f>IF(AND(ISNUMBER(H41),ISNUMBER(I41)),H41*I41,"")</f>
-        <v>597.7965</v>
-      </c>
-      <c r="Q41" s="20" t="s">
-        <v>197</v>
+        <v>640.2837</v>
+      </c>
+      <c r="Q41" s="17">
+        <v>847</v>
       </c>
       <c r="R41" s="17"/>
       <c r="S41" s="18">
-        <f>IFERROR(IF(OR(R41&gt;=T41,H41&gt;=T41),LOOKUP(IF(R41="",H41,R41),{0,1,25,100,2000},{0.0,9.15,7.95,7.67,6.95002}),"MOQ="&amp;T41),"")</f>
+        <f>IFERROR(IF(OR(R41&gt;=T41,H41&gt;=T41),LOOKUP(IF(R41="",H41,R41),{0,1,25,100,2000},{0.0,9.15,7.95,7.67,7.67}),"MOQ="&amp;T41),"")</f>
         <v>7.67</v>
       </c>
       <c r="T41" s="17">
@@ -11283,15 +11258,15 @@
       </c>
       <c r="X41" s="17"/>
       <c r="Y41" s="18">
-        <f>IFERROR(IF(OR(X41&gt;=Z41,H41&gt;=Z41),USD_GBP*LOOKUP(IF(X41="",H41,X41),{0,1,10,25,50,100},{0.0,5.87,5.27,4.66,4.57,4.57}),"MOQ="&amp;Z41),"")</f>
-        <v>5.977965248651888</v>
+        <f>IFERROR(IF(OR(X41&gt;=Z41,H41&gt;=Z41),USD_GBP*LOOKUP(IF(X41="",H41,X41),{0,1,10,25,50,100},{0.0,5.67,5.33,4.98,4.88,4.88}),"MOQ="&amp;Z41),"")</f>
+        <v>6.402836879432625</v>
       </c>
       <c r="Z41" s="17">
         <v>1</v>
       </c>
       <c r="AA41" s="19">
         <f>IFERROR(IF(X41="",H41,X41)*Y41,"")</f>
-        <v>597.7965</v>
+        <v>640.2837</v>
       </c>
       <c r="AB41" s="17" t="s">
         <v>250</v>
@@ -11361,14 +11336,14 @@
       </c>
       <c r="I42" s="18">
         <f>IF(MIN(M42,S42,Y42,AE42,AK42,AQ42,AW42,BC42)&lt;&gt;0,MIN(M42,S42,Y42,AE42,AK42,AQ42,AW42,BC42),"")</f>
-        <v>1.18</v>
+        <v>1.15</v>
       </c>
       <c r="J42" s="19">
         <f>IF(AND(ISNUMBER(H42),ISNUMBER(I42)),H42*I42,"")</f>
-        <v>118.0</v>
+        <v>115.0</v>
       </c>
       <c r="K42" s="17">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="L42" s="17"/>
       <c r="M42" s="18">
@@ -11386,7 +11361,7 @@
         <v>188</v>
       </c>
       <c r="Q42" s="17">
-        <v>2502</v>
+        <v>2487</v>
       </c>
       <c r="R42" s="17"/>
       <c r="S42" s="18">
@@ -11404,25 +11379,25 @@
         <v>222</v>
       </c>
       <c r="W42" s="17">
-        <v>200</v>
+        <v>102</v>
       </c>
       <c r="X42" s="17"/>
       <c r="Y42" s="18">
         <f>IFERROR(IF(OR(X42&gt;=Z42,H42&gt;=Z42),USD_GBP*LOOKUP(IF(X42="",H42,X42),{0,1,5,50,100,250,500,3000,15000},{0.0,1.44,1.44,1.21,1.21,1.09,0.965,0.906,0.888}),"MOQ="&amp;Z42),"")</f>
-        <v>1.5827872977831035</v>
+        <v>1.5875886524822698</v>
       </c>
       <c r="Z42" s="17">
         <v>5</v>
       </c>
       <c r="AA42" s="19">
         <f>IFERROR(IF(X42="",H42,X42)*Y42,"")</f>
-        <v>158.2787</v>
+        <v>158.7589</v>
       </c>
       <c r="AB42" s="17" t="s">
         <v>251</v>
       </c>
       <c r="AI42" s="17">
-        <v>2422</v>
+        <v>2322</v>
       </c>
       <c r="AJ42" s="17"/>
       <c r="AK42" s="18">
@@ -11444,15 +11419,15 @@
       </c>
       <c r="AP42" s="17"/>
       <c r="AQ42" s="18">
-        <f>IFERROR(IF(OR(AP42&gt;=AR42,H42&gt;=AR42),LOOKUP(IF(AP42="",H42,AP42),{0,1,10,25,50,100,1000,2000,3000,4000,6000,10000},{0.0,1.18,1.18,1.18,1.18,1.18,1.34,1.28,1.28,1.17,1.12,1.09}),"MOQ="&amp;AR42),"")</f>
-        <v>1.18</v>
+        <f>IFERROR(IF(OR(AP42&gt;=AR42,H42&gt;=AR42),LOOKUP(IF(AP42="",H42,AP42),{0,1,10,25,50,100,1000,2000,3000,4000,6000,10000},{0.0,1.15,1.15,1.15,1.15,1.15,1.34,1.28,1.28,1.17,1.12,1.09}),"MOQ="&amp;AR42),"")</f>
+        <v>1.15</v>
       </c>
       <c r="AR42" s="17">
         <v>1</v>
       </c>
       <c r="AS42" s="19">
         <f>IFERROR(IF(AP42="",H42,AP42)*AQ42,"")</f>
-        <v>118.0</v>
+        <v>115.0</v>
       </c>
       <c r="AT42" s="17" t="s">
         <v>325</v>
@@ -11463,14 +11438,14 @@
       <c r="AV42" s="17"/>
       <c r="AW42" s="18">
         <f>IFERROR(IF(OR(AV42&gt;=AX42,H42&gt;=AX42),USD_GBP*LOOKUP(IF(AV42="",H42,AV42),{0,1,5,50,100,250,1000,3000},{0.0,1.596,1.596,1.494,1.302,1.276,1.122,1.1}),"MOQ="&amp;AX42),"")</f>
-        <v>1.7031314559616537</v>
+        <v>1.7082978723404258</v>
       </c>
       <c r="AX42" s="17">
         <v>5</v>
       </c>
       <c r="AY42" s="19">
         <f>IFERROR(IF(AV42="",H42,AV42)*AW42,"")</f>
-        <v>170.3131</v>
+        <v>170.8298</v>
       </c>
       <c r="AZ42" s="17" t="s">
         <v>340</v>
@@ -11581,7 +11556,7 @@
         <v>347</v>
       </c>
       <c r="C45">
-        <v>1.308088675853805</v>
+        <v>1.312056737588653</v>
       </c>
       <c r="I45" s="21" t="s">
         <v>345</v>
@@ -13673,112 +13648,112 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO13">
-    <cfRule type="cellIs" dxfId="0" priority="559" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="558" operator="lessThan">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO14">
-    <cfRule type="cellIs" dxfId="0" priority="563" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="562" operator="lessThan">
       <formula>H14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO19">
-    <cfRule type="cellIs" dxfId="0" priority="567" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="566" operator="lessThan">
       <formula>H19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO20">
-    <cfRule type="cellIs" dxfId="0" priority="571" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="570" operator="lessThan">
       <formula>H20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO21">
-    <cfRule type="cellIs" dxfId="0" priority="575" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="574" operator="lessThan">
       <formula>H21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO22">
-    <cfRule type="cellIs" dxfId="0" priority="579" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="578" operator="lessThan">
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO23">
-    <cfRule type="cellIs" dxfId="0" priority="587" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="586" operator="lessThan">
       <formula>H23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO24">
-    <cfRule type="cellIs" dxfId="0" priority="595" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="594" operator="lessThan">
       <formula>H24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO25">
-    <cfRule type="cellIs" dxfId="0" priority="599" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="598" operator="lessThan">
       <formula>H25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO26">
-    <cfRule type="cellIs" dxfId="0" priority="603" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="602" operator="lessThan">
       <formula>H26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO27">
-    <cfRule type="cellIs" dxfId="0" priority="607" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="606" operator="lessThan">
       <formula>H27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO28">
-    <cfRule type="cellIs" dxfId="0" priority="615" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="614" operator="lessThan">
       <formula>H28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO29">
-    <cfRule type="cellIs" dxfId="0" priority="619" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="618" operator="lessThan">
       <formula>H29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO30">
-    <cfRule type="cellIs" dxfId="0" priority="623" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="622" operator="lessThan">
       <formula>H30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO31">
-    <cfRule type="cellIs" dxfId="0" priority="627" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="626" operator="lessThan">
       <formula>H31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO32">
-    <cfRule type="cellIs" dxfId="0" priority="631" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="630" operator="lessThan">
       <formula>H32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO33">
-    <cfRule type="cellIs" dxfId="0" priority="636" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="634" operator="lessThan">
       <formula>H33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO36">
-    <cfRule type="cellIs" dxfId="0" priority="640" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="638" operator="lessThan">
       <formula>H36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO37">
-    <cfRule type="cellIs" dxfId="0" priority="644" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="642" operator="lessThan">
       <formula>H37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO38">
-    <cfRule type="cellIs" dxfId="0" priority="648" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="646" operator="lessThan">
       <formula>H38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO41">
-    <cfRule type="cellIs" dxfId="0" priority="652" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="650" operator="lessThan">
       <formula>H41</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO42">
-    <cfRule type="cellIs" dxfId="0" priority="656" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="654" operator="lessThan">
       <formula>H42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13808,132 +13783,126 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP12">
-    <cfRule type="expression" dxfId="3" priority="555">
-      <formula>AND(AP12&gt;0,MOD(AP12,AR12)&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="556">
+    <cfRule type="expression" dxfId="1" priority="555">
       <formula>AND(NOT(ISBLANK(AP12)),OR(AO12="NonStk",AP12&gt;AO12))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP13">
-    <cfRule type="expression" dxfId="1" priority="560">
+    <cfRule type="expression" dxfId="1" priority="559">
       <formula>AND(NOT(ISBLANK(AP13)),OR(AO13="NonStk",AP13&gt;AO13))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP14">
-    <cfRule type="expression" dxfId="1" priority="564">
+    <cfRule type="expression" dxfId="1" priority="563">
       <formula>AND(NOT(ISBLANK(AP14)),OR(AO14="NonStk",AP14&gt;AO14))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP19">
-    <cfRule type="expression" dxfId="1" priority="568">
+    <cfRule type="expression" dxfId="1" priority="567">
       <formula>AND(NOT(ISBLANK(AP19)),OR(AO19="NonStk",AP19&gt;AO19))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP20">
-    <cfRule type="expression" dxfId="1" priority="572">
+    <cfRule type="expression" dxfId="1" priority="571">
       <formula>AND(NOT(ISBLANK(AP20)),OR(AO20="NonStk",AP20&gt;AO20))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP21">
-    <cfRule type="expression" dxfId="1" priority="576">
+    <cfRule type="expression" dxfId="1" priority="575">
       <formula>AND(NOT(ISBLANK(AP21)),OR(AO21="NonStk",AP21&gt;AO21))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP22">
-    <cfRule type="expression" dxfId="3" priority="580">
+    <cfRule type="expression" dxfId="3" priority="579">
       <formula>AND(AP22&gt;0,MOD(AP22,AR22)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="581">
+    <cfRule type="expression" dxfId="1" priority="580">
       <formula>AND(NOT(ISBLANK(AP22)),OR(AO22="NonStk",AP22&gt;AO22))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP23">
-    <cfRule type="expression" dxfId="3" priority="588">
+    <cfRule type="expression" dxfId="3" priority="587">
       <formula>AND(AP23&gt;0,MOD(AP23,AR23)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="589">
+    <cfRule type="expression" dxfId="1" priority="588">
       <formula>AND(NOT(ISBLANK(AP23)),OR(AO23="NonStk",AP23&gt;AO23))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP24">
-    <cfRule type="expression" dxfId="1" priority="596">
+    <cfRule type="expression" dxfId="1" priority="595">
       <formula>AND(NOT(ISBLANK(AP24)),OR(AO24="NonStk",AP24&gt;AO24))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP25">
-    <cfRule type="expression" dxfId="1" priority="600">
+    <cfRule type="expression" dxfId="1" priority="599">
       <formula>AND(NOT(ISBLANK(AP25)),OR(AO25="NonStk",AP25&gt;AO25))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP26">
-    <cfRule type="expression" dxfId="1" priority="604">
+    <cfRule type="expression" dxfId="1" priority="603">
       <formula>AND(NOT(ISBLANK(AP26)),OR(AO26="NonStk",AP26&gt;AO26))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP27">
-    <cfRule type="expression" dxfId="3" priority="608">
+    <cfRule type="expression" dxfId="3" priority="607">
       <formula>AND(AP27&gt;0,MOD(AP27,AR27)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="609">
+    <cfRule type="expression" dxfId="1" priority="608">
       <formula>AND(NOT(ISBLANK(AP27)),OR(AO27="NonStk",AP27&gt;AO27))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP28">
-    <cfRule type="expression" dxfId="1" priority="616">
+    <cfRule type="expression" dxfId="1" priority="615">
       <formula>AND(NOT(ISBLANK(AP28)),OR(AO28="NonStk",AP28&gt;AO28))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP29">
-    <cfRule type="expression" dxfId="1" priority="620">
+    <cfRule type="expression" dxfId="1" priority="619">
       <formula>AND(NOT(ISBLANK(AP29)),OR(AO29="NonStk",AP29&gt;AO29))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP30">
-    <cfRule type="expression" dxfId="1" priority="624">
+    <cfRule type="expression" dxfId="1" priority="623">
       <formula>AND(NOT(ISBLANK(AP30)),OR(AO30="NonStk",AP30&gt;AO30))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP31">
-    <cfRule type="expression" dxfId="1" priority="628">
+    <cfRule type="expression" dxfId="1" priority="627">
       <formula>AND(NOT(ISBLANK(AP31)),OR(AO31="NonStk",AP31&gt;AO31))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP32">
-    <cfRule type="expression" dxfId="3" priority="632">
-      <formula>AND(AP32&gt;0,MOD(AP32,AR32)&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="633">
+    <cfRule type="expression" dxfId="1" priority="631">
       <formula>AND(NOT(ISBLANK(AP32)),OR(AO32="NonStk",AP32&gt;AO32))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP33">
-    <cfRule type="expression" dxfId="1" priority="637">
+    <cfRule type="expression" dxfId="1" priority="635">
       <formula>AND(NOT(ISBLANK(AP33)),OR(AO33="NonStk",AP33&gt;AO33))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP36">
-    <cfRule type="expression" dxfId="1" priority="641">
+    <cfRule type="expression" dxfId="1" priority="639">
       <formula>AND(NOT(ISBLANK(AP36)),OR(AO36="NonStk",AP36&gt;AO36))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP37">
-    <cfRule type="expression" dxfId="1" priority="645">
+    <cfRule type="expression" dxfId="1" priority="643">
       <formula>AND(NOT(ISBLANK(AP37)),OR(AO37="NonStk",AP37&gt;AO37))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP38">
-    <cfRule type="expression" dxfId="1" priority="649">
+    <cfRule type="expression" dxfId="1" priority="647">
       <formula>AND(NOT(ISBLANK(AP38)),OR(AO38="NonStk",AP38&gt;AO38))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP41">
-    <cfRule type="expression" dxfId="1" priority="653">
+    <cfRule type="expression" dxfId="1" priority="651">
       <formula>AND(NOT(ISBLANK(AP41)),OR(AO41="NonStk",AP41&gt;AO41))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP42">
-    <cfRule type="expression" dxfId="1" priority="657">
+    <cfRule type="expression" dxfId="1" priority="655">
       <formula>AND(NOT(ISBLANK(AP42)),OR(AO42="NonStk",AP42&gt;AO42))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13963,126 +13932,126 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ12">
-    <cfRule type="cellIs" dxfId="2" priority="558" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="557" operator="lessThanOrEqual">
       <formula>I12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ13">
-    <cfRule type="cellIs" dxfId="2" priority="562" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="561" operator="lessThanOrEqual">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ14">
-    <cfRule type="cellIs" dxfId="2" priority="566" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="565" operator="lessThanOrEqual">
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ19">
-    <cfRule type="cellIs" dxfId="2" priority="570" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="569" operator="lessThanOrEqual">
       <formula>I19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ20">
-    <cfRule type="cellIs" dxfId="2" priority="574" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="573" operator="lessThanOrEqual">
       <formula>I20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ21">
-    <cfRule type="cellIs" dxfId="2" priority="578" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="577" operator="lessThanOrEqual">
       <formula>I21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ22">
-    <cfRule type="cellIs" dxfId="2" priority="583" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="582" operator="lessThanOrEqual">
       <formula>I22</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="584">
+    <cfRule type="expression" dxfId="3" priority="583">
       <formula>AND(H22&lt;15000,AP22&lt;15000)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ23">
-    <cfRule type="cellIs" dxfId="2" priority="591" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="590" operator="lessThanOrEqual">
       <formula>I23</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="592">
+    <cfRule type="expression" dxfId="3" priority="591">
       <formula>AND(H23&lt;15000,AP23&lt;15000)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ24">
-    <cfRule type="cellIs" dxfId="2" priority="598" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="597" operator="lessThanOrEqual">
       <formula>I24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ25">
-    <cfRule type="cellIs" dxfId="2" priority="602" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="601" operator="lessThanOrEqual">
       <formula>I25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ26">
-    <cfRule type="cellIs" dxfId="2" priority="606" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="605" operator="lessThanOrEqual">
       <formula>I26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ27">
-    <cfRule type="cellIs" dxfId="2" priority="611" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="610" operator="lessThanOrEqual">
       <formula>I27</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="612">
+    <cfRule type="expression" dxfId="3" priority="611">
       <formula>AND(H27&lt;15000,AP27&lt;15000)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ28">
-    <cfRule type="cellIs" dxfId="2" priority="618" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="617" operator="lessThanOrEqual">
       <formula>I28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ29">
-    <cfRule type="cellIs" dxfId="2" priority="622" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="621" operator="lessThanOrEqual">
       <formula>I29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ30">
-    <cfRule type="cellIs" dxfId="2" priority="626" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="625" operator="lessThanOrEqual">
       <formula>I30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ31">
-    <cfRule type="cellIs" dxfId="2" priority="630" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="629" operator="lessThanOrEqual">
       <formula>I31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ32">
-    <cfRule type="cellIs" dxfId="2" priority="635" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="633" operator="lessThanOrEqual">
       <formula>I32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ33">
-    <cfRule type="cellIs" dxfId="2" priority="639" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="637" operator="lessThanOrEqual">
       <formula>I33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ36">
-    <cfRule type="cellIs" dxfId="2" priority="643" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="641" operator="lessThanOrEqual">
       <formula>I36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ37">
-    <cfRule type="cellIs" dxfId="2" priority="647" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="645" operator="lessThanOrEqual">
       <formula>I37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ38">
-    <cfRule type="cellIs" dxfId="2" priority="651" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="649" operator="lessThanOrEqual">
       <formula>I38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ41">
-    <cfRule type="cellIs" dxfId="2" priority="655" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="653" operator="lessThanOrEqual">
       <formula>I41</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ42">
-    <cfRule type="cellIs" dxfId="2" priority="659" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="657" operator="lessThanOrEqual">
       <formula>I42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14102,17 +14071,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR22">
-    <cfRule type="expression" dxfId="3" priority="585">
+    <cfRule type="expression" dxfId="3" priority="584">
       <formula>AND(H22&lt;15000,AP22&lt;15000)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR23">
-    <cfRule type="expression" dxfId="3" priority="593">
+    <cfRule type="expression" dxfId="3" priority="592">
       <formula>AND(H23&lt;15000,AP23&lt;15000)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR27">
-    <cfRule type="expression" dxfId="3" priority="613">
+    <cfRule type="expression" dxfId="3" priority="612">
       <formula>AND(H27&lt;15000,AP27&lt;15000)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14127,126 +14096,126 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS12">
-    <cfRule type="cellIs" dxfId="2" priority="557" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="556" operator="lessThanOrEqual">
       <formula>J12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS13">
-    <cfRule type="cellIs" dxfId="2" priority="561" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="560" operator="lessThanOrEqual">
       <formula>J13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS14">
-    <cfRule type="cellIs" dxfId="2" priority="565" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="564" operator="lessThanOrEqual">
       <formula>J14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS19">
-    <cfRule type="cellIs" dxfId="2" priority="569" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="568" operator="lessThanOrEqual">
       <formula>J19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS20">
-    <cfRule type="cellIs" dxfId="2" priority="573" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="572" operator="lessThanOrEqual">
       <formula>J20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS21">
-    <cfRule type="cellIs" dxfId="2" priority="577" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="576" operator="lessThanOrEqual">
       <formula>J21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS22">
-    <cfRule type="cellIs" dxfId="2" priority="582" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="581" operator="lessThanOrEqual">
       <formula>J22</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="586">
+    <cfRule type="expression" dxfId="3" priority="585">
       <formula>AND(H22&lt;15000,AP22&lt;15000)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS23">
-    <cfRule type="cellIs" dxfId="2" priority="590" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="589" operator="lessThanOrEqual">
       <formula>J23</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="594">
+    <cfRule type="expression" dxfId="3" priority="593">
       <formula>AND(H23&lt;15000,AP23&lt;15000)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS24">
-    <cfRule type="cellIs" dxfId="2" priority="597" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="596" operator="lessThanOrEqual">
       <formula>J24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS25">
-    <cfRule type="cellIs" dxfId="2" priority="601" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="600" operator="lessThanOrEqual">
       <formula>J25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS26">
-    <cfRule type="cellIs" dxfId="2" priority="605" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="604" operator="lessThanOrEqual">
       <formula>J26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS27">
-    <cfRule type="cellIs" dxfId="2" priority="610" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="609" operator="lessThanOrEqual">
       <formula>J27</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="614">
+    <cfRule type="expression" dxfId="3" priority="613">
       <formula>AND(H27&lt;15000,AP27&lt;15000)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS28">
-    <cfRule type="cellIs" dxfId="2" priority="617" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="616" operator="lessThanOrEqual">
       <formula>J28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS29">
-    <cfRule type="cellIs" dxfId="2" priority="621" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="620" operator="lessThanOrEqual">
       <formula>J29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS30">
-    <cfRule type="cellIs" dxfId="2" priority="625" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="624" operator="lessThanOrEqual">
       <formula>J30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS31">
-    <cfRule type="cellIs" dxfId="2" priority="629" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="628" operator="lessThanOrEqual">
       <formula>J31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS32">
-    <cfRule type="cellIs" dxfId="2" priority="634" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="632" operator="lessThanOrEqual">
       <formula>J32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS33">
-    <cfRule type="cellIs" dxfId="2" priority="638" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="636" operator="lessThanOrEqual">
       <formula>J33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS36">
-    <cfRule type="cellIs" dxfId="2" priority="642" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="640" operator="lessThanOrEqual">
       <formula>J36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS37">
-    <cfRule type="cellIs" dxfId="2" priority="646" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="644" operator="lessThanOrEqual">
       <formula>J37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS38">
-    <cfRule type="cellIs" dxfId="2" priority="650" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="648" operator="lessThanOrEqual">
       <formula>J38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS41">
-    <cfRule type="cellIs" dxfId="2" priority="654" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="652" operator="lessThanOrEqual">
       <formula>J41</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS42">
-    <cfRule type="cellIs" dxfId="2" priority="658" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="656" operator="lessThanOrEqual">
       <formula>J42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14266,1028 +14235,1028 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU10">
-    <cfRule type="cellIs" dxfId="0" priority="660" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="658" operator="lessThan">
       <formula>H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU12">
-    <cfRule type="cellIs" dxfId="0" priority="665" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="663" operator="lessThan">
       <formula>H12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU20">
-    <cfRule type="cellIs" dxfId="0" priority="670" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="668" operator="lessThan">
       <formula>H20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU22">
-    <cfRule type="cellIs" dxfId="0" priority="678" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="676" operator="lessThan">
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU23">
-    <cfRule type="cellIs" dxfId="0" priority="686" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="684" operator="lessThan">
       <formula>H23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU24">
-    <cfRule type="cellIs" dxfId="0" priority="694" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="692" operator="lessThan">
       <formula>H24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU26">
-    <cfRule type="cellIs" dxfId="0" priority="702" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="700" operator="lessThan">
       <formula>H26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU28">
-    <cfRule type="cellIs" dxfId="0" priority="710" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="708" operator="lessThan">
       <formula>H28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU29">
-    <cfRule type="cellIs" dxfId="0" priority="718" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="716" operator="lessThan">
       <formula>H29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU30">
-    <cfRule type="cellIs" dxfId="0" priority="726" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="724" operator="lessThan">
       <formula>H30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU33">
-    <cfRule type="cellIs" dxfId="0" priority="734" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="732" operator="lessThan">
       <formula>H33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU37">
-    <cfRule type="cellIs" dxfId="0" priority="739" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="737" operator="lessThan">
       <formula>H37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU38">
-    <cfRule type="cellIs" dxfId="0" priority="744" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="742" operator="lessThan">
       <formula>H38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU42">
-    <cfRule type="cellIs" dxfId="0" priority="749" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="747" operator="lessThan">
       <formula>H42</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV10">
-    <cfRule type="expression" dxfId="3" priority="661">
+    <cfRule type="expression" dxfId="3" priority="659">
       <formula>AND(AV10&gt;0,MOD(AV10,AX10)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="662">
+    <cfRule type="expression" dxfId="1" priority="660">
       <formula>AND(NOT(ISBLANK(AV10)),OR(AU10="NonStk",AV10&gt;AU10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV12">
-    <cfRule type="expression" dxfId="3" priority="666">
+    <cfRule type="expression" dxfId="3" priority="664">
       <formula>AND(AV12&gt;0,MOD(AV12,AX12)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="667">
+    <cfRule type="expression" dxfId="1" priority="665">
       <formula>AND(NOT(ISBLANK(AV12)),OR(AU12="NonStk",AV12&gt;AU12))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV20">
-    <cfRule type="expression" dxfId="3" priority="671">
+    <cfRule type="expression" dxfId="3" priority="669">
       <formula>AND(AV20&gt;0,MOD(AV20,AX20)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="672">
+    <cfRule type="expression" dxfId="1" priority="670">
       <formula>AND(NOT(ISBLANK(AV20)),OR(AU20="NonStk",AV20&gt;AU20))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV22">
-    <cfRule type="expression" dxfId="3" priority="679">
+    <cfRule type="expression" dxfId="3" priority="677">
       <formula>AND(AV22&gt;0,MOD(AV22,AX22)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="680">
+    <cfRule type="expression" dxfId="1" priority="678">
       <formula>AND(NOT(ISBLANK(AV22)),OR(AU22="NonStk",AV22&gt;AU22))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV23">
-    <cfRule type="expression" dxfId="3" priority="687">
+    <cfRule type="expression" dxfId="3" priority="685">
       <formula>AND(AV23&gt;0,MOD(AV23,AX23)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="688">
+    <cfRule type="expression" dxfId="1" priority="686">
       <formula>AND(NOT(ISBLANK(AV23)),OR(AU23="NonStk",AV23&gt;AU23))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV24">
-    <cfRule type="expression" dxfId="3" priority="695">
+    <cfRule type="expression" dxfId="3" priority="693">
       <formula>AND(AV24&gt;0,MOD(AV24,AX24)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="696">
+    <cfRule type="expression" dxfId="1" priority="694">
       <formula>AND(NOT(ISBLANK(AV24)),OR(AU24="NonStk",AV24&gt;AU24))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV26">
-    <cfRule type="expression" dxfId="3" priority="703">
+    <cfRule type="expression" dxfId="3" priority="701">
       <formula>AND(AV26&gt;0,MOD(AV26,AX26)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="704">
+    <cfRule type="expression" dxfId="1" priority="702">
       <formula>AND(NOT(ISBLANK(AV26)),OR(AU26="NonStk",AV26&gt;AU26))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV28">
-    <cfRule type="expression" dxfId="3" priority="711">
+    <cfRule type="expression" dxfId="3" priority="709">
       <formula>AND(AV28&gt;0,MOD(AV28,AX28)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="712">
+    <cfRule type="expression" dxfId="1" priority="710">
       <formula>AND(NOT(ISBLANK(AV28)),OR(AU28="NonStk",AV28&gt;AU28))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV29">
-    <cfRule type="expression" dxfId="3" priority="719">
+    <cfRule type="expression" dxfId="3" priority="717">
       <formula>AND(AV29&gt;0,MOD(AV29,AX29)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="720">
+    <cfRule type="expression" dxfId="1" priority="718">
       <formula>AND(NOT(ISBLANK(AV29)),OR(AU29="NonStk",AV29&gt;AU29))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV30">
-    <cfRule type="expression" dxfId="3" priority="727">
+    <cfRule type="expression" dxfId="3" priority="725">
       <formula>AND(AV30&gt;0,MOD(AV30,AX30)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="728">
+    <cfRule type="expression" dxfId="1" priority="726">
       <formula>AND(NOT(ISBLANK(AV30)),OR(AU30="NonStk",AV30&gt;AU30))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV33">
-    <cfRule type="expression" dxfId="3" priority="735">
+    <cfRule type="expression" dxfId="3" priority="733">
       <formula>AND(AV33&gt;0,MOD(AV33,AX33)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="736">
+    <cfRule type="expression" dxfId="1" priority="734">
       <formula>AND(NOT(ISBLANK(AV33)),OR(AU33="NonStk",AV33&gt;AU33))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV37">
-    <cfRule type="expression" dxfId="3" priority="740">
+    <cfRule type="expression" dxfId="3" priority="738">
       <formula>AND(AV37&gt;0,MOD(AV37,AX37)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="741">
+    <cfRule type="expression" dxfId="1" priority="739">
       <formula>AND(NOT(ISBLANK(AV37)),OR(AU37="NonStk",AV37&gt;AU37))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV38">
-    <cfRule type="expression" dxfId="3" priority="745">
+    <cfRule type="expression" dxfId="3" priority="743">
       <formula>AND(AV38&gt;0,MOD(AV38,AX38)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="746">
+    <cfRule type="expression" dxfId="1" priority="744">
       <formula>AND(NOT(ISBLANK(AV38)),OR(AU38="NonStk",AV38&gt;AU38))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV42">
-    <cfRule type="expression" dxfId="3" priority="750">
+    <cfRule type="expression" dxfId="3" priority="748">
       <formula>AND(AV42&gt;0,MOD(AV42,AX42)&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="751">
+    <cfRule type="expression" dxfId="1" priority="749">
       <formula>AND(NOT(ISBLANK(AV42)),OR(AU42="NonStk",AV42&gt;AU42))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW10">
-    <cfRule type="cellIs" dxfId="2" priority="664" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="662" operator="lessThanOrEqual">
       <formula>I10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW12">
-    <cfRule type="cellIs" dxfId="2" priority="669" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="667" operator="lessThanOrEqual">
       <formula>I12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW20">
-    <cfRule type="cellIs" dxfId="2" priority="674" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="672" operator="lessThanOrEqual">
       <formula>I20</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="673">
+      <formula>AND(H20&lt;1000,AV20&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW22">
+    <cfRule type="cellIs" dxfId="2" priority="680" operator="lessThanOrEqual">
+      <formula>I22</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="681">
+      <formula>AND(H22&lt;1000,AV22&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW23">
+    <cfRule type="cellIs" dxfId="2" priority="688" operator="lessThanOrEqual">
+      <formula>I23</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="689">
+      <formula>AND(H23&lt;1000,AV23&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW24">
+    <cfRule type="cellIs" dxfId="2" priority="696" operator="lessThanOrEqual">
+      <formula>I24</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="697">
+      <formula>AND(H24&lt;1000,AV24&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW26">
+    <cfRule type="cellIs" dxfId="2" priority="704" operator="lessThanOrEqual">
+      <formula>I26</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="705">
+      <formula>AND(H26&lt;1000,AV26&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW28">
+    <cfRule type="cellIs" dxfId="2" priority="712" operator="lessThanOrEqual">
+      <formula>I28</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="713">
+      <formula>AND(H28&lt;1000,AV28&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW29">
+    <cfRule type="cellIs" dxfId="2" priority="720" operator="lessThanOrEqual">
+      <formula>I29</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="721">
+      <formula>AND(H29&lt;1000,AV29&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW30">
+    <cfRule type="cellIs" dxfId="2" priority="728" operator="lessThanOrEqual">
+      <formula>I30</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="729">
+      <formula>AND(H30&lt;1000,AV30&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW33">
+    <cfRule type="cellIs" dxfId="2" priority="736" operator="lessThanOrEqual">
+      <formula>I33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW37">
+    <cfRule type="cellIs" dxfId="2" priority="741" operator="lessThanOrEqual">
+      <formula>I37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW38">
+    <cfRule type="cellIs" dxfId="2" priority="746" operator="lessThanOrEqual">
+      <formula>I38</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW42">
+    <cfRule type="cellIs" dxfId="2" priority="751" operator="lessThanOrEqual">
+      <formula>I42</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AX20">
+    <cfRule type="expression" dxfId="3" priority="674">
+      <formula>AND(H20&lt;1000,AV20&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AX22">
+    <cfRule type="expression" dxfId="3" priority="682">
+      <formula>AND(H22&lt;1000,AV22&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AX23">
+    <cfRule type="expression" dxfId="3" priority="690">
+      <formula>AND(H23&lt;1000,AV23&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AX24">
+    <cfRule type="expression" dxfId="3" priority="698">
+      <formula>AND(H24&lt;1000,AV24&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AX26">
+    <cfRule type="expression" dxfId="3" priority="706">
+      <formula>AND(H26&lt;1000,AV26&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AX28">
+    <cfRule type="expression" dxfId="3" priority="714">
+      <formula>AND(H28&lt;1000,AV28&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AX29">
+    <cfRule type="expression" dxfId="3" priority="722">
+      <formula>AND(H29&lt;1000,AV29&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AX30">
+    <cfRule type="expression" dxfId="3" priority="730">
+      <formula>AND(H30&lt;1000,AV30&lt;1000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY10">
+    <cfRule type="cellIs" dxfId="2" priority="661" operator="lessThanOrEqual">
+      <formula>J10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY12">
+    <cfRule type="cellIs" dxfId="2" priority="666" operator="lessThanOrEqual">
+      <formula>J12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY20">
+    <cfRule type="cellIs" dxfId="2" priority="671" operator="lessThanOrEqual">
+      <formula>J20</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="675">
       <formula>AND(H20&lt;1000,AV20&lt;1000)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW22">
-    <cfRule type="cellIs" dxfId="2" priority="682" operator="lessThanOrEqual">
-      <formula>I22</formula>
+  <conditionalFormatting sqref="AY22">
+    <cfRule type="cellIs" dxfId="2" priority="679" operator="lessThanOrEqual">
+      <formula>J22</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="683">
       <formula>AND(H22&lt;1000,AV22&lt;1000)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW23">
-    <cfRule type="cellIs" dxfId="2" priority="690" operator="lessThanOrEqual">
-      <formula>I23</formula>
+  <conditionalFormatting sqref="AY23">
+    <cfRule type="cellIs" dxfId="2" priority="687" operator="lessThanOrEqual">
+      <formula>J23</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="691">
       <formula>AND(H23&lt;1000,AV23&lt;1000)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW24">
-    <cfRule type="cellIs" dxfId="2" priority="698" operator="lessThanOrEqual">
-      <formula>I24</formula>
+  <conditionalFormatting sqref="AY24">
+    <cfRule type="cellIs" dxfId="2" priority="695" operator="lessThanOrEqual">
+      <formula>J24</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="699">
       <formula>AND(H24&lt;1000,AV24&lt;1000)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW26">
-    <cfRule type="cellIs" dxfId="2" priority="706" operator="lessThanOrEqual">
-      <formula>I26</formula>
+  <conditionalFormatting sqref="AY26">
+    <cfRule type="cellIs" dxfId="2" priority="703" operator="lessThanOrEqual">
+      <formula>J26</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="707">
       <formula>AND(H26&lt;1000,AV26&lt;1000)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW28">
-    <cfRule type="cellIs" dxfId="2" priority="714" operator="lessThanOrEqual">
-      <formula>I28</formula>
+  <conditionalFormatting sqref="AY28">
+    <cfRule type="cellIs" dxfId="2" priority="711" operator="lessThanOrEqual">
+      <formula>J28</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="715">
       <formula>AND(H28&lt;1000,AV28&lt;1000)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW29">
-    <cfRule type="cellIs" dxfId="2" priority="722" operator="lessThanOrEqual">
-      <formula>I29</formula>
+  <conditionalFormatting sqref="AY29">
+    <cfRule type="cellIs" dxfId="2" priority="719" operator="lessThanOrEqual">
+      <formula>J29</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="723">
       <formula>AND(H29&lt;1000,AV29&lt;1000)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW30">
-    <cfRule type="cellIs" dxfId="2" priority="730" operator="lessThanOrEqual">
-      <formula>I30</formula>
+  <conditionalFormatting sqref="AY30">
+    <cfRule type="cellIs" dxfId="2" priority="727" operator="lessThanOrEqual">
+      <formula>J30</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="731">
       <formula>AND(H30&lt;1000,AV30&lt;1000)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW33">
-    <cfRule type="cellIs" dxfId="2" priority="738" operator="lessThanOrEqual">
-      <formula>I33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW37">
-    <cfRule type="cellIs" dxfId="2" priority="743" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AY33">
+    <cfRule type="cellIs" dxfId="2" priority="735" operator="lessThanOrEqual">
+      <formula>J33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY37">
+    <cfRule type="cellIs" dxfId="2" priority="740" operator="lessThanOrEqual">
+      <formula>J37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY38">
+    <cfRule type="cellIs" dxfId="2" priority="745" operator="lessThanOrEqual">
+      <formula>J38</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY42">
+    <cfRule type="cellIs" dxfId="2" priority="750" operator="lessThanOrEqual">
+      <formula>J42</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BA13">
+    <cfRule type="cellIs" dxfId="0" priority="752" operator="lessThan">
+      <formula>H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BA14">
+    <cfRule type="cellIs" dxfId="0" priority="757" operator="lessThan">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BA32">
+    <cfRule type="cellIs" dxfId="0" priority="762" operator="lessThan">
+      <formula>H32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BA37">
+    <cfRule type="cellIs" dxfId="0" priority="767" operator="lessThan">
+      <formula>H37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BA38">
+    <cfRule type="cellIs" dxfId="0" priority="772" operator="lessThan">
+      <formula>H38</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB13">
+    <cfRule type="expression" dxfId="3" priority="753">
+      <formula>AND(BB13&gt;0,MOD(BB13,BD13)&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="754">
+      <formula>AND(NOT(ISBLANK(BB13)),OR(BA13="NonStk",BB13&gt;BA13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB14">
+    <cfRule type="expression" dxfId="3" priority="758">
+      <formula>AND(BB14&gt;0,MOD(BB14,BD14)&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="759">
+      <formula>AND(NOT(ISBLANK(BB14)),OR(BA14="NonStk",BB14&gt;BA14))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB32">
+    <cfRule type="expression" dxfId="3" priority="763">
+      <formula>AND(BB32&gt;0,MOD(BB32,BD32)&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="764">
+      <formula>AND(NOT(ISBLANK(BB32)),OR(BA32="NonStk",BB32&gt;BA32))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB37">
+    <cfRule type="expression" dxfId="3" priority="768">
+      <formula>AND(BB37&gt;0,MOD(BB37,BD37)&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="769">
+      <formula>AND(NOT(ISBLANK(BB37)),OR(BA37="NonStk",BB37&gt;BA37))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB38">
+    <cfRule type="expression" dxfId="1" priority="773">
+      <formula>AND(NOT(ISBLANK(BB38)),OR(BA38="NonStk",BB38&gt;BA38))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC13">
+    <cfRule type="cellIs" dxfId="2" priority="756" operator="lessThanOrEqual">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC14">
+    <cfRule type="cellIs" dxfId="2" priority="761" operator="lessThanOrEqual">
+      <formula>I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC32">
+    <cfRule type="cellIs" dxfId="2" priority="766" operator="lessThanOrEqual">
+      <formula>I32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC37">
+    <cfRule type="cellIs" dxfId="2" priority="771" operator="lessThanOrEqual">
       <formula>I37</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW38">
-    <cfRule type="cellIs" dxfId="2" priority="748" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="BC38">
+    <cfRule type="cellIs" dxfId="2" priority="775" operator="lessThanOrEqual">
       <formula>I38</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW42">
-    <cfRule type="cellIs" dxfId="2" priority="753" operator="lessThanOrEqual">
-      <formula>I42</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AX20">
-    <cfRule type="expression" dxfId="3" priority="676">
-      <formula>AND(H20&lt;1000,AV20&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AX22">
-    <cfRule type="expression" dxfId="3" priority="684">
-      <formula>AND(H22&lt;1000,AV22&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AX23">
-    <cfRule type="expression" dxfId="3" priority="692">
-      <formula>AND(H23&lt;1000,AV23&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AX24">
-    <cfRule type="expression" dxfId="3" priority="700">
-      <formula>AND(H24&lt;1000,AV24&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AX26">
-    <cfRule type="expression" dxfId="3" priority="708">
-      <formula>AND(H26&lt;1000,AV26&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AX28">
-    <cfRule type="expression" dxfId="3" priority="716">
-      <formula>AND(H28&lt;1000,AV28&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AX29">
-    <cfRule type="expression" dxfId="3" priority="724">
-      <formula>AND(H29&lt;1000,AV29&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AX30">
-    <cfRule type="expression" dxfId="3" priority="732">
-      <formula>AND(H30&lt;1000,AV30&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY10">
-    <cfRule type="cellIs" dxfId="2" priority="663" operator="lessThanOrEqual">
-      <formula>J10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY12">
-    <cfRule type="cellIs" dxfId="2" priority="668" operator="lessThanOrEqual">
-      <formula>J12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY20">
-    <cfRule type="cellIs" dxfId="2" priority="673" operator="lessThanOrEqual">
-      <formula>J20</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="677">
-      <formula>AND(H20&lt;1000,AV20&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY22">
-    <cfRule type="cellIs" dxfId="2" priority="681" operator="lessThanOrEqual">
-      <formula>J22</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="685">
-      <formula>AND(H22&lt;1000,AV22&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY23">
-    <cfRule type="cellIs" dxfId="2" priority="689" operator="lessThanOrEqual">
-      <formula>J23</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="693">
-      <formula>AND(H23&lt;1000,AV23&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY24">
-    <cfRule type="cellIs" dxfId="2" priority="697" operator="lessThanOrEqual">
-      <formula>J24</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="701">
-      <formula>AND(H24&lt;1000,AV24&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY26">
-    <cfRule type="cellIs" dxfId="2" priority="705" operator="lessThanOrEqual">
-      <formula>J26</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="709">
-      <formula>AND(H26&lt;1000,AV26&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY28">
-    <cfRule type="cellIs" dxfId="2" priority="713" operator="lessThanOrEqual">
-      <formula>J28</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="717">
-      <formula>AND(H28&lt;1000,AV28&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY29">
-    <cfRule type="cellIs" dxfId="2" priority="721" operator="lessThanOrEqual">
-      <formula>J29</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="725">
-      <formula>AND(H29&lt;1000,AV29&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY30">
-    <cfRule type="cellIs" dxfId="2" priority="729" operator="lessThanOrEqual">
-      <formula>J30</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="733">
-      <formula>AND(H30&lt;1000,AV30&lt;1000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY33">
-    <cfRule type="cellIs" dxfId="2" priority="737" operator="lessThanOrEqual">
-      <formula>J33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY37">
-    <cfRule type="cellIs" dxfId="2" priority="742" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="BE13">
+    <cfRule type="cellIs" dxfId="2" priority="755" operator="lessThanOrEqual">
+      <formula>J13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BE14">
+    <cfRule type="cellIs" dxfId="2" priority="760" operator="lessThanOrEqual">
+      <formula>J14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BE32">
+    <cfRule type="cellIs" dxfId="2" priority="765" operator="lessThanOrEqual">
+      <formula>J32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BE37">
+    <cfRule type="cellIs" dxfId="2" priority="770" operator="lessThanOrEqual">
       <formula>J37</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AY38">
-    <cfRule type="cellIs" dxfId="2" priority="747" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="BE38">
+    <cfRule type="cellIs" dxfId="2" priority="774" operator="lessThanOrEqual">
       <formula>J38</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AY42">
-    <cfRule type="cellIs" dxfId="2" priority="752" operator="lessThanOrEqual">
-      <formula>J42</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BA13">
-    <cfRule type="cellIs" dxfId="0" priority="754" operator="lessThan">
-      <formula>H13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BA14">
-    <cfRule type="cellIs" dxfId="0" priority="759" operator="lessThan">
-      <formula>H14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BA32">
-    <cfRule type="cellIs" dxfId="0" priority="764" operator="lessThan">
-      <formula>H32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BA37">
-    <cfRule type="cellIs" dxfId="0" priority="769" operator="lessThan">
-      <formula>H37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BA38">
-    <cfRule type="cellIs" dxfId="0" priority="774" operator="lessThan">
-      <formula>H38</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BB13">
-    <cfRule type="expression" dxfId="3" priority="755">
-      <formula>AND(BB13&gt;0,MOD(BB13,BD13)&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="756">
-      <formula>AND(NOT(ISBLANK(BB13)),OR(BA13="NonStk",BB13&gt;BA13))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BB14">
-    <cfRule type="expression" dxfId="3" priority="760">
-      <formula>AND(BB14&gt;0,MOD(BB14,BD14)&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="761">
-      <formula>AND(NOT(ISBLANK(BB14)),OR(BA14="NonStk",BB14&gt;BA14))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BB32">
-    <cfRule type="expression" dxfId="3" priority="765">
-      <formula>AND(BB32&gt;0,MOD(BB32,BD32)&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="766">
-      <formula>AND(NOT(ISBLANK(BB32)),OR(BA32="NonStk",BB32&gt;BA32))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BB37">
-    <cfRule type="expression" dxfId="3" priority="770">
-      <formula>AND(BB37&gt;0,MOD(BB37,BD37)&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="771">
-      <formula>AND(NOT(ISBLANK(BB37)),OR(BA37="NonStk",BB37&gt;BA37))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BB38">
-    <cfRule type="expression" dxfId="1" priority="775">
-      <formula>AND(NOT(ISBLANK(BB38)),OR(BA38="NonStk",BB38&gt;BA38))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BC13">
-    <cfRule type="cellIs" dxfId="2" priority="758" operator="lessThanOrEqual">
-      <formula>I13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BC14">
-    <cfRule type="cellIs" dxfId="2" priority="763" operator="lessThanOrEqual">
-      <formula>I14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BC32">
-    <cfRule type="cellIs" dxfId="2" priority="768" operator="lessThanOrEqual">
-      <formula>I32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BC37">
-    <cfRule type="cellIs" dxfId="2" priority="773" operator="lessThanOrEqual">
-      <formula>I37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BC38">
-    <cfRule type="cellIs" dxfId="2" priority="777" operator="lessThanOrEqual">
-      <formula>I38</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BE13">
-    <cfRule type="cellIs" dxfId="2" priority="757" operator="lessThanOrEqual">
-      <formula>J13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BE14">
-    <cfRule type="cellIs" dxfId="2" priority="762" operator="lessThanOrEqual">
-      <formula>J14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BE32">
-    <cfRule type="cellIs" dxfId="2" priority="767" operator="lessThanOrEqual">
-      <formula>J32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BE37">
-    <cfRule type="cellIs" dxfId="2" priority="772" operator="lessThanOrEqual">
-      <formula>J37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BE38">
-    <cfRule type="cellIs" dxfId="2" priority="776" operator="lessThanOrEqual">
-      <formula>J38</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="4" priority="790">
+    <cfRule type="expression" dxfId="4" priority="788">
       <formula>AND(ISBLANK(G10),ISBLANK(O10),ISBLANK(U10),ISBLANK(AA10),ISBLANK(AG10),ISBLANK(AM10),ISBLANK(AS10),ISBLANK(AY10),ISBLANK(BE10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="791">
+    <cfRule type="expression" dxfId="1" priority="789">
       <formula>IF(SUM(K10,Q10,W10,AC10,AI10,AO10,AU10,BA10)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="792" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="790" operator="greaterThan">
       <formula>SUM(K10,Q10,W10,AC10,AI10,AO10,AU10,BA10)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="793" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="791" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M10),L10,0),IF(ISNUMBER(S10),R10,0),IF(ISNUMBER(Y10),X10,0),IF(ISNUMBER(AE10),AD10,0),IF(ISNUMBER(AK10),AJ10,0),IF(ISNUMBER(AQ10),AP10,0),IF(ISNUMBER(AW10),AV10,0),IF(ISNUMBER(BC10),BB10,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="4" priority="794">
+    <cfRule type="expression" dxfId="4" priority="792">
       <formula>AND(ISBLANK(G11),ISBLANK(O11),ISBLANK(U11),ISBLANK(AA11),ISBLANK(AG11),ISBLANK(AM11),ISBLANK(AS11),ISBLANK(AY11),ISBLANK(BE11))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="795">
+    <cfRule type="expression" dxfId="1" priority="793">
       <formula>IF(SUM(K11,Q11,W11,AC11,AI11,AO11,AU11,BA11)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="796" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="794" operator="greaterThan">
       <formula>SUM(K11,Q11,W11,AC11,AI11,AO11,AU11,BA11)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="797" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="795" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M11),L11,0),IF(ISNUMBER(S11),R11,0),IF(ISNUMBER(Y11),X11,0),IF(ISNUMBER(AE11),AD11,0),IF(ISNUMBER(AK11),AJ11,0),IF(ISNUMBER(AQ11),AP11,0),IF(ISNUMBER(AW11),AV11,0),IF(ISNUMBER(BC11),BB11,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="expression" dxfId="4" priority="798">
+    <cfRule type="expression" dxfId="4" priority="796">
       <formula>AND(ISBLANK(G12),ISBLANK(O12),ISBLANK(U12),ISBLANK(AA12),ISBLANK(AG12),ISBLANK(AM12),ISBLANK(AS12),ISBLANK(AY12),ISBLANK(BE12))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="799">
+    <cfRule type="expression" dxfId="1" priority="797">
       <formula>IF(SUM(K12,Q12,W12,AC12,AI12,AO12,AU12,BA12)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="800" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="798" operator="greaterThan">
       <formula>SUM(K12,Q12,W12,AC12,AI12,AO12,AU12,BA12)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="801" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="799" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M12),L12,0),IF(ISNUMBER(S12),R12,0),IF(ISNUMBER(Y12),X12,0),IF(ISNUMBER(AE12),AD12,0),IF(ISNUMBER(AK12),AJ12,0),IF(ISNUMBER(AQ12),AP12,0),IF(ISNUMBER(AW12),AV12,0),IF(ISNUMBER(BC12),BB12,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="expression" dxfId="4" priority="802">
+    <cfRule type="expression" dxfId="4" priority="800">
       <formula>AND(ISBLANK(G13),ISBLANK(O13),ISBLANK(U13),ISBLANK(AA13),ISBLANK(AG13),ISBLANK(AM13),ISBLANK(AS13),ISBLANK(AY13),ISBLANK(BE13))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="803">
+    <cfRule type="expression" dxfId="1" priority="801">
       <formula>IF(SUM(K13,Q13,W13,AC13,AI13,AO13,AU13,BA13)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="804" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="802" operator="greaterThan">
       <formula>SUM(K13,Q13,W13,AC13,AI13,AO13,AU13,BA13)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="805" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="803" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M13),L13,0),IF(ISNUMBER(S13),R13,0),IF(ISNUMBER(Y13),X13,0),IF(ISNUMBER(AE13),AD13,0),IF(ISNUMBER(AK13),AJ13,0),IF(ISNUMBER(AQ13),AP13,0),IF(ISNUMBER(AW13),AV13,0),IF(ISNUMBER(BC13),BB13,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="expression" dxfId="4" priority="806">
+    <cfRule type="expression" dxfId="4" priority="804">
       <formula>AND(ISBLANK(G14),ISBLANK(O14),ISBLANK(U14),ISBLANK(AA14),ISBLANK(AG14),ISBLANK(AM14),ISBLANK(AS14),ISBLANK(AY14),ISBLANK(BE14))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="807">
+    <cfRule type="expression" dxfId="1" priority="805">
       <formula>IF(SUM(K14,Q14,W14,AC14,AI14,AO14,AU14,BA14)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="808" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="806" operator="greaterThan">
       <formula>SUM(K14,Q14,W14,AC14,AI14,AO14,AU14,BA14)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="809" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="807" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M14),L14,0),IF(ISNUMBER(S14),R14,0),IF(ISNUMBER(Y14),X14,0),IF(ISNUMBER(AE14),AD14,0),IF(ISNUMBER(AK14),AJ14,0),IF(ISNUMBER(AQ14),AP14,0),IF(ISNUMBER(AW14),AV14,0),IF(ISNUMBER(BC14),BB14,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="expression" dxfId="4" priority="810">
+    <cfRule type="expression" dxfId="4" priority="808">
       <formula>AND(ISBLANK(G15),ISBLANK(O15),ISBLANK(U15),ISBLANK(AA15),ISBLANK(AG15),ISBLANK(AM15),ISBLANK(AS15),ISBLANK(AY15),ISBLANK(BE15))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="811">
+    <cfRule type="expression" dxfId="1" priority="809">
       <formula>IF(SUM(K15,Q15,W15,AC15,AI15,AO15,AU15,BA15)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="812" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="810" operator="greaterThan">
       <formula>SUM(K15,Q15,W15,AC15,AI15,AO15,AU15,BA15)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="813" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="811" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M15),L15,0),IF(ISNUMBER(S15),R15,0),IF(ISNUMBER(Y15),X15,0),IF(ISNUMBER(AE15),AD15,0),IF(ISNUMBER(AK15),AJ15,0),IF(ISNUMBER(AQ15),AP15,0),IF(ISNUMBER(AW15),AV15,0),IF(ISNUMBER(BC15),BB15,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="expression" dxfId="4" priority="814">
+    <cfRule type="expression" dxfId="4" priority="812">
       <formula>AND(ISBLANK(G16),ISBLANK(O16),ISBLANK(U16),ISBLANK(AA16),ISBLANK(AG16),ISBLANK(AM16),ISBLANK(AS16),ISBLANK(AY16),ISBLANK(BE16))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="815">
+    <cfRule type="expression" dxfId="1" priority="813">
       <formula>IF(SUM(K16,Q16,W16,AC16,AI16,AO16,AU16,BA16)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="816" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="814" operator="greaterThan">
       <formula>SUM(K16,Q16,W16,AC16,AI16,AO16,AU16,BA16)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="817" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="815" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M16),L16,0),IF(ISNUMBER(S16),R16,0),IF(ISNUMBER(Y16),X16,0),IF(ISNUMBER(AE16),AD16,0),IF(ISNUMBER(AK16),AJ16,0),IF(ISNUMBER(AQ16),AP16,0),IF(ISNUMBER(AW16),AV16,0),IF(ISNUMBER(BC16),BB16,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="expression" dxfId="4" priority="818">
+    <cfRule type="expression" dxfId="4" priority="816">
       <formula>AND(ISBLANK(G17),ISBLANK(O17),ISBLANK(U17),ISBLANK(AA17),ISBLANK(AG17),ISBLANK(AM17),ISBLANK(AS17),ISBLANK(AY17),ISBLANK(BE17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="819">
+    <cfRule type="expression" dxfId="1" priority="817">
       <formula>IF(SUM(K17,Q17,W17,AC17,AI17,AO17,AU17,BA17)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="820" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="818" operator="greaterThan">
       <formula>SUM(K17,Q17,W17,AC17,AI17,AO17,AU17,BA17)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="821" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="819" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M17),L17,0),IF(ISNUMBER(S17),R17,0),IF(ISNUMBER(Y17),X17,0),IF(ISNUMBER(AE17),AD17,0),IF(ISNUMBER(AK17),AJ17,0),IF(ISNUMBER(AQ17),AP17,0),IF(ISNUMBER(AW17),AV17,0),IF(ISNUMBER(BC17),BB17,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="expression" dxfId="4" priority="822">
+    <cfRule type="expression" dxfId="4" priority="820">
       <formula>AND(ISBLANK(G18),ISBLANK(O18),ISBLANK(U18),ISBLANK(AA18),ISBLANK(AG18),ISBLANK(AM18),ISBLANK(AS18),ISBLANK(AY18),ISBLANK(BE18))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="823">
+    <cfRule type="expression" dxfId="1" priority="821">
       <formula>IF(SUM(K18,Q18,W18,AC18,AI18,AO18,AU18,BA18)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="824" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="822" operator="greaterThan">
       <formula>SUM(K18,Q18,W18,AC18,AI18,AO18,AU18,BA18)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="825" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="823" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M18),L18,0),IF(ISNUMBER(S18),R18,0),IF(ISNUMBER(Y18),X18,0),IF(ISNUMBER(AE18),AD18,0),IF(ISNUMBER(AK18),AJ18,0),IF(ISNUMBER(AQ18),AP18,0),IF(ISNUMBER(AW18),AV18,0),IF(ISNUMBER(BC18),BB18,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="expression" dxfId="4" priority="826">
+    <cfRule type="expression" dxfId="4" priority="824">
       <formula>AND(ISBLANK(G19),ISBLANK(O19),ISBLANK(U19),ISBLANK(AA19),ISBLANK(AG19),ISBLANK(AM19),ISBLANK(AS19),ISBLANK(AY19),ISBLANK(BE19))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="827">
+    <cfRule type="expression" dxfId="1" priority="825">
       <formula>IF(SUM(K19,Q19,W19,AC19,AI19,AO19,AU19,BA19)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="828" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="826" operator="greaterThan">
       <formula>SUM(K19,Q19,W19,AC19,AI19,AO19,AU19,BA19)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="829" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="827" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M19),L19,0),IF(ISNUMBER(S19),R19,0),IF(ISNUMBER(Y19),X19,0),IF(ISNUMBER(AE19),AD19,0),IF(ISNUMBER(AK19),AJ19,0),IF(ISNUMBER(AQ19),AP19,0),IF(ISNUMBER(AW19),AV19,0),IF(ISNUMBER(BC19),BB19,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="expression" dxfId="4" priority="830">
+    <cfRule type="expression" dxfId="4" priority="828">
       <formula>AND(ISBLANK(G20),ISBLANK(O20),ISBLANK(U20),ISBLANK(AA20),ISBLANK(AG20),ISBLANK(AM20),ISBLANK(AS20),ISBLANK(AY20),ISBLANK(BE20))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="831">
+    <cfRule type="expression" dxfId="1" priority="829">
       <formula>IF(SUM(K20,Q20,W20,AC20,AI20,AO20,AU20,BA20)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="832" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="830" operator="greaterThan">
       <formula>SUM(K20,Q20,W20,AC20,AI20,AO20,AU20,BA20)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="833" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="831" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M20),L20,0),IF(ISNUMBER(S20),R20,0),IF(ISNUMBER(Y20),X20,0),IF(ISNUMBER(AE20),AD20,0),IF(ISNUMBER(AK20),AJ20,0),IF(ISNUMBER(AQ20),AP20,0),IF(ISNUMBER(AW20),AV20,0),IF(ISNUMBER(BC20),BB20,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="expression" dxfId="4" priority="834">
+    <cfRule type="expression" dxfId="4" priority="832">
       <formula>AND(ISBLANK(G21),ISBLANK(O21),ISBLANK(U21),ISBLANK(AA21),ISBLANK(AG21),ISBLANK(AM21),ISBLANK(AS21),ISBLANK(AY21),ISBLANK(BE21))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="835">
+    <cfRule type="expression" dxfId="1" priority="833">
       <formula>IF(SUM(K21,Q21,W21,AC21,AI21,AO21,AU21,BA21)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="836" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="834" operator="greaterThan">
       <formula>SUM(K21,Q21,W21,AC21,AI21,AO21,AU21,BA21)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="837" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="835" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M21),L21,0),IF(ISNUMBER(S21),R21,0),IF(ISNUMBER(Y21),X21,0),IF(ISNUMBER(AE21),AD21,0),IF(ISNUMBER(AK21),AJ21,0),IF(ISNUMBER(AQ21),AP21,0),IF(ISNUMBER(AW21),AV21,0),IF(ISNUMBER(BC21),BB21,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" dxfId="4" priority="838">
+    <cfRule type="expression" dxfId="4" priority="836">
       <formula>AND(ISBLANK(G22),ISBLANK(O22),ISBLANK(U22),ISBLANK(AA22),ISBLANK(AG22),ISBLANK(AM22),ISBLANK(AS22),ISBLANK(AY22),ISBLANK(BE22))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="839">
+    <cfRule type="expression" dxfId="1" priority="837">
       <formula>IF(SUM(K22,Q22,W22,AC22,AI22,AO22,AU22,BA22)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="840" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="838" operator="greaterThan">
       <formula>SUM(K22,Q22,W22,AC22,AI22,AO22,AU22,BA22)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="841" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="839" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M22),L22,0),IF(ISNUMBER(S22),R22,0),IF(ISNUMBER(Y22),X22,0),IF(ISNUMBER(AE22),AD22,0),IF(ISNUMBER(AK22),AJ22,0),IF(ISNUMBER(AQ22),AP22,0),IF(ISNUMBER(AW22),AV22,0),IF(ISNUMBER(BC22),BB22,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="expression" dxfId="4" priority="842">
+    <cfRule type="expression" dxfId="4" priority="840">
       <formula>AND(ISBLANK(G23),ISBLANK(O23),ISBLANK(U23),ISBLANK(AA23),ISBLANK(AG23),ISBLANK(AM23),ISBLANK(AS23),ISBLANK(AY23),ISBLANK(BE23))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="843">
+    <cfRule type="expression" dxfId="1" priority="841">
       <formula>IF(SUM(K23,Q23,W23,AC23,AI23,AO23,AU23,BA23)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="844" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="842" operator="greaterThan">
       <formula>SUM(K23,Q23,W23,AC23,AI23,AO23,AU23,BA23)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="845" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="843" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M23),L23,0),IF(ISNUMBER(S23),R23,0),IF(ISNUMBER(Y23),X23,0),IF(ISNUMBER(AE23),AD23,0),IF(ISNUMBER(AK23),AJ23,0),IF(ISNUMBER(AQ23),AP23,0),IF(ISNUMBER(AW23),AV23,0),IF(ISNUMBER(BC23),BB23,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="expression" dxfId="4" priority="846">
+    <cfRule type="expression" dxfId="4" priority="844">
       <formula>AND(ISBLANK(G24),ISBLANK(O24),ISBLANK(U24),ISBLANK(AA24),ISBLANK(AG24),ISBLANK(AM24),ISBLANK(AS24),ISBLANK(AY24),ISBLANK(BE24))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="847">
+    <cfRule type="expression" dxfId="1" priority="845">
       <formula>IF(SUM(K24,Q24,W24,AC24,AI24,AO24,AU24,BA24)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="848" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="846" operator="greaterThan">
       <formula>SUM(K24,Q24,W24,AC24,AI24,AO24,AU24,BA24)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="849" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="847" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M24),L24,0),IF(ISNUMBER(S24),R24,0),IF(ISNUMBER(Y24),X24,0),IF(ISNUMBER(AE24),AD24,0),IF(ISNUMBER(AK24),AJ24,0),IF(ISNUMBER(AQ24),AP24,0),IF(ISNUMBER(AW24),AV24,0),IF(ISNUMBER(BC24),BB24,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="expression" dxfId="4" priority="850">
+    <cfRule type="expression" dxfId="4" priority="848">
       <formula>AND(ISBLANK(G25),ISBLANK(O25),ISBLANK(U25),ISBLANK(AA25),ISBLANK(AG25),ISBLANK(AM25),ISBLANK(AS25),ISBLANK(AY25),ISBLANK(BE25))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="851">
+    <cfRule type="expression" dxfId="1" priority="849">
       <formula>IF(SUM(K25,Q25,W25,AC25,AI25,AO25,AU25,BA25)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="852" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="850" operator="greaterThan">
       <formula>SUM(K25,Q25,W25,AC25,AI25,AO25,AU25,BA25)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="853" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="851" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M25),L25,0),IF(ISNUMBER(S25),R25,0),IF(ISNUMBER(Y25),X25,0),IF(ISNUMBER(AE25),AD25,0),IF(ISNUMBER(AK25),AJ25,0),IF(ISNUMBER(AQ25),AP25,0),IF(ISNUMBER(AW25),AV25,0),IF(ISNUMBER(BC25),BB25,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="expression" dxfId="4" priority="854">
+    <cfRule type="expression" dxfId="4" priority="852">
       <formula>AND(ISBLANK(G26),ISBLANK(O26),ISBLANK(U26),ISBLANK(AA26),ISBLANK(AG26),ISBLANK(AM26),ISBLANK(AS26),ISBLANK(AY26),ISBLANK(BE26))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="855">
+    <cfRule type="expression" dxfId="1" priority="853">
       <formula>IF(SUM(K26,Q26,W26,AC26,AI26,AO26,AU26,BA26)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="856" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="854" operator="greaterThan">
       <formula>SUM(K26,Q26,W26,AC26,AI26,AO26,AU26,BA26)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="857" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="855" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M26),L26,0),IF(ISNUMBER(S26),R26,0),IF(ISNUMBER(Y26),X26,0),IF(ISNUMBER(AE26),AD26,0),IF(ISNUMBER(AK26),AJ26,0),IF(ISNUMBER(AQ26),AP26,0),IF(ISNUMBER(AW26),AV26,0),IF(ISNUMBER(BC26),BB26,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="expression" dxfId="4" priority="858">
+    <cfRule type="expression" dxfId="4" priority="856">
       <formula>AND(ISBLANK(G27),ISBLANK(O27),ISBLANK(U27),ISBLANK(AA27),ISBLANK(AG27),ISBLANK(AM27),ISBLANK(AS27),ISBLANK(AY27),ISBLANK(BE27))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="859">
+    <cfRule type="expression" dxfId="1" priority="857">
       <formula>IF(SUM(K27,Q27,W27,AC27,AI27,AO27,AU27,BA27)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="860" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="858" operator="greaterThan">
       <formula>SUM(K27,Q27,W27,AC27,AI27,AO27,AU27,BA27)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="861" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="859" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M27),L27,0),IF(ISNUMBER(S27),R27,0),IF(ISNUMBER(Y27),X27,0),IF(ISNUMBER(AE27),AD27,0),IF(ISNUMBER(AK27),AJ27,0),IF(ISNUMBER(AQ27),AP27,0),IF(ISNUMBER(AW27),AV27,0),IF(ISNUMBER(BC27),BB27,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="expression" dxfId="4" priority="862">
+    <cfRule type="expression" dxfId="4" priority="860">
       <formula>AND(ISBLANK(G28),ISBLANK(O28),ISBLANK(U28),ISBLANK(AA28),ISBLANK(AG28),ISBLANK(AM28),ISBLANK(AS28),ISBLANK(AY28),ISBLANK(BE28))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="863">
+    <cfRule type="expression" dxfId="1" priority="861">
       <formula>IF(SUM(K28,Q28,W28,AC28,AI28,AO28,AU28,BA28)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="864" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="862" operator="greaterThan">
       <formula>SUM(K28,Q28,W28,AC28,AI28,AO28,AU28,BA28)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="865" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="863" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M28),L28,0),IF(ISNUMBER(S28),R28,0),IF(ISNUMBER(Y28),X28,0),IF(ISNUMBER(AE28),AD28,0),IF(ISNUMBER(AK28),AJ28,0),IF(ISNUMBER(AQ28),AP28,0),IF(ISNUMBER(AW28),AV28,0),IF(ISNUMBER(BC28),BB28,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="expression" dxfId="4" priority="866">
+    <cfRule type="expression" dxfId="4" priority="864">
       <formula>AND(ISBLANK(G29),ISBLANK(O29),ISBLANK(U29),ISBLANK(AA29),ISBLANK(AG29),ISBLANK(AM29),ISBLANK(AS29),ISBLANK(AY29),ISBLANK(BE29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="867">
+    <cfRule type="expression" dxfId="1" priority="865">
       <formula>IF(SUM(K29,Q29,W29,AC29,AI29,AO29,AU29,BA29)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="868" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="866" operator="greaterThan">
       <formula>SUM(K29,Q29,W29,AC29,AI29,AO29,AU29,BA29)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="869" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="867" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M29),L29,0),IF(ISNUMBER(S29),R29,0),IF(ISNUMBER(Y29),X29,0),IF(ISNUMBER(AE29),AD29,0),IF(ISNUMBER(AK29),AJ29,0),IF(ISNUMBER(AQ29),AP29,0),IF(ISNUMBER(AW29),AV29,0),IF(ISNUMBER(BC29),BB29,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="expression" dxfId="4" priority="870">
+    <cfRule type="expression" dxfId="4" priority="868">
       <formula>AND(ISBLANK(G30),ISBLANK(O30),ISBLANK(U30),ISBLANK(AA30),ISBLANK(AG30),ISBLANK(AM30),ISBLANK(AS30),ISBLANK(AY30),ISBLANK(BE30))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="871">
+    <cfRule type="expression" dxfId="1" priority="869">
       <formula>IF(SUM(K30,Q30,W30,AC30,AI30,AO30,AU30,BA30)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="872" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="870" operator="greaterThan">
       <formula>SUM(K30,Q30,W30,AC30,AI30,AO30,AU30,BA30)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="873" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="871" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M30),L30,0),IF(ISNUMBER(S30),R30,0),IF(ISNUMBER(Y30),X30,0),IF(ISNUMBER(AE30),AD30,0),IF(ISNUMBER(AK30),AJ30,0),IF(ISNUMBER(AQ30),AP30,0),IF(ISNUMBER(AW30),AV30,0),IF(ISNUMBER(BC30),BB30,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="expression" dxfId="4" priority="874">
+    <cfRule type="expression" dxfId="4" priority="872">
       <formula>AND(ISBLANK(G31),ISBLANK(O31),ISBLANK(U31),ISBLANK(AA31),ISBLANK(AG31),ISBLANK(AM31),ISBLANK(AS31),ISBLANK(AY31),ISBLANK(BE31))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="875">
+    <cfRule type="expression" dxfId="1" priority="873">
       <formula>IF(SUM(K31,Q31,W31,AC31,AI31,AO31,AU31,BA31)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="876" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="874" operator="greaterThan">
       <formula>SUM(K31,Q31,W31,AC31,AI31,AO31,AU31,BA31)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="877" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="875" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M31),L31,0),IF(ISNUMBER(S31),R31,0),IF(ISNUMBER(Y31),X31,0),IF(ISNUMBER(AE31),AD31,0),IF(ISNUMBER(AK31),AJ31,0),IF(ISNUMBER(AQ31),AP31,0),IF(ISNUMBER(AW31),AV31,0),IF(ISNUMBER(BC31),BB31,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" dxfId="4" priority="878">
+    <cfRule type="expression" dxfId="4" priority="876">
       <formula>AND(ISBLANK(G32),ISBLANK(O32),ISBLANK(U32),ISBLANK(AA32),ISBLANK(AG32),ISBLANK(AM32),ISBLANK(AS32),ISBLANK(AY32),ISBLANK(BE32))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="879">
+    <cfRule type="expression" dxfId="1" priority="877">
       <formula>IF(SUM(K32,Q32,W32,AC32,AI32,AO32,AU32,BA32)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="880" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="878" operator="greaterThan">
       <formula>SUM(K32,Q32,W32,AC32,AI32,AO32,AU32,BA32)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="881" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="879" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M32),L32,0),IF(ISNUMBER(S32),R32,0),IF(ISNUMBER(Y32),X32,0),IF(ISNUMBER(AE32),AD32,0),IF(ISNUMBER(AK32),AJ32,0),IF(ISNUMBER(AQ32),AP32,0),IF(ISNUMBER(AW32),AV32,0),IF(ISNUMBER(BC32),BB32,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="expression" dxfId="4" priority="882">
+    <cfRule type="expression" dxfId="4" priority="880">
       <formula>AND(ISBLANK(G33),ISBLANK(O33),ISBLANK(U33),ISBLANK(AA33),ISBLANK(AG33),ISBLANK(AM33),ISBLANK(AS33),ISBLANK(AY33),ISBLANK(BE33))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="883">
+    <cfRule type="expression" dxfId="1" priority="881">
       <formula>IF(SUM(K33,Q33,W33,AC33,AI33,AO33,AU33,BA33)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="884" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="882" operator="greaterThan">
       <formula>SUM(K33,Q33,W33,AC33,AI33,AO33,AU33,BA33)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="885" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="883" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M33),L33,0),IF(ISNUMBER(S33),R33,0),IF(ISNUMBER(Y33),X33,0),IF(ISNUMBER(AE33),AD33,0),IF(ISNUMBER(AK33),AJ33,0),IF(ISNUMBER(AQ33),AP33,0),IF(ISNUMBER(AW33),AV33,0),IF(ISNUMBER(BC33),BB33,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="4" priority="886">
+    <cfRule type="expression" dxfId="4" priority="884">
       <formula>AND(ISBLANK(G34),ISBLANK(O34),ISBLANK(U34),ISBLANK(AA34),ISBLANK(AG34),ISBLANK(AM34),ISBLANK(AS34),ISBLANK(AY34),ISBLANK(BE34))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="887">
+    <cfRule type="expression" dxfId="1" priority="885">
       <formula>IF(SUM(K34,Q34,W34,AC34,AI34,AO34,AU34,BA34)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="888" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="886" operator="greaterThan">
       <formula>SUM(K34,Q34,W34,AC34,AI34,AO34,AU34,BA34)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="889" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="887" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M34),L34,0),IF(ISNUMBER(S34),R34,0),IF(ISNUMBER(Y34),X34,0),IF(ISNUMBER(AE34),AD34,0),IF(ISNUMBER(AK34),AJ34,0),IF(ISNUMBER(AQ34),AP34,0),IF(ISNUMBER(AW34),AV34,0),IF(ISNUMBER(BC34),BB34,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="4" priority="890">
+    <cfRule type="expression" dxfId="4" priority="888">
       <formula>AND(ISBLANK(G35),ISBLANK(O35),ISBLANK(U35),ISBLANK(AA35),ISBLANK(AG35),ISBLANK(AM35),ISBLANK(AS35),ISBLANK(AY35),ISBLANK(BE35))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="891">
+    <cfRule type="expression" dxfId="1" priority="889">
       <formula>IF(SUM(K35,Q35,W35,AC35,AI35,AO35,AU35,BA35)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="892" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="890" operator="greaterThan">
       <formula>SUM(K35,Q35,W35,AC35,AI35,AO35,AU35,BA35)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="893" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="891" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M35),L35,0),IF(ISNUMBER(S35),R35,0),IF(ISNUMBER(Y35),X35,0),IF(ISNUMBER(AE35),AD35,0),IF(ISNUMBER(AK35),AJ35,0),IF(ISNUMBER(AQ35),AP35,0),IF(ISNUMBER(AW35),AV35,0),IF(ISNUMBER(BC35),BB35,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="4" priority="894">
+    <cfRule type="expression" dxfId="4" priority="892">
       <formula>AND(ISBLANK(G36),ISBLANK(O36),ISBLANK(U36),ISBLANK(AA36),ISBLANK(AG36),ISBLANK(AM36),ISBLANK(AS36),ISBLANK(AY36),ISBLANK(BE36))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="895">
+    <cfRule type="expression" dxfId="1" priority="893">
       <formula>IF(SUM(K36,Q36,W36,AC36,AI36,AO36,AU36,BA36)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="896" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="894" operator="greaterThan">
       <formula>SUM(K36,Q36,W36,AC36,AI36,AO36,AU36,BA36)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="897" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="895" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M36),L36,0),IF(ISNUMBER(S36),R36,0),IF(ISNUMBER(Y36),X36,0),IF(ISNUMBER(AE36),AD36,0),IF(ISNUMBER(AK36),AJ36,0),IF(ISNUMBER(AQ36),AP36,0),IF(ISNUMBER(AW36),AV36,0),IF(ISNUMBER(BC36),BB36,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="4" priority="898">
+    <cfRule type="expression" dxfId="4" priority="896">
       <formula>AND(ISBLANK(G37),ISBLANK(O37),ISBLANK(U37),ISBLANK(AA37),ISBLANK(AG37),ISBLANK(AM37),ISBLANK(AS37),ISBLANK(AY37),ISBLANK(BE37))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="899">
+    <cfRule type="expression" dxfId="1" priority="897">
       <formula>IF(SUM(K37,Q37,W37,AC37,AI37,AO37,AU37,BA37)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="900" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="898" operator="greaterThan">
       <formula>SUM(K37,Q37,W37,AC37,AI37,AO37,AU37,BA37)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="901" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="899" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M37),L37,0),IF(ISNUMBER(S37),R37,0),IF(ISNUMBER(Y37),X37,0),IF(ISNUMBER(AE37),AD37,0),IF(ISNUMBER(AK37),AJ37,0),IF(ISNUMBER(AQ37),AP37,0),IF(ISNUMBER(AW37),AV37,0),IF(ISNUMBER(BC37),BB37,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="4" priority="902">
+    <cfRule type="expression" dxfId="4" priority="900">
       <formula>AND(ISBLANK(G38),ISBLANK(O38),ISBLANK(U38),ISBLANK(AA38),ISBLANK(AG38),ISBLANK(AM38),ISBLANK(AS38),ISBLANK(AY38),ISBLANK(BE38))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="903">
+    <cfRule type="expression" dxfId="1" priority="901">
       <formula>IF(SUM(K38,Q38,W38,AC38,AI38,AO38,AU38,BA38)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="904" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="902" operator="greaterThan">
       <formula>SUM(K38,Q38,W38,AC38,AI38,AO38,AU38,BA38)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="905" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="903" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M38),L38,0),IF(ISNUMBER(S38),R38,0),IF(ISNUMBER(Y38),X38,0),IF(ISNUMBER(AE38),AD38,0),IF(ISNUMBER(AK38),AJ38,0),IF(ISNUMBER(AQ38),AP38,0),IF(ISNUMBER(AW38),AV38,0),IF(ISNUMBER(BC38),BB38,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="expression" dxfId="4" priority="906">
+    <cfRule type="expression" dxfId="4" priority="904">
       <formula>AND(ISBLANK(G39),ISBLANK(O39),ISBLANK(U39),ISBLANK(AA39),ISBLANK(AG39),ISBLANK(AM39),ISBLANK(AS39),ISBLANK(AY39),ISBLANK(BE39))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="907">
+    <cfRule type="expression" dxfId="1" priority="905">
       <formula>IF(SUM(K39,Q39,W39,AC39,AI39,AO39,AU39,BA39)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="908" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="906" operator="greaterThan">
       <formula>SUM(K39,Q39,W39,AC39,AI39,AO39,AU39,BA39)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="909" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="907" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M39),L39,0),IF(ISNUMBER(S39),R39,0),IF(ISNUMBER(Y39),X39,0),IF(ISNUMBER(AE39),AD39,0),IF(ISNUMBER(AK39),AJ39,0),IF(ISNUMBER(AQ39),AP39,0),IF(ISNUMBER(AW39),AV39,0),IF(ISNUMBER(BC39),BB39,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="expression" dxfId="4" priority="910">
+    <cfRule type="expression" dxfId="4" priority="908">
       <formula>AND(ISBLANK(G40),ISBLANK(O40),ISBLANK(U40),ISBLANK(AA40),ISBLANK(AG40),ISBLANK(AM40),ISBLANK(AS40),ISBLANK(AY40),ISBLANK(BE40))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="911">
+    <cfRule type="expression" dxfId="1" priority="909">
       <formula>IF(SUM(K40,Q40,W40,AC40,AI40,AO40,AU40,BA40)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="912" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="910" operator="greaterThan">
       <formula>SUM(K40,Q40,W40,AC40,AI40,AO40,AU40,BA40)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="913" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="911" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M40),L40,0),IF(ISNUMBER(S40),R40,0),IF(ISNUMBER(Y40),X40,0),IF(ISNUMBER(AE40),AD40,0),IF(ISNUMBER(AK40),AJ40,0),IF(ISNUMBER(AQ40),AP40,0),IF(ISNUMBER(AW40),AV40,0),IF(ISNUMBER(BC40),BB40,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="expression" dxfId="4" priority="914">
+    <cfRule type="expression" dxfId="4" priority="912">
       <formula>AND(ISBLANK(G41),ISBLANK(O41),ISBLANK(U41),ISBLANK(AA41),ISBLANK(AG41),ISBLANK(AM41),ISBLANK(AS41),ISBLANK(AY41),ISBLANK(BE41))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="915">
+    <cfRule type="expression" dxfId="1" priority="913">
       <formula>IF(SUM(K41,Q41,W41,AC41,AI41,AO41,AU41,BA41)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="916" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="914" operator="greaterThan">
       <formula>SUM(K41,Q41,W41,AC41,AI41,AO41,AU41,BA41)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="917" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="915" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M41),L41,0),IF(ISNUMBER(S41),R41,0),IF(ISNUMBER(Y41),X41,0),IF(ISNUMBER(AE41),AD41,0),IF(ISNUMBER(AK41),AJ41,0),IF(ISNUMBER(AQ41),AP41,0),IF(ISNUMBER(AW41),AV41,0),IF(ISNUMBER(BC41),BB41,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="expression" dxfId="4" priority="918">
+    <cfRule type="expression" dxfId="4" priority="916">
       <formula>AND(ISBLANK(G42),ISBLANK(O42),ISBLANK(U42),ISBLANK(AA42),ISBLANK(AG42),ISBLANK(AM42),ISBLANK(AS42),ISBLANK(AY42),ISBLANK(BE42))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="919">
+    <cfRule type="expression" dxfId="1" priority="917">
       <formula>IF(SUM(K42,Q42,W42,AC42,AI42,AO42,AU42,BA42)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="920" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="918" operator="greaterThan">
       <formula>SUM(K42,Q42,W42,AC42,AI42,AO42,AU42,BA42)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="921" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="919" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M42),L42,0),IF(ISNUMBER(S42),R42,0),IF(ISNUMBER(Y42),X42,0),IF(ISNUMBER(AE42),AD42,0),IF(ISNUMBER(AK42),AJ42,0),IF(ISNUMBER(AQ42),AP42,0),IF(ISNUMBER(AW42),AV42,0),IF(ISNUMBER(BC42),BB42,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="4" priority="778">
+    <cfRule type="expression" dxfId="4" priority="776">
       <formula>AND(ISBLANK(G7),ISBLANK(O7),ISBLANK(U7),ISBLANK(AA7),ISBLANK(AG7),ISBLANK(AM7),ISBLANK(AS7),ISBLANK(AY7),ISBLANK(BE7))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="779">
+    <cfRule type="expression" dxfId="1" priority="777">
       <formula>IF(SUM(K7,Q7,W7,AC7,AI7,AO7,AU7,BA7)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="780" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="778" operator="greaterThan">
       <formula>SUM(K7,Q7,W7,AC7,AI7,AO7,AU7,BA7)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="781" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="779" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M7),L7,0),IF(ISNUMBER(S7),R7,0),IF(ISNUMBER(Y7),X7,0),IF(ISNUMBER(AE7),AD7,0),IF(ISNUMBER(AK7),AJ7,0),IF(ISNUMBER(AQ7),AP7,0),IF(ISNUMBER(AW7),AV7,0),IF(ISNUMBER(BC7),BB7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="4" priority="782">
+    <cfRule type="expression" dxfId="4" priority="780">
       <formula>AND(ISBLANK(G8),ISBLANK(O8),ISBLANK(U8),ISBLANK(AA8),ISBLANK(AG8),ISBLANK(AM8),ISBLANK(AS8),ISBLANK(AY8),ISBLANK(BE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="783">
+    <cfRule type="expression" dxfId="1" priority="781">
       <formula>IF(SUM(K8,Q8,W8,AC8,AI8,AO8,AU8,BA8)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="784" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="782" operator="greaterThan">
       <formula>SUM(K8,Q8,W8,AC8,AI8,AO8,AU8,BA8)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="785" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="783" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M8),L8,0),IF(ISNUMBER(S8),R8,0),IF(ISNUMBER(Y8),X8,0),IF(ISNUMBER(AE8),AD8,0),IF(ISNUMBER(AK8),AJ8,0),IF(ISNUMBER(AQ8),AP8,0),IF(ISNUMBER(AW8),AV8,0),IF(ISNUMBER(BC8),BB8,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="4" priority="786">
+    <cfRule type="expression" dxfId="4" priority="784">
       <formula>AND(ISBLANK(G9),ISBLANK(O9),ISBLANK(U9),ISBLANK(AA9),ISBLANK(AG9),ISBLANK(AM9),ISBLANK(AS9),ISBLANK(AY9),ISBLANK(BE9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="787">
+    <cfRule type="expression" dxfId="1" priority="785">
       <formula>IF(SUM(K9,Q9,W9,AC9,AI9,AO9,AU9,BA9)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="788" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="786" operator="greaterThan">
       <formula>SUM(K9,Q9,W9,AC9,AI9,AO9,AU9,BA9)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="789" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="787" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(M9),L9,0),IF(ISNUMBER(S9),R9,0),IF(ISNUMBER(Y9),X9,0),IF(ISNUMBER(AE9),AD9,0),IF(ISNUMBER(AK9),AJ9,0),IF(ISNUMBER(AQ9),AP9,0),IF(ISNUMBER(AW9),AV9,0),IF(ISNUMBER(BC9),BB9,0))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>